<commit_message>
routes info, delete func
</commit_message>
<xml_diff>
--- a/src/backend/fileStorage/excel/roadXS.xlsx
+++ b/src/backend/fileStorage/excel/roadXS.xlsx
@@ -57,7 +57,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="285" uniqueCount="175">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="154">
   <si>
     <t>року</t>
   </si>
@@ -461,6 +461,9 @@
     <t>Звання старшого</t>
   </si>
   <si>
+    <t>id</t>
+  </si>
+  <si>
     <t>тип дорожнього покриття</t>
   </si>
   <si>
@@ -491,34 +494,46 @@
     <t>маршрут</t>
   </si>
   <si>
-    <t>жигуль</t>
-  </si>
-  <si>
-    <t>аа2245аа</t>
+    <t>тестМобіль</t>
+  </si>
+  <si>
+    <t>3</t>
   </si>
   <si>
     <t>Бензин</t>
   </si>
   <si>
-    <t>10</t>
+    <t>5</t>
   </si>
   <si>
     <t>Олива 10 w40</t>
   </si>
   <si>
+    <t>1</t>
+  </si>
+  <si>
     <t>тр</t>
   </si>
   <si>
     <t>транспортна</t>
   </si>
   <si>
+    <t>Кличко К.Л.</t>
+  </si>
+  <si>
+    <t>солдат</t>
+  </si>
+  <si>
     <t>А0000 (ПВЗ)</t>
   </si>
   <si>
     <t>Солярка К.Р.</t>
   </si>
   <si>
-    <t>Начальник автомобільної служби</t>
+    <t>лейтенант</t>
+  </si>
+  <si>
+    <t>старший відділення</t>
   </si>
   <si>
     <t>капітан</t>
@@ -527,85 +542,7 @@
     <t>к-н</t>
   </si>
   <si>
-    <t>Кременець</t>
-  </si>
-  <si>
-    <t>Тернопіль</t>
-  </si>
-  <si>
-    <t>так</t>
-  </si>
-  <si>
-    <t>ВВ4535ОО</t>
-  </si>
-  <si>
-    <t>ДТ</t>
-  </si>
-  <si>
-    <t>Олива 30 w40</t>
-  </si>
-  <si>
-    <t>начальник КТП</t>
-  </si>
-  <si>
-    <t>солдат</t>
-  </si>
-  <si>
-    <t>солд</t>
-  </si>
-  <si>
-    <t>Львів</t>
-  </si>
-  <si>
-    <t>Хмельницький</t>
-  </si>
-  <si>
-    <t>Formula1</t>
-  </si>
-  <si>
-    <t>аА234ба</t>
-  </si>
-  <si>
-    <t>2</t>
-  </si>
-  <si>
-    <t>Зувій К.Л.</t>
-  </si>
-  <si>
-    <t>лейтенант</t>
-  </si>
-  <si>
-    <t>технік</t>
-  </si>
-  <si>
-    <t>л-т</t>
-  </si>
-  <si>
-    <t>старший машини</t>
-  </si>
-  <si>
-    <t>майор</t>
-  </si>
-  <si>
-    <t>м-р</t>
-  </si>
-  <si>
-    <t>Дрин А.П.</t>
-  </si>
-  <si>
-    <t>водій</t>
-  </si>
-  <si>
-    <t>Зібров С.Л.</t>
-  </si>
-  <si>
-    <t>старший лейтенант</t>
-  </si>
-  <si>
-    <t>ст. л-т</t>
-  </si>
-  <si>
-    <t>Карпов С.Л.</t>
+    <t>Майбах С.Т.</t>
   </si>
 </sst>
 </file>
@@ -1118,7 +1055,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="148">
+  <cellXfs count="146">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1483,8 +1420,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1616,25 +1551,7 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" name="Таблиця3" displayName="Таблиця3" ref="S2:V7" totalsRowShown="1" headerRowCount="0">
-  <autoFilter>
-    <filterColumn colId="0" hiddenButton="1"/>
-    <filterColumn colId="1" hiddenButton="1"/>
-    <filterColumn colId="2" hiddenButton="1"/>
-    <filterColumn colId="3" hiddenButton="1"/>
-  </autoFilter>
-  <tableColumns count="4">
-    <tableColumn id="1" name="посада"/>
-    <tableColumn id="2" name="звання"/>
-    <tableColumn id="3" name="звання скорочено"/>
-    <tableColumn id="4" name="ПІБ"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" name="Таблиця4" displayName="Таблиця4" ref="Z2:AC4" totalsRowShown="1" headerRowCount="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" name="Таблиця4" displayName="Таблиця4" ref="Z2:AC4" totalsRowShown="1" headerRowCount="0">
   <autoFilter>
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -1914,10 +1831,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:AC8"/>
+  <dimension ref="A2:AC29"/>
   <sheetViews>
     <sheetView workbookViewId="0" zoomScale="100" zoomScaleNormal="100">
-      <selection activeCell="L11" sqref="L11"/>
+      <selection activeCell="P9" sqref="P9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="0.25"/>
@@ -1929,7 +1846,8 @@
     <col min="5" max="5" width="13.85546875" customWidth="1"/>
     <col min="6" max="6" width="12.140625" customWidth="1"/>
     <col min="7" max="7" width="13.5703125" customWidth="1"/>
-    <col min="8" max="14" width="16.5703125" customWidth="1"/>
+    <col min="8" max="13" width="16.5703125" customWidth="1"/>
+    <col min="14" max="14" width="7" customWidth="1"/>
     <col min="16" max="16" width="35.42578125" customWidth="1"/>
     <col min="17" max="17" width="11.42578125" customWidth="1"/>
     <col min="19" max="19" width="30.140625" customWidth="1"/>
@@ -1982,268 +1900,124 @@
       <c r="M2" s="145" t="s">
         <v>125</v>
       </c>
+      <c r="O2" s="145" t="s">
+        <v>126</v>
+      </c>
       <c r="P2" s="145" t="s">
+        <v>127</v>
+      </c>
+      <c r="Q2" s="145" t="s">
+        <v>128</v>
+      </c>
+      <c r="S2" s="145" t="s">
+        <v>129</v>
+      </c>
+      <c r="T2" s="145" t="s">
+        <v>130</v>
+      </c>
+      <c r="U2" s="145" t="s">
+        <v>131</v>
+      </c>
+      <c r="V2" s="145" t="s">
+        <v>132</v>
+      </c>
+      <c r="Y2" s="145" t="s">
         <v>126</v>
       </c>
-      <c r="Q2" s="145" t="s">
-        <v>127</v>
-      </c>
-      <c r="S2" s="145" t="s">
-        <v>128</v>
-      </c>
-      <c r="T2" s="145" t="s">
-        <v>129</v>
-      </c>
-      <c r="U2" s="145" t="s">
-        <v>130</v>
-      </c>
-      <c r="V2" s="145" t="s">
-        <v>131</v>
-      </c>
       <c r="Z2" s="145" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="AA2" s="145" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="AB2" s="145" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="AC2" s="145" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
     </row>
     <row r="3" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="B3" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="C3" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="D3" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="E3" t="s">
-        <v>140</v>
-      </c>
-      <c r="F3">
-        <v>1</v>
+        <v>141</v>
+      </c>
+      <c r="F3" t="s">
+        <v>142</v>
       </c>
       <c r="G3" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="H3" t="s">
-        <v>142</v>
-      </c>
-      <c r="I3" s="146" t="s">
-        <v>111</v>
-      </c>
-      <c r="J3">
-        <f>IFERROR(INDEX(Таблиця3[звання],MATCH(#REF!,Таблиця3[ПІБ],0)),"")</f>
+        <v>144</v>
+      </c>
+      <c r="I3" t="s">
+        <v>145</v>
+      </c>
+      <c r="J3" t="s">
+        <v>146</v>
       </c>
       <c r="K3" t="s">
-        <v>143</v>
-      </c>
-      <c r="L3" s="146" t="s">
-        <v>144</v>
-      </c>
-      <c r="M3">
-        <f>IFERROR(INDEX(Таблиця3[звання],MATCH(#REF!,Таблиця3[ПІБ],0)),"")</f>
-      </c>
-      <c r="P3" t="s">
-        <v>100</v>
-      </c>
-      <c r="Q3" s="147">
-        <v>0.15</v>
+        <v>147</v>
+      </c>
+      <c r="L3" t="s">
+        <v>148</v>
+      </c>
+      <c r="M3" t="s">
+        <v>149</v>
       </c>
       <c r="S3" t="s">
-        <v>145</v>
+        <v>150</v>
       </c>
       <c r="T3" t="s">
-        <v>146</v>
+        <v>151</v>
       </c>
       <c r="U3" t="s">
-        <v>147</v>
+        <v>152</v>
       </c>
       <c r="V3" t="s">
-        <v>13</v>
-      </c>
-      <c r="Z3" t="s">
-        <v>148</v>
-      </c>
-      <c r="AA3" t="s">
-        <v>149</v>
-      </c>
-      <c r="AB3" t="s">
-        <v>150</v>
-      </c>
-      <c r="AC3" t="str">
-        <f>IF(Таблиця4[[#This Row],[в один кінець]]="так",Таблиця4[[#This Row],[Звідки]]&amp;" - "&amp;Таблиця4[[#This Row],[Куди]],Таблиця4[[#This Row],[Звідки]]&amp;" - "&amp;Таблиця4[[#This Row],[Куди]]&amp;" - "&amp;Таблиця4[[#This Row],[Звідки]])</f>
-        <v>Кременець - Тернопіль</v>
-      </c>
-    </row>
-    <row r="4" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>61</v>
-      </c>
-      <c r="B4" t="s">
-        <v>151</v>
-      </c>
-      <c r="C4" t="s">
-        <v>152</v>
-      </c>
-      <c r="D4">
-        <v>11.5</v>
-      </c>
-      <c r="E4" t="s">
         <v>153</v>
       </c>
-      <c r="F4">
-        <v>1.2</v>
-      </c>
-      <c r="G4" t="s">
-        <v>141</v>
-      </c>
-      <c r="H4" t="s">
-        <v>142</v>
-      </c>
-      <c r="I4" s="146" t="s">
-        <v>111</v>
-      </c>
-      <c r="J4">
-        <f>IFERROR(INDEX(Таблиця3[звання],MATCH(#REF!,Таблиця3[ПІБ],0)),"")</f>
-      </c>
-      <c r="K4" t="s">
-        <v>143</v>
-      </c>
-      <c r="L4" s="146" t="s">
-        <v>13</v>
-      </c>
-      <c r="M4">
-        <f>IFERROR(INDEX(Таблиця3[звання],MATCH(#REF!,Таблиця3[ПІБ],0)),"")</f>
-      </c>
-      <c r="S4" t="s">
-        <v>154</v>
-      </c>
-      <c r="T4" t="s">
-        <v>155</v>
-      </c>
-      <c r="U4" t="s">
-        <v>156</v>
-      </c>
-      <c r="V4" t="s">
-        <v>17</v>
-      </c>
-      <c r="Z4" t="s">
-        <v>157</v>
-      </c>
-      <c r="AA4" t="s">
-        <v>158</v>
-      </c>
-      <c r="AC4" t="str">
-        <f>IF(Таблиця4[[#This Row],[в один кінець]]="так",Таблиця4[[#This Row],[Звідки]]&amp;" - "&amp;Таблиця4[[#This Row],[Куди]],Таблиця4[[#This Row],[Звідки]]&amp;" - "&amp;Таблиця4[[#This Row],[Куди]]&amp;" - "&amp;Таблиця4[[#This Row],[Звідки]])</f>
-        <v>Львів - Хмельницький - Львів</v>
-      </c>
-    </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>159</v>
-      </c>
-      <c r="B5" t="s">
-        <v>160</v>
-      </c>
-      <c r="C5" t="s">
-        <v>138</v>
-      </c>
-      <c r="D5" t="s">
-        <v>139</v>
-      </c>
-      <c r="E5" t="s">
-        <v>153</v>
-      </c>
-      <c r="F5" t="s">
-        <v>161</v>
-      </c>
-      <c r="G5" t="s">
-        <v>141</v>
-      </c>
-      <c r="H5" t="s">
-        <v>142</v>
-      </c>
-      <c r="I5" t="s">
-        <v>162</v>
-      </c>
-      <c r="J5" t="s">
-        <v>155</v>
-      </c>
-      <c r="K5" t="s">
-        <v>143</v>
-      </c>
-      <c r="L5" t="s">
-        <v>144</v>
-      </c>
-      <c r="M5" t="s">
-        <v>163</v>
-      </c>
-      <c r="S5" t="s">
-        <v>164</v>
-      </c>
-      <c r="T5" t="s">
-        <v>163</v>
-      </c>
-      <c r="U5" t="s">
-        <v>165</v>
-      </c>
-      <c r="V5" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="6" spans="19:22" x14ac:dyDescent="0.25">
-      <c r="S6" t="s">
-        <v>166</v>
-      </c>
-      <c r="T6" t="s">
-        <v>167</v>
-      </c>
-      <c r="U6" t="s">
-        <v>168</v>
-      </c>
-      <c r="V6" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="7" spans="19:22" x14ac:dyDescent="0.25">
-      <c r="S7" t="s">
-        <v>170</v>
-      </c>
-      <c r="T7" t="s">
-        <v>167</v>
-      </c>
-      <c r="U7" t="s">
-        <v>168</v>
-      </c>
-      <c r="V7" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="8" spans="19:22" x14ac:dyDescent="0.25">
-      <c r="S8" t="s">
-        <v>170</v>
-      </c>
-      <c r="T8" t="s">
-        <v>172</v>
-      </c>
-      <c r="U8" t="s">
-        <v>173</v>
-      </c>
-      <c r="V8" t="s">
-        <v>174</v>
-      </c>
-    </row>
+    </row>
+    <row r="4" spans="25:25" x14ac:dyDescent="0.25"/>
+    <row r="5" spans="25:25" x14ac:dyDescent="0.25"/>
+    <row r="6" spans="25:25" x14ac:dyDescent="0.25"/>
+    <row r="7" spans="25:25" x14ac:dyDescent="0.25"/>
+    <row r="8" spans="25:25" x14ac:dyDescent="0.25"/>
+    <row r="9" spans="25:25" x14ac:dyDescent="0.25"/>
+    <row r="10" spans="25:25" x14ac:dyDescent="0.25"/>
+    <row r="11" spans="25:25" x14ac:dyDescent="0.25"/>
+    <row r="12" spans="25:25" x14ac:dyDescent="0.25"/>
+    <row r="13" spans="25:25" x14ac:dyDescent="0.25"/>
+    <row r="14" spans="25:25" x14ac:dyDescent="0.25"/>
+    <row r="15" spans="25:25" x14ac:dyDescent="0.25"/>
+    <row r="16" spans="25:25" x14ac:dyDescent="0.25"/>
+    <row r="17" spans="25:25" x14ac:dyDescent="0.25"/>
+    <row r="18" spans="25:25" x14ac:dyDescent="0.25"/>
+    <row r="19" spans="25:25" x14ac:dyDescent="0.25"/>
+    <row r="20" spans="25:25" x14ac:dyDescent="0.25"/>
+    <row r="21" spans="25:25" x14ac:dyDescent="0.25"/>
+    <row r="22" spans="25:25" x14ac:dyDescent="0.25"/>
+    <row r="23" spans="25:25" x14ac:dyDescent="0.25"/>
+    <row r="24" spans="25:25" x14ac:dyDescent="0.25"/>
+    <row r="25" spans="25:25" x14ac:dyDescent="0.25"/>
+    <row r="26" spans="25:25" x14ac:dyDescent="0.25"/>
+    <row r="27" spans="25:25" x14ac:dyDescent="0.25"/>
+    <row r="28" spans="25:25" x14ac:dyDescent="0.25"/>
+    <row r="29" spans="25:25" x14ac:dyDescent="0.25"/>
   </sheetData>
+  <autoFilter ref="S2:V2"/>
   <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I3:I4">
       <formula1>PIB</formula1>
@@ -2254,10 +2028,9 @@
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1" firstPageNumber="1" useFirstPageNumber="1" copies="1"/>
-  <tableParts count="3">
+  <tableParts count="2">
     <tablePart r:id="rId1"/>
     <tablePart r:id="rId2"/>
-    <tablePart r:id="rId3"/>
   </tableParts>
 </worksheet>
 </file>
@@ -2414,7 +2187,7 @@
         <v>10</v>
       </c>
       <c r="J5" s="22">
-        <f>IFERROR(INDEX(Таблиця3[звання],MATCH('Ш Лист 1'!L5,Таблиця3[ПІБ],0)),"")</f>
+        <f>IFERROR(INDEX(#REF!,MATCH('Ш Лист 1'!L5,#REF!,0)),"")</f>
       </c>
       <c r="K5" s="19"/>
       <c r="L5" s="23" t="e">
@@ -2426,7 +2199,7 @@
         <v>11</v>
       </c>
       <c r="P5" s="22">
-        <f>IFERROR(INDEX(Таблиця3[звання],MATCH('Ш Лист 1'!R5,Таблиця3[ПІБ],0)),"")</f>
+        <f>IFERROR(INDEX(#REF!,MATCH('Ш Лист 1'!R5,#REF!,0)),"")</f>
       </c>
       <c r="Q5" s="19"/>
       <c r="R5" s="23" t="e">
@@ -2477,8 +2250,8 @@
       <c r="G7" s="7"/>
       <c r="H7" s="8"/>
       <c r="I7" s="29" t="str">
-        <f>IFERROR(INDEX(Таблиця3[посада],MATCH('Ш Лист 1'!R7,Таблиця3[ПІБ],0)),"")&amp;", "&amp;IFERROR(INDEX(Таблиця3[звання],MATCH('Ш Лист 1'!R7,Таблиця3[ПІБ],0)),"")</f>
-        <v>Начальник автомобільної служби, капітан</v>
+        <f>IFERROR(INDEX(#REF!,MATCH('Ш Лист 1'!R7,#REF!,0)),"")&amp;", "&amp;IFERROR(INDEX(#REF!,MATCH('Ш Лист 1'!R7,#REF!,0)),"")</f>
+        <v>, </v>
       </c>
       <c r="J7" s="30"/>
       <c r="K7" s="30"/>
@@ -2733,9 +2506,8 @@
       <c r="F12" s="43"/>
       <c r="G12" s="35"/>
       <c r="H12" s="8"/>
-      <c r="I12" s="66" t="str">
-        <f>IFERROR(INDEX(Таблиця3[звання скорочено],MATCH('Ш Лист 1'!J12,Таблиця3[ПІБ],0)),"")</f>
-        <v>к-н</v>
+      <c r="I12" s="66">
+        <f>IFERROR(INDEX(#REF!,MATCH('Ш Лист 1'!J12,#REF!,0)),"")</f>
       </c>
       <c r="J12" s="67" t="str">
         <f>IF(T12,$U$5,"")</f>
@@ -2745,9 +2517,8 @@
         <f>IF(T12,T12,"")</f>
         <v>45198</v>
       </c>
-      <c r="L12" s="66" t="str">
-        <f>IFERROR(INDEX(Таблиця3[звання скорочено],MATCH('Ш Лист 1'!M12,Таблиця3[ПІБ],0)),"")</f>
-        <v>солд</v>
+      <c r="L12" s="66">
+        <f>IFERROR(INDEX(#REF!,MATCH('Ш Лист 1'!M12,#REF!,0)),"")</f>
       </c>
       <c r="M12" s="67" t="str">
         <f>IF(T12,$U$6,"")</f>
@@ -2864,9 +2635,8 @@
       <c r="F14" s="43"/>
       <c r="G14" s="35"/>
       <c r="H14" s="8"/>
-      <c r="I14" s="83" t="str">
-        <f>IFERROR(INDEX(Таблиця3[звання скорочено],MATCH('Ш Лист 1'!J14,Таблиця3[ПІБ],0)),"")</f>
-        <v>к-н</v>
+      <c r="I14" s="83">
+        <f>IFERROR(INDEX(#REF!,MATCH('Ш Лист 1'!J14,#REF!,0)),"")</f>
       </c>
       <c r="J14" s="84" t="str">
         <f>IF(T14,$U$5,"")</f>
@@ -2876,9 +2646,8 @@
         <f>IF(T14,T14,"")</f>
         <v>45199</v>
       </c>
-      <c r="L14" s="83" t="str">
-        <f>IFERROR(INDEX(Таблиця3[звання скорочено],MATCH('Ш Лист 1'!M14,Таблиця3[ПІБ],0)),"")</f>
-        <v>солд</v>
+      <c r="L14" s="83">
+        <f>IFERROR(INDEX(#REF!,MATCH('Ш Лист 1'!M14,#REF!,0)),"")</f>
       </c>
       <c r="M14" s="84" t="str">
         <f>IF(T14,$U$6,"")</f>
@@ -2997,9 +2766,8 @@
       <c r="F16" s="43"/>
       <c r="G16" s="35"/>
       <c r="H16" s="8"/>
-      <c r="I16" s="83" t="str">
-        <f>IFERROR(INDEX(Таблиця3[звання скорочено],MATCH('Ш Лист 1'!J16,Таблиця3[ПІБ],0)),"")</f>
-        <v>к-н</v>
+      <c r="I16" s="83">
+        <f>IFERROR(INDEX(#REF!,MATCH('Ш Лист 1'!J16,#REF!,0)),"")</f>
       </c>
       <c r="J16" s="84" t="str">
         <f>IF(T16,$U$5,"")</f>
@@ -3009,9 +2777,8 @@
         <f>IF(T16,T16,"")</f>
         <v>45198</v>
       </c>
-      <c r="L16" s="83" t="str">
-        <f>IFERROR(INDEX(Таблиця3[звання скорочено],MATCH('Ш Лист 1'!M16,Таблиця3[ПІБ],0)),"")</f>
-        <v>солд</v>
+      <c r="L16" s="83">
+        <f>IFERROR(INDEX(#REF!,MATCH('Ш Лист 1'!M16,#REF!,0)),"")</f>
       </c>
       <c r="M16" s="84" t="str">
         <f>IF(T16,$U$6,"")</f>
@@ -3120,9 +2887,8 @@
       <c r="F18" s="43"/>
       <c r="G18" s="35"/>
       <c r="H18" s="8"/>
-      <c r="I18" s="83" t="str">
-        <f>IFERROR(INDEX(Таблиця3[звання скорочено],MATCH('Ш Лист 1'!J18,Таблиця3[ПІБ],0)),"")</f>
-        <v>к-н</v>
+      <c r="I18" s="83">
+        <f>IFERROR(INDEX(#REF!,MATCH('Ш Лист 1'!J18,#REF!,0)),"")</f>
       </c>
       <c r="J18" s="84" t="str">
         <f>IF(T18,$U$5,"")</f>
@@ -3132,9 +2898,8 @@
         <f>IF(T18,T18,"")</f>
         <v>45198</v>
       </c>
-      <c r="L18" s="83" t="str">
-        <f>IFERROR(INDEX(Таблиця3[звання скорочено],MATCH('Ш Лист 1'!M18,Таблиця3[ПІБ],0)),"")</f>
-        <v>солд</v>
+      <c r="L18" s="83">
+        <f>IFERROR(INDEX(#REF!,MATCH('Ш Лист 1'!M18,#REF!,0)),"")</f>
       </c>
       <c r="M18" s="84" t="str">
         <f>IF(T18,$U$6,"")</f>
@@ -3231,9 +2996,8 @@
       <c r="F20" s="43"/>
       <c r="G20" s="35"/>
       <c r="H20" s="8"/>
-      <c r="I20" s="83" t="str">
-        <f>IFERROR(INDEX(Таблиця3[звання скорочено],MATCH('Ш Лист 1'!J20,Таблиця3[ПІБ],0)),"")</f>
-        <v>к-н</v>
+      <c r="I20" s="83">
+        <f>IFERROR(INDEX(#REF!,MATCH('Ш Лист 1'!J20,#REF!,0)),"")</f>
       </c>
       <c r="J20" s="84" t="str">
         <f>IF(T20,$U$5,"")</f>
@@ -3243,9 +3007,8 @@
         <f>IF(T20,T20,"")</f>
         <v>45198</v>
       </c>
-      <c r="L20" s="83" t="str">
-        <f>IFERROR(INDEX(Таблиця3[звання скорочено],MATCH('Ш Лист 1'!M20,Таблиця3[ПІБ],0)),"")</f>
-        <v>солд</v>
+      <c r="L20" s="83">
+        <f>IFERROR(INDEX(#REF!,MATCH('Ш Лист 1'!M20,#REF!,0)),"")</f>
       </c>
       <c r="M20" s="84" t="str">
         <f>IF(T20,$U$6,"")</f>
@@ -3340,9 +3103,8 @@
       <c r="F22" s="43"/>
       <c r="G22" s="35"/>
       <c r="H22" s="8"/>
-      <c r="I22" s="83" t="str">
-        <f>IFERROR(INDEX(Таблиця3[звання скорочено],MATCH('Ш Лист 1'!J22,Таблиця3[ПІБ],0)),"")</f>
-        <v>к-н</v>
+      <c r="I22" s="83">
+        <f>IFERROR(INDEX(#REF!,MATCH('Ш Лист 1'!J22,#REF!,0)),"")</f>
       </c>
       <c r="J22" s="84" t="str">
         <f>IF(T22,$U$5,"")</f>
@@ -3352,9 +3114,8 @@
         <f>IF(T22,T22,"")</f>
         <v>45198</v>
       </c>
-      <c r="L22" s="83" t="str">
-        <f>IFERROR(INDEX(Таблиця3[звання скорочено],MATCH('Ш Лист 1'!M22,Таблиця3[ПІБ],0)),"")</f>
-        <v>солд</v>
+      <c r="L22" s="83">
+        <f>IFERROR(INDEX(#REF!,MATCH('Ш Лист 1'!M22,#REF!,0)),"")</f>
       </c>
       <c r="M22" s="84" t="str">
         <f>IF(T22,$U$6,"")</f>
@@ -3449,9 +3210,8 @@
       <c r="F24" s="43"/>
       <c r="G24" s="35"/>
       <c r="H24" s="8"/>
-      <c r="I24" s="83" t="str">
-        <f>IFERROR(INDEX(Таблиця3[звання скорочено],MATCH('Ш Лист 1'!J24,Таблиця3[ПІБ],0)),"")</f>
-        <v>к-н</v>
+      <c r="I24" s="83">
+        <f>IFERROR(INDEX(#REF!,MATCH('Ш Лист 1'!J24,#REF!,0)),"")</f>
       </c>
       <c r="J24" s="84" t="str">
         <f>IF(T24,$U$5,"")</f>
@@ -3461,9 +3221,8 @@
         <f>IF(T24,T24,"")</f>
         <v>45198</v>
       </c>
-      <c r="L24" s="83" t="str">
-        <f>IFERROR(INDEX(Таблиця3[звання скорочено],MATCH('Ш Лист 1'!M24,Таблиця3[ПІБ],0)),"")</f>
-        <v>солд</v>
+      <c r="L24" s="83">
+        <f>IFERROR(INDEX(#REF!,MATCH('Ш Лист 1'!M24,#REF!,0)),"")</f>
       </c>
       <c r="M24" s="84" t="str">
         <f>IF(T24,$U$6,"")</f>
@@ -3560,9 +3319,8 @@
       <c r="F26" s="43"/>
       <c r="G26" s="35"/>
       <c r="H26" s="8"/>
-      <c r="I26" s="83" t="str">
-        <f>IFERROR(INDEX(Таблиця3[звання скорочено],MATCH('Ш Лист 1'!J26,Таблиця3[ПІБ],0)),"")</f>
-        <v>к-н</v>
+      <c r="I26" s="83">
+        <f>IFERROR(INDEX(#REF!,MATCH('Ш Лист 1'!J26,#REF!,0)),"")</f>
       </c>
       <c r="J26" s="84" t="str">
         <f>IF(T26,$U$5,"")</f>
@@ -3572,9 +3330,8 @@
         <f>IF(T26,T26,"")</f>
         <v>45198</v>
       </c>
-      <c r="L26" s="83" t="str">
-        <f>IFERROR(INDEX(Таблиця3[звання скорочено],MATCH('Ш Лист 1'!M26,Таблиця3[ПІБ],0)),"")</f>
-        <v>солд</v>
+      <c r="L26" s="83">
+        <f>IFERROR(INDEX(#REF!,MATCH('Ш Лист 1'!M26,#REF!,0)),"")</f>
       </c>
       <c r="M26" s="84" t="str">
         <f>IF(T26,$U$6,"")</f>
@@ -3658,7 +3415,7 @@
       <c r="G28" s="35"/>
       <c r="H28" s="8"/>
       <c r="I28" s="83">
-        <f>IFERROR(INDEX(Таблиця3[звання скорочено],MATCH('Ш Лист 1'!J28,Таблиця3[ПІБ],0)),"")</f>
+        <f>IFERROR(INDEX(#REF!,MATCH('Ш Лист 1'!J28,#REF!,0)),"")</f>
       </c>
       <c r="J28" s="84">
         <f>IF(T28,$U$5,"")</f>
@@ -3667,7 +3424,7 @@
         <f>IF(T28,T28,"")</f>
       </c>
       <c r="L28" s="83">
-        <f>IFERROR(INDEX(Таблиця3[звання скорочено],MATCH('Ш Лист 1'!M28,Таблиця3[ПІБ],0)),"")</f>
+        <f>IFERROR(INDEX(#REF!,MATCH('Ш Лист 1'!M28,#REF!,0)),"")</f>
       </c>
       <c r="M28" s="84">
         <f>IF(T28,$U$6,"")</f>
@@ -3736,7 +3493,7 @@
       <c r="G30" s="35"/>
       <c r="H30" s="8"/>
       <c r="I30" s="83">
-        <f>IFERROR(INDEX(Таблиця3[звання скорочено],MATCH('Ш Лист 1'!J30,Таблиця3[ПІБ],0)),"")</f>
+        <f>IFERROR(INDEX(#REF!,MATCH('Ш Лист 1'!J30,#REF!,0)),"")</f>
       </c>
       <c r="J30" s="84">
         <f>IF(T30,$U$5,"")</f>
@@ -3745,7 +3502,7 @@
         <f>IF(T30,T30,"")</f>
       </c>
       <c r="L30" s="83">
-        <f>IFERROR(INDEX(Таблиця3[звання скорочено],MATCH('Ш Лист 1'!M30,Таблиця3[ПІБ],0)),"")</f>
+        <f>IFERROR(INDEX(#REF!,MATCH('Ш Лист 1'!M30,#REF!,0)),"")</f>
       </c>
       <c r="M30" s="84">
         <f>IF(T30,$U$6,"")</f>
@@ -5129,7 +4886,7 @@
         <v>110</v>
       </c>
       <c r="G26" s="19">
-        <f>IFERROR(INDEX(Таблиця3[звання],MATCH(N26,Таблиця3[ПІБ],0)),"")</f>
+        <f>IFERROR(INDEX(#REF!,MATCH(N26,#REF!,0)),"")</f>
       </c>
       <c r="H26" s="141"/>
       <c r="I26" s="141"/>

</xml_diff>

<commit_message>
Table styles and scroll
Refactored styles for Directory table with using anothers styles. A bit hardcoding but with better visual interface
</commit_message>
<xml_diff>
--- a/src/backend/fileStorage/excel/roadXS.xlsx
+++ b/src/backend/fileStorage/excel/roadXS.xlsx
@@ -57,7 +57,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="307" uniqueCount="159">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="320" uniqueCount="160">
   <si>
     <t>року</t>
   </si>
@@ -497,7 +497,7 @@
     <t>жигуль</t>
   </si>
   <si>
-    <t>BB1234ЗД</t>
+    <t>BB1234ЗA</t>
   </si>
   <si>
     <t>ДТ</t>
@@ -524,7 +524,7 @@
     <t>Старший сержант</t>
   </si>
   <si>
-    <t>Відділ</t>
+    <t>А0000 (ПВЗ)</t>
   </si>
   <si>
     <t>Іван І.І.</t>
@@ -545,19 +545,22 @@
     <t>Майбах С.Т.</t>
   </si>
   <si>
-    <t>BB1234ЗЦ</t>
-  </si>
-  <si>
-    <t>BB1234ЗQ</t>
-  </si>
-  <si>
-    <t>BB1234ЗL</t>
-  </si>
-  <si>
-    <t>BB1234Зa</t>
-  </si>
-  <si>
-    <t>BB1234ЗK</t>
+    <t>BB1234ЗX</t>
+  </si>
+  <si>
+    <t>BB12342X</t>
+  </si>
+  <si>
+    <t>BB12344X</t>
+  </si>
+  <si>
+    <t>BB12345X</t>
+  </si>
+  <si>
+    <t>BB12346X</t>
+  </si>
+  <si>
+    <t>BB12347X</t>
   </si>
 </sst>
 </file>
@@ -2210,7 +2213,47 @@
         <v>149</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25"/>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>137</v>
+      </c>
+      <c r="B9" t="s">
+        <v>159</v>
+      </c>
+      <c r="C9" t="s">
+        <v>139</v>
+      </c>
+      <c r="D9" t="s">
+        <v>140</v>
+      </c>
+      <c r="E9" t="s">
+        <v>141</v>
+      </c>
+      <c r="F9" t="s">
+        <v>142</v>
+      </c>
+      <c r="G9" t="s">
+        <v>143</v>
+      </c>
+      <c r="H9" t="s">
+        <v>144</v>
+      </c>
+      <c r="I9" t="s">
+        <v>145</v>
+      </c>
+      <c r="J9" t="s">
+        <v>146</v>
+      </c>
+      <c r="K9" t="s">
+        <v>147</v>
+      </c>
+      <c r="L9" t="s">
+        <v>148</v>
+      </c>
+      <c r="M9" t="s">
+        <v>149</v>
+      </c>
+    </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25"/>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25"/>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
modal delete and add form
</commit_message>
<xml_diff>
--- a/src/backend/fileStorage/excel/roadXS.xlsx
+++ b/src/backend/fileStorage/excel/roadXS.xlsx
@@ -57,7 +57,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="155">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="268" uniqueCount="167">
   <si>
     <t>року</t>
   </si>
@@ -546,6 +546,42 @@
   </si>
   <si>
     <t>BB12347Й</t>
+  </si>
+  <si>
+    <t>Камаз</t>
+  </si>
+  <si>
+    <t>AS1234A5</t>
+  </si>
+  <si>
+    <t>voda</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>maslo</t>
+  </si>
+  <si>
+    <t>Tr</t>
+  </si>
+  <si>
+    <t>Transportna</t>
+  </si>
+  <si>
+    <t>Кирил П.Ы.</t>
+  </si>
+  <si>
+    <t>Pilot</t>
+  </si>
+  <si>
+    <t>AZOV</t>
+  </si>
+  <si>
+    <t>Мазок К.Й.</t>
+  </si>
+  <si>
+    <t>Bog</t>
   </si>
 </sst>
 </file>
@@ -2034,7 +2070,47 @@
         <v>149</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25"/>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>155</v>
+      </c>
+      <c r="B5" t="s">
+        <v>156</v>
+      </c>
+      <c r="C5" t="s">
+        <v>157</v>
+      </c>
+      <c r="D5" t="s">
+        <v>158</v>
+      </c>
+      <c r="E5" t="s">
+        <v>159</v>
+      </c>
+      <c r="F5" t="s">
+        <v>142</v>
+      </c>
+      <c r="G5" t="s">
+        <v>160</v>
+      </c>
+      <c r="H5" t="s">
+        <v>161</v>
+      </c>
+      <c r="I5" t="s">
+        <v>162</v>
+      </c>
+      <c r="J5" t="s">
+        <v>163</v>
+      </c>
+      <c r="K5" t="s">
+        <v>164</v>
+      </c>
+      <c r="L5" t="s">
+        <v>165</v>
+      </c>
+      <c r="M5" t="s">
+        <v>166</v>
+      </c>
+    </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25"/>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25"/>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Calendar + dropdown modal
</commit_message>
<xml_diff>
--- a/src/backend/fileStorage/excel/roadXS.xlsx
+++ b/src/backend/fileStorage/excel/roadXS.xlsx
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="365" uniqueCount="194">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="381" uniqueCount="202">
   <si>
     <t>року</t>
   </si>
@@ -664,6 +664,30 @@
   </si>
   <si>
     <t>Генерал Й.К.</t>
+  </si>
+  <si>
+    <t>Водiй</t>
+  </si>
+  <si>
+    <t>майор</t>
+  </si>
+  <si>
+    <t>м-р</t>
+  </si>
+  <si>
+    <t>Оранж В.Ф.</t>
+  </si>
+  <si>
+    <t>водій</t>
+  </si>
+  <si>
+    <t>Чек А.Ф.</t>
+  </si>
+  <si>
+    <t>Попов Й.Й.</t>
+  </si>
+  <si>
+    <t>Ловин У.У.</t>
   </si>
 </sst>
 </file>
@@ -1796,7 +1820,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:AC6"/>
+  <dimension ref="A2:AC10"/>
   <sheetViews>
     <sheetView workbookViewId="0" zoomScale="100" zoomScaleNormal="100">
       <selection activeCell="P9" sqref="P9"/>
@@ -2073,6 +2097,62 @@
       </c>
       <c r="V6" t="s">
         <v>193</v>
+      </c>
+    </row>
+    <row r="7" spans="19:22" x14ac:dyDescent="0.25">
+      <c r="S7" t="s">
+        <v>194</v>
+      </c>
+      <c r="T7" t="s">
+        <v>195</v>
+      </c>
+      <c r="U7" t="s">
+        <v>196</v>
+      </c>
+      <c r="V7" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="8" spans="19:22" x14ac:dyDescent="0.25">
+      <c r="S8" t="s">
+        <v>198</v>
+      </c>
+      <c r="T8" t="s">
+        <v>171</v>
+      </c>
+      <c r="U8" t="s">
+        <v>172</v>
+      </c>
+      <c r="V8" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="9" spans="19:22" x14ac:dyDescent="0.25">
+      <c r="S9" t="s">
+        <v>198</v>
+      </c>
+      <c r="T9" t="s">
+        <v>195</v>
+      </c>
+      <c r="U9" t="s">
+        <v>196</v>
+      </c>
+      <c r="V9" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="10" spans="19:22" x14ac:dyDescent="0.25">
+      <c r="S10" t="s">
+        <v>144</v>
+      </c>
+      <c r="T10" t="s">
+        <v>195</v>
+      </c>
+      <c r="U10" t="s">
+        <v>196</v>
+      </c>
+      <c r="V10" t="s">
+        <v>201</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Calendar + dropdown modal+favicon
</commit_message>
<xml_diff>
--- a/src/backend/fileStorage/excel/roadXS.xlsx
+++ b/src/backend/fileStorage/excel/roadXS.xlsx
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="381" uniqueCount="202">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="385" uniqueCount="203">
   <si>
     <t>року</t>
   </si>
@@ -688,6 +688,9 @@
   </si>
   <si>
     <t>Ловин У.У.</t>
+  </si>
+  <si>
+    <t>Филин В.В.</t>
   </si>
 </sst>
 </file>
@@ -1820,7 +1823,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:AC10"/>
+  <dimension ref="A2:AC11"/>
   <sheetViews>
     <sheetView workbookViewId="0" zoomScale="100" zoomScaleNormal="100">
       <selection activeCell="P9" sqref="P9"/>
@@ -2153,6 +2156,20 @@
       </c>
       <c r="V10" t="s">
         <v>201</v>
+      </c>
+    </row>
+    <row r="11" spans="19:22" x14ac:dyDescent="0.25">
+      <c r="S11" t="s">
+        <v>13</v>
+      </c>
+      <c r="T11" t="s">
+        <v>171</v>
+      </c>
+      <c r="U11" t="s">
+        <v>172</v>
+      </c>
+      <c r="V11" t="s">
+        <v>202</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Calendar Style + changes input
</commit_message>
<xml_diff>
--- a/src/backend/fileStorage/excel/roadXS.xlsx
+++ b/src/backend/fileStorage/excel/roadXS.xlsx
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="385" uniqueCount="203">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="389" uniqueCount="204">
   <si>
     <t>року</t>
   </si>
@@ -691,6 +691,9 @@
   </si>
   <si>
     <t>Филин В.В.</t>
+  </si>
+  <si>
+    <t>Орлятко У.У.</t>
   </si>
 </sst>
 </file>
@@ -1823,7 +1826,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:AC11"/>
+  <dimension ref="A2:AC12"/>
   <sheetViews>
     <sheetView workbookViewId="0" zoomScale="100" zoomScaleNormal="100">
       <selection activeCell="P9" sqref="P9"/>
@@ -2170,6 +2173,20 @@
       </c>
       <c r="V11" t="s">
         <v>202</v>
+      </c>
+    </row>
+    <row r="12" spans="19:22" x14ac:dyDescent="0.25">
+      <c r="S12" t="s">
+        <v>13</v>
+      </c>
+      <c r="T12" t="s">
+        <v>171</v>
+      </c>
+      <c r="U12" t="s">
+        <v>172</v>
+      </c>
+      <c r="V12" t="s">
+        <v>203</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Sending data from Modals to CarGeneralInfo
</commit_message>
<xml_diff>
--- a/src/backend/fileStorage/excel/roadXS.xlsx
+++ b/src/backend/fileStorage/excel/roadXS.xlsx
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="393" uniqueCount="209">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="401" uniqueCount="211">
   <si>
     <t>року</t>
   </si>
@@ -709,6 +709,12 @@
   </si>
   <si>
     <t>Баран І.Й.</t>
+  </si>
+  <si>
+    <t>Вар Ц.Ц.</t>
+  </si>
+  <si>
+    <t>Диван Ф.Ф.</t>
   </si>
 </sst>
 </file>
@@ -1841,7 +1847,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:AC13"/>
+  <dimension ref="A2:AC15"/>
   <sheetViews>
     <sheetView workbookViewId="0" zoomScale="100" zoomScaleNormal="100">
       <selection activeCell="P9" sqref="P9"/>
@@ -2216,6 +2222,34 @@
       </c>
       <c r="V13" t="s">
         <v>208</v>
+      </c>
+    </row>
+    <row r="14" spans="19:22" x14ac:dyDescent="0.25">
+      <c r="S14" t="s">
+        <v>17</v>
+      </c>
+      <c r="T14" t="s">
+        <v>195</v>
+      </c>
+      <c r="U14" t="s">
+        <v>196</v>
+      </c>
+      <c r="V14" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="15" spans="19:22" x14ac:dyDescent="0.25">
+      <c r="S15" t="s">
+        <v>37</v>
+      </c>
+      <c r="T15" t="s">
+        <v>171</v>
+      </c>
+      <c r="U15" t="s">
+        <v>172</v>
+      </c>
+      <c r="V15" t="s">
+        <v>210</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
409 fixed, update WIP
</commit_message>
<xml_diff>
--- a/src/backend/fileStorage/excel/roadXS.xlsx
+++ b/src/backend/fileStorage/excel/roadXS.xlsx
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="393" uniqueCount="201">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="605" uniqueCount="211">
   <si>
     <t>року</t>
   </si>
@@ -169,6 +169,12 @@
     <t>За нарядом</t>
   </si>
   <si>
+    <t>7:30 29.09.2023</t>
+  </si>
+  <si>
+    <t>18:10 29.09.2023</t>
+  </si>
+  <si>
     <t>EndSpeedometer4</t>
   </si>
   <si>
@@ -304,6 +310,9 @@
     <t>AA1234FF</t>
   </si>
   <si>
+    <t>Транспорт</t>
+  </si>
+  <si>
     <t>1. Витрата пально-мастильних матеріалів (у літрах)</t>
   </si>
   <si>
@@ -347,9 +356,6 @@
   </si>
   <si>
     <t>Масло</t>
-  </si>
-  <si>
-    <t>24</t>
   </si>
   <si>
     <t>Марка машини</t>
@@ -416,10 +422,25 @@
     <t>Корінець дорожнього листа</t>
   </si>
   <si>
-    <t>Кременець - Тернопіль</t>
-  </si>
-  <si>
-    <t>Львів - Хмельницький - Львів</t>
+    <t>Київ - Вінниця - Київ</t>
+  </si>
+  <si>
+    <t>7:30, 29.00.23</t>
+  </si>
+  <si>
+    <t>18:10, 29.00.23</t>
+  </si>
+  <si>
+    <t>Пісок</t>
+  </si>
+  <si>
+    <t>Тернопіль - Львів</t>
+  </si>
+  <si>
+    <t>7:30, 30.00.23</t>
+  </si>
+  <si>
+    <t>18:10, 31.00.23</t>
   </si>
   <si>
     <t>Всього:</t>
@@ -428,10 +449,16 @@
     <t>Рух по дорозі з покращеним покриттям</t>
   </si>
   <si>
+    <t>ДТ</t>
+  </si>
+  <si>
     <t>x</t>
   </si>
   <si>
     <t>-</t>
+  </si>
+  <si>
+    <t>15%</t>
   </si>
   <si>
     <t>=</t>
@@ -555,18 +582,21 @@
     <t>маршрут</t>
   </si>
   <si>
-    <t>тойота корола</t>
+    <t>тойота</t>
   </si>
   <si>
     <t>AI8523FE</t>
   </si>
   <si>
-    <t>ДТ</t>
+    <t>12</t>
   </si>
   <si>
     <t>10w40</t>
   </si>
   <si>
+    <t>1.5</t>
+  </si>
+  <si>
     <t>Тр</t>
   </si>
   <si>
@@ -615,7 +645,7 @@
     <t>CE0548IS</t>
   </si>
   <si>
-    <t>Чек А.Ф.</t>
+    <t>Чекаут А.Ф.</t>
   </si>
   <si>
     <t>сержант</t>
@@ -624,67 +654,67 @@
     <t>старший відділення</t>
   </si>
   <si>
-    <t>мерседес транз</t>
-  </si>
-  <si>
-    <t>AS0025A5</t>
-  </si>
-  <si>
-    <t>Бензин</t>
-  </si>
-  <si>
-    <t>5w40</t>
+    <t>Reno</t>
+  </si>
+  <si>
+    <t>ДЖ1548ВБ</t>
+  </si>
+  <si>
+    <t>Дріжі</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>Тісто</t>
+  </si>
+  <si>
+    <t>харч.</t>
+  </si>
+  <si>
+    <t>Харчова</t>
+  </si>
+  <si>
+    <t>Щітмен Д.Р.</t>
+  </si>
+  <si>
+    <t>Їдалка</t>
+  </si>
+  <si>
+    <t>майор</t>
+  </si>
+  <si>
+    <t>м-р</t>
+  </si>
+  <si>
+    <t>Вар Ц.Ц.</t>
+  </si>
+  <si>
+    <t>Хліб</t>
+  </si>
+  <si>
+    <t>ДЖ1548ВК</t>
+  </si>
+  <si>
+    <t>с-т</t>
+  </si>
+  <si>
+    <t>Диван Ф.Ф.</t>
+  </si>
+  <si>
+    <t>соладт</t>
   </si>
   <si>
     <t>Попов Й.Й.</t>
   </si>
   <si>
-    <t>AZOV</t>
-  </si>
-  <si>
-    <t>майор</t>
-  </si>
-  <si>
-    <t>м-р</t>
-  </si>
-  <si>
-    <t>Вар Ц.Ц.</t>
-  </si>
-  <si>
-    <t>Порш</t>
-  </si>
-  <si>
-    <t>AS1234AV</t>
-  </si>
-  <si>
-    <t>voda</t>
-  </si>
-  <si>
-    <t>4</t>
-  </si>
-  <si>
-    <t>maslo</t>
-  </si>
-  <si>
-    <t>1</t>
-  </si>
-  <si>
-    <t>Tr</t>
-  </si>
-  <si>
-    <t>Transportna</t>
-  </si>
-  <si>
     <t>Кирило Володимир Петрович</t>
   </si>
   <si>
-    <t>с-т</t>
-  </si>
-  <si>
-    <t>Диван Ф.Ф.</t>
-  </si>
-  <si>
-    <t>соладт</t>
+    <t>водій</t>
+  </si>
+  <si>
+    <t>Тестовий А.А.</t>
   </si>
 </sst>
 </file>
@@ -1079,7 +1109,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="133">
+  <cellXfs count="134">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1363,14 +1393,23 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="28" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1820,7 +1859,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:AC10"/>
+  <dimension ref="A2:AC11"/>
   <sheetViews>
     <sheetView workbookViewId="0" zoomScale="100" zoomScaleNormal="100">
       <selection activeCell="F18" sqref="F18"/>
@@ -1849,119 +1888,119 @@
     <col min="29" max="29" width="34.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" ht="45" customHeight="1" spans="1:29" s="130" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="130" t="s">
-        <v>135</v>
-      </c>
-      <c r="B2" s="130" t="s">
-        <v>136</v>
-      </c>
-      <c r="C2" s="130" t="s">
-        <v>137</v>
-      </c>
-      <c r="D2" s="130" t="s">
-        <v>138</v>
-      </c>
-      <c r="E2" s="130" t="s">
-        <v>139</v>
-      </c>
-      <c r="F2" s="130" t="s">
-        <v>140</v>
-      </c>
-      <c r="G2" s="130" t="s">
-        <v>75</v>
-      </c>
-      <c r="H2" s="130" t="s">
-        <v>141</v>
-      </c>
-      <c r="I2" s="130" t="s">
+    <row r="2" ht="45" customHeight="1" spans="1:29" s="131" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="131" t="s">
+        <v>144</v>
+      </c>
+      <c r="B2" s="131" t="s">
+        <v>145</v>
+      </c>
+      <c r="C2" s="131" t="s">
+        <v>146</v>
+      </c>
+      <c r="D2" s="131" t="s">
+        <v>147</v>
+      </c>
+      <c r="E2" s="131" t="s">
+        <v>148</v>
+      </c>
+      <c r="F2" s="131" t="s">
+        <v>149</v>
+      </c>
+      <c r="G2" s="131" t="s">
+        <v>77</v>
+      </c>
+      <c r="H2" s="131" t="s">
+        <v>150</v>
+      </c>
+      <c r="I2" s="131" t="s">
         <v>10</v>
       </c>
-      <c r="J2" s="130" t="s">
-        <v>142</v>
-      </c>
-      <c r="K2" s="130" t="s">
-        <v>143</v>
-      </c>
-      <c r="L2" s="130" t="s">
-        <v>144</v>
-      </c>
-      <c r="M2" s="130" t="s">
-        <v>145</v>
-      </c>
-      <c r="O2" s="130" t="s">
-        <v>146</v>
-      </c>
-      <c r="P2" s="130" t="s">
-        <v>147</v>
-      </c>
-      <c r="Q2" s="130" t="s">
-        <v>148</v>
-      </c>
-      <c r="S2" s="130" t="s">
-        <v>149</v>
-      </c>
-      <c r="T2" s="130" t="s">
-        <v>150</v>
-      </c>
-      <c r="U2" s="130" t="s">
+      <c r="J2" s="131" t="s">
         <v>151</v>
       </c>
-      <c r="V2" s="130" t="s">
+      <c r="K2" s="131" t="s">
         <v>152</v>
       </c>
-      <c r="Y2" s="130" t="s">
-        <v>146</v>
-      </c>
-      <c r="Z2" s="130" t="s">
+      <c r="L2" s="131" t="s">
         <v>153</v>
       </c>
-      <c r="AA2" s="130" t="s">
+      <c r="M2" s="131" t="s">
         <v>154</v>
       </c>
-      <c r="AB2" s="130" t="s">
+      <c r="O2" s="131" t="s">
         <v>155</v>
       </c>
-      <c r="AC2" s="130" t="s">
+      <c r="P2" s="131" t="s">
         <v>156</v>
+      </c>
+      <c r="Q2" s="131" t="s">
+        <v>157</v>
+      </c>
+      <c r="S2" s="131" t="s">
+        <v>158</v>
+      </c>
+      <c r="T2" s="131" t="s">
+        <v>159</v>
+      </c>
+      <c r="U2" s="131" t="s">
+        <v>160</v>
+      </c>
+      <c r="V2" s="131" t="s">
+        <v>161</v>
+      </c>
+      <c r="Y2" s="131" t="s">
+        <v>155</v>
+      </c>
+      <c r="Z2" s="131" t="s">
+        <v>162</v>
+      </c>
+      <c r="AA2" s="131" t="s">
+        <v>163</v>
+      </c>
+      <c r="AB2" s="131" t="s">
+        <v>164</v>
+      </c>
+      <c r="AC2" s="131" t="s">
+        <v>165</v>
       </c>
     </row>
     <row r="3" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>157</v>
+        <v>166</v>
       </c>
       <c r="B3" t="s">
-        <v>158</v>
+        <v>167</v>
       </c>
       <c r="C3" t="s">
-        <v>159</v>
-      </c>
-      <c r="D3">
-        <v>12</v>
+        <v>129</v>
+      </c>
+      <c r="D3" t="s">
+        <v>168</v>
       </c>
       <c r="E3" t="s">
-        <v>160</v>
-      </c>
-      <c r="F3">
-        <v>1.5</v>
+        <v>169</v>
+      </c>
+      <c r="F3" t="s">
+        <v>170</v>
       </c>
       <c r="G3" t="s">
-        <v>161</v>
+        <v>171</v>
       </c>
       <c r="H3" t="s">
-        <v>162</v>
+        <v>172</v>
       </c>
       <c r="I3" t="s">
-        <v>163</v>
+        <v>173</v>
       </c>
       <c r="J3" t="s">
-        <v>164</v>
+        <v>174</v>
       </c>
       <c r="K3" t="s">
-        <v>165</v>
+        <v>175</v>
       </c>
       <c r="L3" t="s">
-        <v>166</v>
+        <v>176</v>
       </c>
       <c r="M3" t="s">
         <v>14</v>
@@ -1970,163 +2009,163 @@
         <v>10</v>
       </c>
       <c r="P3" t="s">
-        <v>167</v>
-      </c>
-      <c r="Q3" s="131">
+        <v>177</v>
+      </c>
+      <c r="Q3" s="132">
         <v>0.15</v>
       </c>
       <c r="S3" t="s">
-        <v>168</v>
+        <v>178</v>
       </c>
       <c r="T3" t="s">
-        <v>164</v>
+        <v>174</v>
       </c>
       <c r="U3" t="s">
-        <v>169</v>
+        <v>179</v>
       </c>
       <c r="V3" t="s">
-        <v>170</v>
+        <v>180</v>
       </c>
       <c r="Y3">
         <v>1</v>
       </c>
       <c r="Z3" t="s">
-        <v>171</v>
+        <v>181</v>
       </c>
       <c r="AA3" t="s">
-        <v>172</v>
+        <v>182</v>
       </c>
       <c r="AB3" t="s">
-        <v>173</v>
+        <v>183</v>
       </c>
       <c r="AC3" t="s">
-        <v>174</v>
+        <v>184</v>
       </c>
     </row>
     <row r="4" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>175</v>
+        <v>185</v>
       </c>
       <c r="B4" t="s">
-        <v>176</v>
+        <v>186</v>
       </c>
       <c r="C4" t="s">
-        <v>159</v>
+        <v>129</v>
       </c>
       <c r="D4">
         <v>9</v>
       </c>
       <c r="E4" t="s">
-        <v>160</v>
-      </c>
-      <c r="F4" s="132">
+        <v>169</v>
+      </c>
+      <c r="F4" s="133">
         <v>1.2</v>
       </c>
       <c r="G4" t="s">
-        <v>161</v>
+        <v>171</v>
       </c>
       <c r="H4" t="s">
-        <v>162</v>
+        <v>172</v>
       </c>
       <c r="I4" t="s">
-        <v>177</v>
+        <v>187</v>
       </c>
       <c r="J4" t="s">
-        <v>178</v>
+        <v>188</v>
       </c>
       <c r="K4" t="s">
-        <v>165</v>
+        <v>175</v>
       </c>
       <c r="L4" t="s">
-        <v>166</v>
+        <v>176</v>
       </c>
       <c r="M4" t="s">
         <v>14</v>
       </c>
       <c r="S4" t="s">
-        <v>179</v>
+        <v>189</v>
       </c>
       <c r="T4" t="s">
         <v>14</v>
       </c>
       <c r="U4" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="V4" t="s">
-        <v>166</v>
+        <v>176</v>
       </c>
     </row>
     <row r="5" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>190</v>
+      </c>
+      <c r="B5" t="s">
+        <v>191</v>
+      </c>
+      <c r="C5" t="s">
+        <v>192</v>
+      </c>
+      <c r="D5" t="s">
+        <v>193</v>
+      </c>
+      <c r="E5" t="s">
+        <v>194</v>
+      </c>
+      <c r="F5" t="s">
+        <v>193</v>
+      </c>
+      <c r="G5" t="s">
+        <v>195</v>
+      </c>
+      <c r="H5" t="s">
+        <v>196</v>
+      </c>
+      <c r="I5" t="s">
+        <v>197</v>
+      </c>
+      <c r="J5" t="s">
+        <v>188</v>
+      </c>
+      <c r="K5" t="s">
+        <v>198</v>
+      </c>
+      <c r="L5" t="s">
         <v>180</v>
       </c>
-      <c r="B5" t="s">
-        <v>181</v>
-      </c>
-      <c r="C5" t="s">
-        <v>182</v>
-      </c>
-      <c r="D5">
-        <v>11</v>
-      </c>
-      <c r="E5" t="s">
-        <v>183</v>
-      </c>
-      <c r="F5">
-        <v>1.1</v>
-      </c>
-      <c r="G5" t="s">
-        <v>161</v>
-      </c>
-      <c r="H5" t="s">
-        <v>162</v>
-      </c>
-      <c r="I5" t="s">
-        <v>184</v>
-      </c>
-      <c r="J5" t="s">
-        <v>11</v>
-      </c>
-      <c r="K5" t="s">
-        <v>185</v>
-      </c>
-      <c r="L5" t="s">
-        <v>166</v>
-      </c>
       <c r="M5" t="s">
-        <v>14</v>
+        <v>174</v>
       </c>
       <c r="S5" t="s">
         <v>17</v>
       </c>
       <c r="T5" t="s">
-        <v>186</v>
+        <v>199</v>
       </c>
       <c r="U5" t="s">
-        <v>187</v>
+        <v>200</v>
       </c>
       <c r="V5" t="s">
-        <v>188</v>
+        <v>201</v>
       </c>
     </row>
     <row r="6" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>189</v>
+        <v>202</v>
       </c>
       <c r="B6" t="s">
-        <v>190</v>
+        <v>203</v>
       </c>
       <c r="C6" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="D6" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="E6" t="s">
+        <v>194</v>
+      </c>
+      <c r="F6" t="s">
         <v>193</v>
-      </c>
-      <c r="F6" t="s">
-        <v>194</v>
       </c>
       <c r="G6" t="s">
         <v>195</v>
@@ -2135,31 +2174,31 @@
         <v>196</v>
       </c>
       <c r="I6" t="s">
-        <v>177</v>
+        <v>197</v>
       </c>
       <c r="J6" t="s">
-        <v>178</v>
+        <v>188</v>
       </c>
       <c r="K6" t="s">
-        <v>185</v>
+        <v>198</v>
       </c>
       <c r="L6" t="s">
-        <v>197</v>
+        <v>176</v>
       </c>
       <c r="M6" t="s">
         <v>14</v>
       </c>
       <c r="S6" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="T6" t="s">
-        <v>178</v>
+        <v>188</v>
       </c>
       <c r="U6" t="s">
-        <v>198</v>
+        <v>204</v>
       </c>
       <c r="V6" t="s">
-        <v>199</v>
+        <v>205</v>
       </c>
     </row>
     <row r="7" spans="1:22" x14ac:dyDescent="0.25">
@@ -2167,13 +2206,13 @@
         <v>10</v>
       </c>
       <c r="T7" t="s">
-        <v>164</v>
+        <v>174</v>
       </c>
       <c r="U7" t="s">
-        <v>169</v>
+        <v>179</v>
       </c>
       <c r="V7" t="s">
-        <v>163</v>
+        <v>173</v>
       </c>
     </row>
     <row r="8" spans="1:22" x14ac:dyDescent="0.25">
@@ -2181,13 +2220,13 @@
         <v>10</v>
       </c>
       <c r="T8" t="s">
-        <v>178</v>
+        <v>188</v>
       </c>
       <c r="U8" t="s">
-        <v>198</v>
+        <v>204</v>
       </c>
       <c r="V8" t="s">
-        <v>177</v>
+        <v>197</v>
       </c>
     </row>
     <row r="9" spans="1:22" x14ac:dyDescent="0.25">
@@ -2195,27 +2234,41 @@
         <v>10</v>
       </c>
       <c r="T9" t="s">
-        <v>200</v>
+        <v>206</v>
       </c>
       <c r="U9" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="V9" t="s">
-        <v>184</v>
+        <v>207</v>
       </c>
     </row>
     <row r="10" spans="1:22" x14ac:dyDescent="0.25">
       <c r="S10" t="s">
-        <v>144</v>
+        <v>153</v>
       </c>
       <c r="T10" t="s">
         <v>14</v>
       </c>
       <c r="U10" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="V10" t="s">
-        <v>197</v>
+        <v>208</v>
+      </c>
+    </row>
+    <row r="11" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="S11" t="s">
+        <v>209</v>
+      </c>
+      <c r="T11" t="s">
+        <v>188</v>
+      </c>
+      <c r="U11" t="s">
+        <v>204</v>
+      </c>
+      <c r="V11" t="s">
+        <v>210</v>
       </c>
     </row>
   </sheetData>
@@ -2564,14 +2617,14 @@
       <c r="O10" s="55" t="s">
         <v>35</v>
       </c>
-      <c r="P10" s="56">
-        <f>IF(T10,TEXT(U10,"ч:мм")&amp;" "&amp;TEXT(T10,"дд.мм.гггг"),"")</f>
+      <c r="P10" s="56" t="s">
+        <v>36</v>
       </c>
       <c r="Q10" s="55" t="s">
         <v>35</v>
       </c>
-      <c r="R10" s="57">
-        <f>IF(V10,TEXT(W10,"ч:мм")&amp;" "&amp;TEXT(V10,"дд.мм.гггг"),"")</f>
+      <c r="R10" s="57" t="s">
+        <v>37</v>
       </c>
       <c r="T10" s="58"/>
       <c r="U10" s="59"/>
@@ -2581,7 +2634,7 @@
         <v>19</v>
       </c>
       <c r="AF10" s="1" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="AG10" s="1" t="s">
         <v>21</v>
@@ -2602,16 +2655,16 @@
       <c r="J11" s="50"/>
       <c r="K11" s="51"/>
       <c r="L11" s="52" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="M11" s="53"/>
       <c r="N11" s="54"/>
       <c r="O11" s="60" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="P11" s="60"/>
       <c r="Q11" s="60" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="R11" s="60"/>
       <c r="T11" s="61"/>
@@ -2622,7 +2675,7 @@
         <v>19</v>
       </c>
       <c r="AF11" s="1" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="AG11" s="1" t="s">
         <v>21</v>
@@ -2647,31 +2700,31 @@
       <c r="G12" s="37"/>
       <c r="H12" s="8"/>
       <c r="I12" s="63" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="J12" s="63" t="s">
         <v>18</v>
       </c>
       <c r="K12" s="64" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="L12" s="63" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="M12" s="63" t="s">
+        <v>45</v>
+      </c>
+      <c r="N12" s="64" t="s">
         <v>43</v>
       </c>
-      <c r="N12" s="64" t="s">
-        <v>41</v>
-      </c>
       <c r="O12" s="63" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="P12" s="65">
         <v>12337</v>
       </c>
       <c r="Q12" s="63" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="R12" s="65">
         <v>12338</v>
@@ -2685,7 +2738,7 @@
         <v>19</v>
       </c>
       <c r="AF12" s="1" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="AG12" s="1" t="s">
         <v>21</v>
@@ -2705,20 +2758,20 @@
       <c r="H13" s="8"/>
       <c r="I13" s="67"/>
       <c r="J13" s="68" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="K13" s="17"/>
       <c r="L13" s="67"/>
       <c r="M13" s="68" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="N13" s="17"/>
       <c r="O13" s="69" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="P13" s="70"/>
       <c r="Q13" s="69" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="R13" s="71"/>
       <c r="T13" s="72"/>
@@ -2729,7 +2782,7 @@
         <v>19</v>
       </c>
       <c r="AF13" s="1" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="AG13" s="1" t="s">
         <v>21</v>
@@ -2748,31 +2801,31 @@
       <c r="G14" s="37"/>
       <c r="H14" s="8"/>
       <c r="I14" s="63" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="J14" s="63" t="s">
         <v>18</v>
       </c>
       <c r="K14" s="64" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="L14" s="63" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="M14" s="63" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="N14" s="64" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="O14" s="63" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="P14" s="75">
         <v>12339</v>
       </c>
       <c r="Q14" s="63" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="R14" s="65">
         <v>12340</v>
@@ -2786,7 +2839,7 @@
         <v>19</v>
       </c>
       <c r="AF14" s="1" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="AG14" s="1" t="s">
         <v>21</v>
@@ -2806,20 +2859,20 @@
       <c r="H15" s="8"/>
       <c r="I15" s="67"/>
       <c r="J15" s="68" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="K15" s="17"/>
       <c r="L15" s="67"/>
       <c r="M15" s="68" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="N15" s="17"/>
       <c r="O15" s="69" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="P15" s="70"/>
       <c r="Q15" s="69" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="R15" s="71"/>
       <c r="S15" s="76"/>
@@ -2831,7 +2884,7 @@
         <v>19</v>
       </c>
       <c r="AF15" s="1" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="AG15" s="1" t="s">
         <v>21</v>
@@ -2850,31 +2903,31 @@
       <c r="G16" s="37"/>
       <c r="H16" s="8"/>
       <c r="I16" s="63" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="J16" s="63" t="s">
         <v>18</v>
       </c>
       <c r="K16" s="64" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="L16" s="63" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="M16" s="63" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="N16" s="64" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="O16" s="63" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="P16" s="75">
         <v>12340</v>
       </c>
       <c r="Q16" s="63" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="R16" s="65">
         <v>12345</v>
@@ -2888,7 +2941,7 @@
         <v>19</v>
       </c>
       <c r="AF16" s="1" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="AG16" s="1" t="s">
         <v>21</v>
@@ -2908,20 +2961,20 @@
       <c r="H17" s="8"/>
       <c r="I17" s="67"/>
       <c r="J17" s="68" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="K17" s="77"/>
       <c r="L17" s="67"/>
       <c r="M17" s="68" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="N17" s="77"/>
       <c r="O17" s="69" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="P17" s="70"/>
       <c r="Q17" s="69" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="R17" s="71"/>
       <c r="S17" s="76"/>
@@ -2932,7 +2985,7 @@
     </row>
     <row r="18" ht="9.6" customHeight="1" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A18" s="78" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="B18" s="3"/>
       <c r="C18" s="24"/>
@@ -2942,31 +2995,31 @@
       <c r="G18" s="37"/>
       <c r="H18" s="8"/>
       <c r="I18" s="63" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="J18" s="63" t="s">
         <v>18</v>
       </c>
       <c r="K18" s="64" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="L18" s="63" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="M18" s="63" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="N18" s="64" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="O18" s="63" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="P18" s="75">
         <v>12345</v>
       </c>
       <c r="Q18" s="63" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="R18" s="65">
         <v>12349</v>
@@ -2988,20 +3041,20 @@
       <c r="H19" s="8"/>
       <c r="I19" s="67"/>
       <c r="J19" s="68" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="K19" s="77"/>
       <c r="L19" s="67"/>
       <c r="M19" s="68" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="N19" s="77"/>
       <c r="O19" s="69" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="P19" s="70"/>
       <c r="Q19" s="69" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="R19" s="71"/>
       <c r="S19" s="76"/>
@@ -3013,7 +3066,7 @@
     <row r="20" ht="9.6" customHeight="1" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A20" s="78"/>
       <c r="B20" s="24" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="C20" s="24"/>
       <c r="D20" s="4"/>
@@ -3022,31 +3075,31 @@
       <c r="G20" s="37"/>
       <c r="H20" s="8"/>
       <c r="I20" s="63" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="J20" s="63" t="s">
         <v>18</v>
       </c>
       <c r="K20" s="64" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="L20" s="63" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="M20" s="63" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="N20" s="64" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="O20" s="63" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="P20" s="75">
         <v>12349</v>
       </c>
       <c r="Q20" s="63" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="R20" s="65">
         <v>12353</v>
@@ -3068,20 +3121,20 @@
       <c r="H21" s="8"/>
       <c r="I21" s="67"/>
       <c r="J21" s="68" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="K21" s="77"/>
       <c r="L21" s="67"/>
       <c r="M21" s="68" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="N21" s="77"/>
       <c r="O21" s="69" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="P21" s="70"/>
       <c r="Q21" s="69" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="R21" s="71"/>
       <c r="S21" s="76"/>
@@ -3100,34 +3153,34 @@
       <c r="G22" s="37"/>
       <c r="H22" s="8"/>
       <c r="I22" s="63" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="J22" s="63" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="K22" s="64" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="L22" s="63" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="M22" s="63" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="N22" s="64" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="O22" s="63" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="P22" s="75" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="Q22" s="63" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="R22" s="65" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="S22" s="76"/>
       <c r="T22" s="58"/>
@@ -3146,20 +3199,20 @@
       <c r="H23" s="8"/>
       <c r="I23" s="67"/>
       <c r="J23" s="68" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="K23" s="77"/>
       <c r="L23" s="67"/>
       <c r="M23" s="68" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="N23" s="77"/>
       <c r="O23" s="69" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="P23" s="70"/>
       <c r="Q23" s="69" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="R23" s="71"/>
       <c r="S23" s="76"/>
@@ -3178,34 +3231,34 @@
       <c r="G24" s="37"/>
       <c r="H24" s="8"/>
       <c r="I24" s="63" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="J24" s="63" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="K24" s="64" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="L24" s="63" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="M24" s="63" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="N24" s="64" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="O24" s="63" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="P24" s="75" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="Q24" s="63" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="R24" s="65" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="S24" s="76"/>
       <c r="T24" s="58"/>
@@ -3224,20 +3277,20 @@
       <c r="H25" s="8"/>
       <c r="I25" s="67"/>
       <c r="J25" s="68" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="K25" s="77"/>
       <c r="L25" s="67"/>
       <c r="M25" s="68" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="N25" s="77"/>
       <c r="O25" s="69" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="P25" s="70"/>
       <c r="Q25" s="69" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="R25" s="71"/>
       <c r="S25" s="76"/>
@@ -3258,34 +3311,34 @@
       <c r="G26" s="37"/>
       <c r="H26" s="8"/>
       <c r="I26" s="63" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="J26" s="63" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="K26" s="64" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="L26" s="63" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="M26" s="63" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="N26" s="64" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="O26" s="63" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="P26" s="75" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="Q26" s="63" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="R26" s="65" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="S26" s="76"/>
       <c r="T26" s="58"/>
@@ -3304,20 +3357,20 @@
       <c r="H27" s="8"/>
       <c r="I27" s="67"/>
       <c r="J27" s="68" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="K27" s="77"/>
       <c r="L27" s="67"/>
       <c r="M27" s="68" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="N27" s="77"/>
       <c r="O27" s="69" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="P27" s="70"/>
       <c r="Q27" s="69" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="R27" s="71"/>
       <c r="S27" s="76"/>
@@ -3336,34 +3389,34 @@
       <c r="G28" s="37"/>
       <c r="H28" s="8"/>
       <c r="I28" s="63" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="J28" s="63" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="K28" s="64" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="L28" s="63" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="M28" s="63" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="N28" s="64" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="O28" s="63" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="P28" s="75" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="Q28" s="63" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="R28" s="65" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="S28" s="76"/>
       <c r="T28" s="58"/>
@@ -3382,20 +3435,20 @@
       <c r="H29" s="8"/>
       <c r="I29" s="67"/>
       <c r="J29" s="68" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="K29" s="77"/>
       <c r="L29" s="67"/>
       <c r="M29" s="68" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="N29" s="77"/>
       <c r="O29" s="69" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="P29" s="70"/>
       <c r="Q29" s="69" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="R29" s="71"/>
       <c r="S29" s="76"/>
@@ -3414,34 +3467,34 @@
       <c r="G30" s="37"/>
       <c r="H30" s="8"/>
       <c r="I30" s="63" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="J30" s="63" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="K30" s="64" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="L30" s="63" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="M30" s="63" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="N30" s="64" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="O30" s="63" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="P30" s="75" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="Q30" s="63" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="R30" s="65" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="S30" s="76"/>
       <c r="T30" s="58"/>
@@ -3460,20 +3513,20 @@
       <c r="H31" s="8"/>
       <c r="I31" s="67"/>
       <c r="J31" s="68" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="K31" s="17"/>
       <c r="L31" s="67"/>
       <c r="M31" s="68" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="N31" s="17"/>
       <c r="O31" s="69" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="P31" s="70"/>
       <c r="Q31" s="69" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="R31" s="71"/>
       <c r="T31" s="72"/>
@@ -3491,34 +3544,34 @@
       <c r="G32" s="37"/>
       <c r="H32" s="8"/>
       <c r="I32" s="82" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="J32" s="82" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="K32" s="82" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="L32" s="82" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="M32" s="83" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="N32" s="83" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="O32" s="83" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="P32" s="83" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="Q32" s="83" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="R32" s="83" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
     </row>
     <row r="33" ht="25.7" customHeight="1" spans="1:19" s="50" customFormat="1" x14ac:dyDescent="0.25">
@@ -3541,21 +3594,20 @@
         <v>3</v>
       </c>
       <c r="K33" s="88" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="L33" s="89" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="M33" s="86" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="N33" s="89"/>
       <c r="O33" s="86">
         <f>IFERROR(INDEX(#REF!,MATCH('Ш Лист 1'!N33,#REF!,0)),"")</f>
       </c>
-      <c r="P33" s="86" t="e">
-        <f>INDEX(#REF!,MATCH('Ш Лист 1'!L33,#REF!,0))</f>
-        <v>#REF!</v>
+      <c r="P33" s="86" t="s">
+        <v>83</v>
       </c>
       <c r="Q33" s="86"/>
       <c r="R33" s="86"/>
@@ -3571,7 +3623,7 @@
       <c r="G34" s="37"/>
       <c r="H34" s="8"/>
       <c r="I34" s="91" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="J34" s="92"/>
       <c r="K34" s="92"/>
@@ -3588,42 +3640,42 @@
       <c r="A35" s="78"/>
       <c r="B35" s="84"/>
       <c r="C35" s="24" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="D35" s="4"/>
       <c r="E35" s="5"/>
       <c r="F35" s="24" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="G35" s="37"/>
       <c r="H35" s="8"/>
       <c r="I35" s="82" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="J35" s="82" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="K35" s="82" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="L35" s="94" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="M35" s="95"/>
       <c r="N35" s="83" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="O35" s="83" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="P35" s="83" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="Q35" s="83" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="R35" s="83" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
     </row>
     <row r="36" ht="10.7" customHeight="1" spans="1:19" x14ac:dyDescent="0.25">
@@ -3631,25 +3683,25 @@
       <c r="B36" s="84"/>
       <c r="C36" s="24"/>
       <c r="D36" s="24" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="E36" s="24" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="F36" s="24"/>
       <c r="G36" s="96"/>
       <c r="H36" s="8"/>
       <c r="I36" s="97" t="s">
-        <v>95</v>
-      </c>
-      <c r="J36" s="98" t="s">
-        <v>96</v>
+        <v>98</v>
+      </c>
+      <c r="J36" s="98">
+        <v>24</v>
       </c>
       <c r="K36" s="98">
         <v>10</v>
       </c>
       <c r="L36" s="99" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="M36" s="98">
         <v>5</v>
@@ -3678,15 +3730,33 @@
       <c r="F37" s="24"/>
       <c r="G37" s="96"/>
       <c r="H37" s="8"/>
-      <c r="I37" s="97"/>
-      <c r="J37" s="98"/>
-      <c r="K37" s="98"/>
-      <c r="L37" s="99"/>
-      <c r="M37" s="98"/>
-      <c r="N37" s="100"/>
-      <c r="O37" s="100"/>
-      <c r="P37" s="100"/>
-      <c r="Q37" s="100"/>
+      <c r="I37" s="97" t="s">
+        <v>69</v>
+      </c>
+      <c r="J37" s="98" t="s">
+        <v>69</v>
+      </c>
+      <c r="K37" s="98" t="s">
+        <v>69</v>
+      </c>
+      <c r="L37" s="99" t="s">
+        <v>69</v>
+      </c>
+      <c r="M37" s="98" t="s">
+        <v>69</v>
+      </c>
+      <c r="N37" s="100" t="s">
+        <v>69</v>
+      </c>
+      <c r="O37" s="100" t="s">
+        <v>69</v>
+      </c>
+      <c r="P37" s="100" t="s">
+        <v>69</v>
+      </c>
+      <c r="Q37" s="100" t="s">
+        <v>69</v>
+      </c>
       <c r="R37" s="100"/>
       <c r="S37" s="29"/>
     </row>
@@ -3699,28 +3769,42 @@
       <c r="F38" s="24"/>
       <c r="G38" s="96"/>
       <c r="H38" s="8"/>
-      <c r="I38" s="97">
-        <f>IF(M38,'Ш Лист 2'!$A$18,"")</f>
-      </c>
-      <c r="J38" s="98"/>
-      <c r="K38" s="98"/>
-      <c r="L38" s="99"/>
-      <c r="M38" s="98"/>
-      <c r="N38" s="100"/>
-      <c r="O38" s="100"/>
-      <c r="P38" s="100"/>
-      <c r="Q38" s="100">
-        <f t="shared" ref="Q38:Q42" si="0">IF(O38&lt;P38,P38-O38,"")</f>
+      <c r="I38" s="97" t="s">
+        <v>69</v>
+      </c>
+      <c r="J38" s="98" t="s">
+        <v>69</v>
+      </c>
+      <c r="K38" s="98" t="s">
+        <v>69</v>
+      </c>
+      <c r="L38" s="99" t="s">
+        <v>69</v>
+      </c>
+      <c r="M38" s="98" t="s">
+        <v>69</v>
+      </c>
+      <c r="N38" s="100" t="s">
+        <v>69</v>
+      </c>
+      <c r="O38" s="100" t="s">
+        <v>69</v>
+      </c>
+      <c r="P38" s="100" t="s">
+        <v>69</v>
+      </c>
+      <c r="Q38" s="100" t="s">
+        <v>69</v>
       </c>
       <c r="R38" s="100">
-        <f t="shared" ref="R38:R42" si="1">IF(O38&gt;P38,O38-P38,"")</f>
+        <f t="shared" ref="R38:R42" si="0">IF(O38&gt;P38,O38-P38,"")</f>
       </c>
       <c r="S38" s="29"/>
     </row>
     <row r="39" ht="10.7" customHeight="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A39" s="43"/>
       <c r="B39" s="24" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="C39" s="24"/>
       <c r="D39" s="24"/>
@@ -3728,21 +3812,35 @@
       <c r="F39" s="24"/>
       <c r="G39" s="96"/>
       <c r="H39" s="8"/>
-      <c r="I39" s="97">
-        <f>IF(M39,'Ш Лист 2'!$A$18,"")</f>
-      </c>
-      <c r="J39" s="98"/>
-      <c r="K39" s="98"/>
-      <c r="L39" s="99"/>
-      <c r="M39" s="98"/>
-      <c r="N39" s="100"/>
-      <c r="O39" s="100"/>
-      <c r="P39" s="100"/>
-      <c r="Q39" s="100">
+      <c r="I39" s="97" t="s">
+        <v>69</v>
+      </c>
+      <c r="J39" s="98" t="s">
+        <v>69</v>
+      </c>
+      <c r="K39" s="98" t="s">
+        <v>69</v>
+      </c>
+      <c r="L39" s="99" t="s">
+        <v>69</v>
+      </c>
+      <c r="M39" s="98" t="s">
+        <v>69</v>
+      </c>
+      <c r="N39" s="100" t="s">
+        <v>69</v>
+      </c>
+      <c r="O39" s="100" t="s">
+        <v>69</v>
+      </c>
+      <c r="P39" s="100" t="s">
+        <v>69</v>
+      </c>
+      <c r="Q39" s="100" t="s">
+        <v>69</v>
+      </c>
+      <c r="R39" s="100">
         <f t="shared" si="0"/>
-      </c>
-      <c r="R39" s="100">
-        <f t="shared" si="1"/>
       </c>
     </row>
     <row r="40" ht="10.7" customHeight="1" spans="1:19" x14ac:dyDescent="0.25">
@@ -3754,21 +3852,35 @@
       <c r="F40" s="24"/>
       <c r="G40" s="96"/>
       <c r="H40" s="8"/>
-      <c r="I40" s="97">
-        <f>IF(M40,'Ш Лист 2'!$A$18,"")</f>
-      </c>
-      <c r="J40" s="98"/>
-      <c r="K40" s="98"/>
-      <c r="L40" s="99"/>
-      <c r="M40" s="98"/>
-      <c r="N40" s="100"/>
-      <c r="O40" s="100"/>
-      <c r="P40" s="100"/>
-      <c r="Q40" s="100">
+      <c r="I40" s="97" t="s">
+        <v>69</v>
+      </c>
+      <c r="J40" s="98" t="s">
+        <v>69</v>
+      </c>
+      <c r="K40" s="98" t="s">
+        <v>69</v>
+      </c>
+      <c r="L40" s="99" t="s">
+        <v>69</v>
+      </c>
+      <c r="M40" s="98" t="s">
+        <v>69</v>
+      </c>
+      <c r="N40" s="100" t="s">
+        <v>69</v>
+      </c>
+      <c r="O40" s="100" t="s">
+        <v>69</v>
+      </c>
+      <c r="P40" s="100" t="s">
+        <v>69</v>
+      </c>
+      <c r="Q40" s="100" t="s">
+        <v>69</v>
+      </c>
+      <c r="R40" s="100">
         <f t="shared" si="0"/>
-      </c>
-      <c r="R40" s="100">
-        <f t="shared" si="1"/>
       </c>
       <c r="S40" s="29"/>
     </row>
@@ -3781,27 +3893,35 @@
       <c r="F41" s="24"/>
       <c r="G41" s="96"/>
       <c r="H41" s="8"/>
-      <c r="I41" s="97">
-        <f>IF(M41,'Ш Лист 2'!$A$20,"")</f>
-      </c>
-      <c r="J41" s="101"/>
-      <c r="K41" s="101"/>
-      <c r="L41" s="102"/>
-      <c r="M41" s="101"/>
-      <c r="N41" s="100">
-        <f>IFERROR(SUMIFS($M$36:$M$44,$I$36:$I$44,I41)+SUMIFS($K$36:$K$44,$I$36:$I$44,I41)-O41,"")</f>
-      </c>
-      <c r="O41" s="100">
-        <f>'Ш Лист 2'!F20</f>
-      </c>
-      <c r="P41" s="100">
-        <f t="shared" ref="P41" si="2">O41</f>
-      </c>
-      <c r="Q41" s="100">
+      <c r="I41" s="97" t="s">
+        <v>69</v>
+      </c>
+      <c r="J41" s="101" t="s">
+        <v>69</v>
+      </c>
+      <c r="K41" s="101" t="s">
+        <v>69</v>
+      </c>
+      <c r="L41" s="102" t="s">
+        <v>69</v>
+      </c>
+      <c r="M41" s="101" t="s">
+        <v>69</v>
+      </c>
+      <c r="N41" s="100" t="s">
+        <v>69</v>
+      </c>
+      <c r="O41" s="100" t="s">
+        <v>69</v>
+      </c>
+      <c r="P41" s="100" t="s">
+        <v>69</v>
+      </c>
+      <c r="Q41" s="100" t="s">
+        <v>69</v>
+      </c>
+      <c r="R41" s="100">
         <f t="shared" si="0"/>
-      </c>
-      <c r="R41" s="100">
-        <f t="shared" si="1"/>
       </c>
       <c r="S41" s="29"/>
     </row>
@@ -3814,21 +3934,35 @@
       <c r="F42" s="24"/>
       <c r="G42" s="96"/>
       <c r="H42" s="8"/>
-      <c r="I42" s="97">
-        <f>IF(M42,'Ш Лист 2'!$A$20,"")</f>
-      </c>
-      <c r="J42" s="101"/>
-      <c r="K42" s="101"/>
-      <c r="L42" s="102"/>
-      <c r="M42" s="101"/>
-      <c r="N42" s="100"/>
-      <c r="O42" s="100"/>
-      <c r="P42" s="100"/>
-      <c r="Q42" s="100">
+      <c r="I42" s="97" t="s">
+        <v>69</v>
+      </c>
+      <c r="J42" s="101" t="s">
+        <v>69</v>
+      </c>
+      <c r="K42" s="101" t="s">
+        <v>69</v>
+      </c>
+      <c r="L42" s="102" t="s">
+        <v>69</v>
+      </c>
+      <c r="M42" s="101" t="s">
+        <v>69</v>
+      </c>
+      <c r="N42" s="100" t="s">
+        <v>69</v>
+      </c>
+      <c r="O42" s="100" t="s">
+        <v>69</v>
+      </c>
+      <c r="P42" s="100" t="s">
+        <v>69</v>
+      </c>
+      <c r="Q42" s="100" t="s">
+        <v>69</v>
+      </c>
+      <c r="R42" s="100">
         <f t="shared" si="0"/>
-      </c>
-      <c r="R42" s="100">
-        <f t="shared" si="1"/>
       </c>
       <c r="S42" s="29"/>
     </row>
@@ -3841,21 +3975,35 @@
       <c r="F43" s="24"/>
       <c r="G43" s="96"/>
       <c r="H43" s="8"/>
-      <c r="I43" s="97">
-        <f>IF(M43,'Ш Лист 2'!$A$20,"")</f>
-      </c>
-      <c r="J43" s="101"/>
-      <c r="K43" s="101"/>
-      <c r="L43" s="102"/>
-      <c r="M43" s="101"/>
-      <c r="N43" s="100"/>
-      <c r="O43" s="100"/>
-      <c r="P43" s="100"/>
-      <c r="Q43" s="100">
-        <f t="shared" ref="Q43:Q44" si="3">IF(O43&lt;P43,P43-O43,"")</f>
+      <c r="I43" s="97" t="s">
+        <v>69</v>
+      </c>
+      <c r="J43" s="101" t="s">
+        <v>69</v>
+      </c>
+      <c r="K43" s="101" t="s">
+        <v>69</v>
+      </c>
+      <c r="L43" s="102" t="s">
+        <v>69</v>
+      </c>
+      <c r="M43" s="101" t="s">
+        <v>69</v>
+      </c>
+      <c r="N43" s="100" t="s">
+        <v>69</v>
+      </c>
+      <c r="O43" s="100" t="s">
+        <v>69</v>
+      </c>
+      <c r="P43" s="100" t="s">
+        <v>69</v>
+      </c>
+      <c r="Q43" s="100" t="s">
+        <v>69</v>
       </c>
       <c r="R43" s="100">
-        <f t="shared" ref="R43:R44" si="4">IF(O43&gt;P43,O43-P43,"")</f>
+        <f t="shared" ref="R43:R44" si="1">IF(O43&gt;P43,O43-P43,"")</f>
       </c>
       <c r="S43" s="29"/>
     </row>
@@ -3867,21 +4015,35 @@
       <c r="F44" s="24"/>
       <c r="G44" s="96"/>
       <c r="H44" s="8"/>
-      <c r="I44" s="97">
-        <f>IF(M44,'Ш Лист 2'!$A$20,"")</f>
-      </c>
-      <c r="J44" s="101"/>
-      <c r="K44" s="101"/>
-      <c r="L44" s="102"/>
-      <c r="M44" s="101"/>
-      <c r="N44" s="100"/>
-      <c r="O44" s="100"/>
-      <c r="P44" s="100"/>
-      <c r="Q44" s="100">
-        <f t="shared" si="3"/>
+      <c r="I44" s="97" t="s">
+        <v>69</v>
+      </c>
+      <c r="J44" s="101" t="s">
+        <v>69</v>
+      </c>
+      <c r="K44" s="101" t="s">
+        <v>69</v>
+      </c>
+      <c r="L44" s="102" t="s">
+        <v>69</v>
+      </c>
+      <c r="M44" s="101" t="s">
+        <v>69</v>
+      </c>
+      <c r="N44" s="100" t="s">
+        <v>69</v>
+      </c>
+      <c r="O44" s="100" t="s">
+        <v>69</v>
+      </c>
+      <c r="P44" s="100" t="s">
+        <v>69</v>
+      </c>
+      <c r="Q44" s="100" t="s">
+        <v>69</v>
       </c>
       <c r="R44" s="100">
-        <f t="shared" si="4"/>
+        <f t="shared" si="1"/>
       </c>
       <c r="S44" s="29"/>
     </row>
@@ -4053,7 +4215,7 @@
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="103" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="B1" s="103"/>
       <c r="C1" s="103"/>
@@ -4071,30 +4233,30 @@
     </row>
     <row r="2" ht="15.75" customHeight="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="104" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="B2" s="105" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="C2" s="105"/>
       <c r="D2" s="106" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="E2" s="106"/>
       <c r="F2" s="106"/>
       <c r="G2" s="106"/>
       <c r="H2" s="106"/>
       <c r="I2" s="105" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="J2" s="105"/>
       <c r="K2" s="105"/>
       <c r="L2" s="105" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="M2" s="105"/>
       <c r="N2" s="105" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
     </row>
     <row r="3" ht="30.6" customHeight="1" spans="1:14" x14ac:dyDescent="0.25">
@@ -4102,16 +4264,16 @@
       <c r="B3" s="105"/>
       <c r="C3" s="105"/>
       <c r="D3" s="107" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="E3" s="107" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="F3" s="107" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="G3" s="106" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="H3" s="106"/>
       <c r="I3" s="105"/>
@@ -4124,38 +4286,38 @@
     <row r="4" ht="91.35" customHeight="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" s="104"/>
       <c r="B4" s="107" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="C4" s="107" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="D4" s="107"/>
       <c r="E4" s="107"/>
       <c r="F4" s="107"/>
       <c r="G4" s="108" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="H4" s="108" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="I4" s="107" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="J4" s="107" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="K4" s="107" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="L4" s="108" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="M4" s="107" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="N4" s="105"/>
       <c r="O4" s="109" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
     </row>
     <row r="5" ht="15.75" customHeight="1" spans="1:14" x14ac:dyDescent="0.25">
@@ -4204,316 +4366,510 @@
     </row>
     <row r="6" ht="16.7" customHeight="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" s="111" t="s">
-        <v>118</v>
-      </c>
-      <c r="B6" s="112">
-        <f>IF('Ш Лист 1'!T12,TEXT('Ш Лист 1'!U12,"ч:мм")&amp;CHAR(10)&amp;TEXT('Ш Лист 1'!T12,"дд.мм.гг"),"")</f>
-      </c>
-      <c r="C6" s="112">
-        <f>IF('Ш Лист 1'!T12,TEXT('Ш Лист 1'!W12,"ч:мм")&amp;CHAR(10)&amp;TEXT('Ш Лист 1'!V12,"дд.мм.гг"),"")</f>
-      </c>
-      <c r="D6" s="113"/>
-      <c r="E6" s="113"/>
+        <v>120</v>
+      </c>
+      <c r="B6" s="112" t="s">
+        <v>121</v>
+      </c>
+      <c r="C6" s="112" t="s">
+        <v>122</v>
+      </c>
+      <c r="D6" s="113">
+        <v>10</v>
+      </c>
+      <c r="E6" s="113">
+        <v>10</v>
+      </c>
       <c r="F6" s="114">
-        <f>IFERROR('Ш Лист 1'!R12-'Ш Лист 1'!P12,0)</f>
-        <v>1</v>
-      </c>
-      <c r="G6" s="113"/>
-      <c r="H6" s="113"/>
-      <c r="I6" s="113"/>
-      <c r="J6" s="113"/>
-      <c r="K6" s="113"/>
-      <c r="L6" s="113"/>
-      <c r="M6" s="113"/>
+        <v>20</v>
+      </c>
+      <c r="G6" s="113" t="s">
+        <v>69</v>
+      </c>
+      <c r="H6" s="113" t="s">
+        <v>69</v>
+      </c>
+      <c r="I6" s="113">
+        <v>10</v>
+      </c>
+      <c r="J6" s="113">
+        <v>50</v>
+      </c>
+      <c r="K6" s="113">
+        <v>60</v>
+      </c>
+      <c r="L6" s="113" t="s">
+        <v>123</v>
+      </c>
+      <c r="M6" s="113">
+        <v>15</v>
+      </c>
       <c r="N6" s="115">
-        <f>IF('Ш Лист 1'!R12,'Ш Лист 1'!R12,"")</f>
-        <v>12338</v>
-      </c>
-      <c r="P6" s="116">
+        <v>12354</v>
+      </c>
+      <c r="O6" s="116" t="s">
+        <v>69</v>
+      </c>
+      <c r="P6" s="117">
         <v>1</v>
       </c>
     </row>
     <row r="7" ht="16.7" customHeight="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" s="111" t="s">
-        <v>119</v>
-      </c>
-      <c r="B7" s="112">
-        <f>IF('Ш Лист 1'!T14,TEXT('Ш Лист 1'!U14,"ч:мм")&amp;CHAR(10)&amp;TEXT('Ш Лист 1'!T14,"дд.мм.гг"),"")</f>
-      </c>
-      <c r="C7" s="112">
-        <f>IF('Ш Лист 1'!T14,TEXT('Ш Лист 1'!W14,"ч:мм")&amp;CHAR(10)&amp;TEXT('Ш Лист 1'!V14,"дд.мм.гг"),"")</f>
-      </c>
-      <c r="D7" s="113"/>
-      <c r="E7" s="113"/>
+        <v>124</v>
+      </c>
+      <c r="B7" s="112" t="s">
+        <v>125</v>
+      </c>
+      <c r="C7" s="112" t="s">
+        <v>126</v>
+      </c>
+      <c r="D7" s="113">
+        <v>10</v>
+      </c>
+      <c r="E7" s="113">
+        <v>10</v>
+      </c>
       <c r="F7" s="114">
-        <f>IFERROR('Ш Лист 1'!R14-'Ш Лист 1'!P14,0)</f>
-        <v>1</v>
-      </c>
-      <c r="G7" s="113"/>
-      <c r="H7" s="113"/>
-      <c r="I7" s="113"/>
-      <c r="J7" s="113"/>
-      <c r="K7" s="113"/>
-      <c r="L7" s="113"/>
-      <c r="M7" s="113"/>
+        <v>20</v>
+      </c>
+      <c r="G7" s="113" t="s">
+        <v>69</v>
+      </c>
+      <c r="H7" s="113" t="s">
+        <v>69</v>
+      </c>
+      <c r="I7" s="113">
+        <v>10</v>
+      </c>
+      <c r="J7" s="113">
+        <v>50</v>
+      </c>
+      <c r="K7" s="113">
+        <v>60</v>
+      </c>
+      <c r="L7" s="113" t="s">
+        <v>123</v>
+      </c>
+      <c r="M7" s="113">
+        <v>15</v>
+      </c>
       <c r="N7" s="115">
-        <f>IF('Ш Лист 1'!R14,'Ш Лист 1'!R14,"")</f>
-        <v>12340</v>
-      </c>
-      <c r="P7" s="116">
+        <v>12454</v>
+      </c>
+      <c r="O7" s="116" t="s">
+        <v>69</v>
+      </c>
+      <c r="P7" s="117">
         <v>2</v>
       </c>
     </row>
     <row r="8" ht="16.7" customHeight="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" s="111" t="s">
-        <v>119</v>
-      </c>
-      <c r="B8" s="112">
-        <f>IF('Ш Лист 1'!T16,TEXT('Ш Лист 1'!U16,"ч:мм")&amp;CHAR(10)&amp;TEXT('Ш Лист 1'!T16,"дд.мм.гг"),"")</f>
-      </c>
-      <c r="C8" s="112">
-        <f>IF('Ш Лист 1'!T16,TEXT('Ш Лист 1'!W16,"ч:мм")&amp;CHAR(10)&amp;TEXT('Ш Лист 1'!V16,"дд.мм.гг"),"")</f>
-      </c>
-      <c r="D8" s="113"/>
-      <c r="E8" s="113"/>
-      <c r="F8" s="114">
-        <f>IFERROR('Ш Лист 1'!R16-'Ш Лист 1'!P16,0)</f>
-        <v>5</v>
-      </c>
-      <c r="G8" s="113"/>
-      <c r="H8" s="113"/>
-      <c r="I8" s="113"/>
-      <c r="J8" s="113"/>
-      <c r="K8" s="113"/>
-      <c r="L8" s="113"/>
-      <c r="M8" s="113"/>
-      <c r="N8" s="115">
-        <f>IF('Ш Лист 1'!R16,'Ш Лист 1'!R16,"")</f>
-        <v>12345</v>
-      </c>
-      <c r="P8" s="116">
+        <v>69</v>
+      </c>
+      <c r="B8" s="112" t="s">
+        <v>69</v>
+      </c>
+      <c r="C8" s="112" t="s">
+        <v>69</v>
+      </c>
+      <c r="D8" s="113" t="s">
+        <v>69</v>
+      </c>
+      <c r="E8" s="113" t="s">
+        <v>69</v>
+      </c>
+      <c r="F8" s="114" t="s">
+        <v>69</v>
+      </c>
+      <c r="G8" s="113" t="s">
+        <v>69</v>
+      </c>
+      <c r="H8" s="113" t="s">
+        <v>69</v>
+      </c>
+      <c r="I8" s="113" t="s">
+        <v>69</v>
+      </c>
+      <c r="J8" s="113" t="s">
+        <v>69</v>
+      </c>
+      <c r="K8" s="113" t="s">
+        <v>69</v>
+      </c>
+      <c r="L8" s="113" t="s">
+        <v>69</v>
+      </c>
+      <c r="M8" s="113" t="s">
+        <v>69</v>
+      </c>
+      <c r="N8" s="115" t="s">
+        <v>69</v>
+      </c>
+      <c r="O8" s="116" t="s">
+        <v>69</v>
+      </c>
+      <c r="P8" s="117">
         <v>3</v>
       </c>
     </row>
     <row r="9" ht="16.7" customHeight="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" s="111" t="s">
-        <v>119</v>
-      </c>
-      <c r="B9" s="112">
-        <f>IF('Ш Лист 1'!T18,TEXT('Ш Лист 1'!U18,"ч:мм")&amp;CHAR(10)&amp;TEXT('Ш Лист 1'!T18,"дд.мм.гг"),"")</f>
-      </c>
-      <c r="C9" s="112">
-        <f>IF('Ш Лист 1'!T18,TEXT('Ш Лист 1'!W18,"ч:мм")&amp;CHAR(10)&amp;TEXT('Ш Лист 1'!V18,"дд.мм.гг"),"")</f>
-      </c>
-      <c r="D9" s="113"/>
-      <c r="E9" s="113"/>
-      <c r="F9" s="114">
-        <f>IFERROR('Ш Лист 1'!R18-'Ш Лист 1'!P18,0)</f>
-        <v>4</v>
-      </c>
-      <c r="G9" s="113"/>
-      <c r="H9" s="113"/>
-      <c r="I9" s="113"/>
-      <c r="J9" s="113"/>
-      <c r="K9" s="113"/>
-      <c r="L9" s="113"/>
-      <c r="M9" s="113"/>
-      <c r="N9" s="115">
-        <f>IF('Ш Лист 1'!R18,'Ш Лист 1'!R18,"")</f>
-        <v>12349</v>
-      </c>
-      <c r="P9" s="116">
+        <v>69</v>
+      </c>
+      <c r="B9" s="112" t="s">
+        <v>69</v>
+      </c>
+      <c r="C9" s="112" t="s">
+        <v>69</v>
+      </c>
+      <c r="D9" s="113" t="s">
+        <v>69</v>
+      </c>
+      <c r="E9" s="113" t="s">
+        <v>69</v>
+      </c>
+      <c r="F9" s="114" t="s">
+        <v>69</v>
+      </c>
+      <c r="G9" s="113" t="s">
+        <v>69</v>
+      </c>
+      <c r="H9" s="113" t="s">
+        <v>69</v>
+      </c>
+      <c r="I9" s="113" t="s">
+        <v>69</v>
+      </c>
+      <c r="J9" s="113" t="s">
+        <v>69</v>
+      </c>
+      <c r="K9" s="113" t="s">
+        <v>69</v>
+      </c>
+      <c r="L9" s="113" t="s">
+        <v>69</v>
+      </c>
+      <c r="M9" s="113" t="s">
+        <v>69</v>
+      </c>
+      <c r="N9" s="115" t="s">
+        <v>69</v>
+      </c>
+      <c r="O9" s="116" t="s">
+        <v>69</v>
+      </c>
+      <c r="P9" s="117">
         <v>4</v>
       </c>
     </row>
     <row r="10" ht="16.7" customHeight="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" s="111" t="s">
-        <v>118</v>
-      </c>
-      <c r="B10" s="112">
-        <f>IF('Ш Лист 1'!T20,TEXT('Ш Лист 1'!U20,"ч:мм")&amp;CHAR(10)&amp;TEXT('Ш Лист 1'!T20,"дд.мм.гг"),"")</f>
-      </c>
-      <c r="C10" s="112">
-        <f>IF('Ш Лист 1'!T20,TEXT('Ш Лист 1'!W20,"ч:мм")&amp;CHAR(10)&amp;TEXT('Ш Лист 1'!V20,"дд.мм.гг"),"")</f>
-      </c>
-      <c r="D10" s="113"/>
-      <c r="E10" s="113"/>
-      <c r="F10" s="114">
-        <f>IFERROR('Ш Лист 1'!R20-'Ш Лист 1'!P20,0)</f>
-        <v>4</v>
-      </c>
-      <c r="G10" s="113"/>
-      <c r="H10" s="113"/>
-      <c r="I10" s="113"/>
-      <c r="J10" s="113"/>
-      <c r="K10" s="113"/>
-      <c r="L10" s="113"/>
-      <c r="M10" s="113"/>
-      <c r="N10" s="115">
-        <f>IF('Ш Лист 1'!R20,'Ш Лист 1'!R20,"")</f>
-        <v>12353</v>
-      </c>
-      <c r="P10" s="116">
+        <v>69</v>
+      </c>
+      <c r="B10" s="112" t="s">
+        <v>69</v>
+      </c>
+      <c r="C10" s="112" t="s">
+        <v>69</v>
+      </c>
+      <c r="D10" s="113" t="s">
+        <v>69</v>
+      </c>
+      <c r="E10" s="113" t="s">
+        <v>69</v>
+      </c>
+      <c r="F10" s="114" t="s">
+        <v>69</v>
+      </c>
+      <c r="G10" s="113" t="s">
+        <v>69</v>
+      </c>
+      <c r="H10" s="113" t="s">
+        <v>69</v>
+      </c>
+      <c r="I10" s="113" t="s">
+        <v>69</v>
+      </c>
+      <c r="J10" s="113" t="s">
+        <v>69</v>
+      </c>
+      <c r="K10" s="113" t="s">
+        <v>69</v>
+      </c>
+      <c r="L10" s="113" t="s">
+        <v>69</v>
+      </c>
+      <c r="M10" s="113" t="s">
+        <v>69</v>
+      </c>
+      <c r="N10" s="115" t="s">
+        <v>69</v>
+      </c>
+      <c r="O10" s="116" t="s">
+        <v>69</v>
+      </c>
+      <c r="P10" s="117">
         <v>5</v>
       </c>
     </row>
     <row r="11" ht="16.7" customHeight="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" s="111" t="s">
-        <v>118</v>
-      </c>
-      <c r="B11" s="112">
-        <f>IF('Ш Лист 1'!T22,TEXT('Ш Лист 1'!U22,"ч:мм")&amp;CHAR(10)&amp;TEXT('Ш Лист 1'!T22,"дд.мм.гг"),"")</f>
-      </c>
-      <c r="C11" s="112">
-        <f>IF('Ш Лист 1'!T22,TEXT('Ш Лист 1'!W22,"ч:мм")&amp;CHAR(10)&amp;TEXT('Ш Лист 1'!V22,"дд.мм.гг"),"")</f>
-      </c>
-      <c r="D11" s="113"/>
-      <c r="E11" s="113"/>
-      <c r="F11" s="114">
-        <f>IFERROR('Ш Лист 1'!R22-'Ш Лист 1'!P22,0)</f>
-        <v>0</v>
-      </c>
-      <c r="G11" s="113"/>
-      <c r="H11" s="113"/>
-      <c r="I11" s="113"/>
-      <c r="J11" s="113"/>
-      <c r="K11" s="113"/>
-      <c r="L11" s="113"/>
-      <c r="M11" s="113"/>
-      <c r="N11" s="115" t="e">
-        <f>IF('Ш Лист 1'!R22,'Ш Лист 1'!R22,"")</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="P11" s="116">
+        <v>69</v>
+      </c>
+      <c r="B11" s="112" t="s">
+        <v>69</v>
+      </c>
+      <c r="C11" s="112" t="s">
+        <v>69</v>
+      </c>
+      <c r="D11" s="113" t="s">
+        <v>69</v>
+      </c>
+      <c r="E11" s="113" t="s">
+        <v>69</v>
+      </c>
+      <c r="F11" s="114" t="s">
+        <v>69</v>
+      </c>
+      <c r="G11" s="113" t="s">
+        <v>69</v>
+      </c>
+      <c r="H11" s="113" t="s">
+        <v>69</v>
+      </c>
+      <c r="I11" s="113" t="s">
+        <v>69</v>
+      </c>
+      <c r="J11" s="113" t="s">
+        <v>69</v>
+      </c>
+      <c r="K11" s="113" t="s">
+        <v>69</v>
+      </c>
+      <c r="L11" s="113" t="s">
+        <v>69</v>
+      </c>
+      <c r="M11" s="113" t="s">
+        <v>69</v>
+      </c>
+      <c r="N11" s="115" t="s">
+        <v>69</v>
+      </c>
+      <c r="O11" s="116" t="s">
+        <v>69</v>
+      </c>
+      <c r="P11" s="117">
         <v>6</v>
       </c>
     </row>
     <row r="12" ht="16.7" customHeight="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" s="111" t="s">
-        <v>118</v>
-      </c>
-      <c r="B12" s="112">
-        <f>IF('Ш Лист 1'!T24,TEXT('Ш Лист 1'!U24,"ч:мм")&amp;CHAR(10)&amp;TEXT('Ш Лист 1'!T24,"дд.мм.гг"),"")</f>
-      </c>
-      <c r="C12" s="112">
-        <f>IF('Ш Лист 1'!T24,TEXT('Ш Лист 1'!W24,"ч:мм")&amp;CHAR(10)&amp;TEXT('Ш Лист 1'!V24,"дд.мм.гг"),"")</f>
-      </c>
-      <c r="D12" s="113"/>
-      <c r="E12" s="113"/>
-      <c r="F12" s="114">
-        <f>IFERROR('Ш Лист 1'!R24-'Ш Лист 1'!P24,0)</f>
-        <v>0</v>
-      </c>
-      <c r="G12" s="113"/>
-      <c r="H12" s="113"/>
-      <c r="I12" s="113"/>
-      <c r="J12" s="113"/>
-      <c r="K12" s="113"/>
-      <c r="L12" s="113"/>
-      <c r="M12" s="113"/>
-      <c r="N12" s="115" t="e">
-        <f>IF('Ш Лист 1'!R24,'Ш Лист 1'!R24,"")</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="P12" s="116">
+        <v>69</v>
+      </c>
+      <c r="B12" s="112" t="s">
+        <v>69</v>
+      </c>
+      <c r="C12" s="112" t="s">
+        <v>69</v>
+      </c>
+      <c r="D12" s="113" t="s">
+        <v>69</v>
+      </c>
+      <c r="E12" s="113" t="s">
+        <v>69</v>
+      </c>
+      <c r="F12" s="114" t="s">
+        <v>69</v>
+      </c>
+      <c r="G12" s="113" t="s">
+        <v>69</v>
+      </c>
+      <c r="H12" s="113" t="s">
+        <v>69</v>
+      </c>
+      <c r="I12" s="113" t="s">
+        <v>69</v>
+      </c>
+      <c r="J12" s="113" t="s">
+        <v>69</v>
+      </c>
+      <c r="K12" s="113" t="s">
+        <v>69</v>
+      </c>
+      <c r="L12" s="113" t="s">
+        <v>69</v>
+      </c>
+      <c r="M12" s="113" t="s">
+        <v>69</v>
+      </c>
+      <c r="N12" s="115" t="s">
+        <v>69</v>
+      </c>
+      <c r="O12" s="116" t="s">
+        <v>69</v>
+      </c>
+      <c r="P12" s="117">
         <v>7</v>
       </c>
     </row>
     <row r="13" ht="16.7" customHeight="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13" s="111" t="s">
-        <v>118</v>
-      </c>
-      <c r="B13" s="112">
-        <f>IF('Ш Лист 1'!T26,TEXT('Ш Лист 1'!U26,"ч:мм")&amp;CHAR(10)&amp;TEXT('Ш Лист 1'!T26,"дд.мм.гг"),"")</f>
-      </c>
-      <c r="C13" s="112">
-        <f>IF('Ш Лист 1'!T26,TEXT('Ш Лист 1'!W26,"ч:мм")&amp;CHAR(10)&amp;TEXT('Ш Лист 1'!V26,"дд.мм.гг"),"")</f>
-      </c>
-      <c r="D13" s="113"/>
-      <c r="E13" s="113"/>
-      <c r="F13" s="114">
-        <f>IFERROR('Ш Лист 1'!R26-'Ш Лист 1'!P26,0)</f>
-        <v>0</v>
-      </c>
-      <c r="G13" s="113"/>
-      <c r="H13" s="113"/>
-      <c r="I13" s="113"/>
-      <c r="J13" s="113"/>
-      <c r="K13" s="113"/>
-      <c r="L13" s="113"/>
-      <c r="M13" s="113"/>
-      <c r="N13" s="115" t="e">
-        <f>IF('Ш Лист 1'!R26,'Ш Лист 1'!R26,"")</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="P13" s="116">
+        <v>69</v>
+      </c>
+      <c r="B13" s="112" t="s">
+        <v>69</v>
+      </c>
+      <c r="C13" s="112" t="s">
+        <v>69</v>
+      </c>
+      <c r="D13" s="113" t="s">
+        <v>69</v>
+      </c>
+      <c r="E13" s="113" t="s">
+        <v>69</v>
+      </c>
+      <c r="F13" s="114" t="s">
+        <v>69</v>
+      </c>
+      <c r="G13" s="113" t="s">
+        <v>69</v>
+      </c>
+      <c r="H13" s="113" t="s">
+        <v>69</v>
+      </c>
+      <c r="I13" s="113" t="s">
+        <v>69</v>
+      </c>
+      <c r="J13" s="113" t="s">
+        <v>69</v>
+      </c>
+      <c r="K13" s="113" t="s">
+        <v>69</v>
+      </c>
+      <c r="L13" s="113" t="s">
+        <v>69</v>
+      </c>
+      <c r="M13" s="113" t="s">
+        <v>69</v>
+      </c>
+      <c r="N13" s="115" t="s">
+        <v>69</v>
+      </c>
+      <c r="O13" s="116" t="s">
+        <v>69</v>
+      </c>
+      <c r="P13" s="117">
         <v>8</v>
       </c>
     </row>
     <row r="14" ht="16.7" customHeight="1" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A14" s="111"/>
-      <c r="B14" s="112">
-        <f>IF('Ш Лист 1'!T28,TEXT('Ш Лист 1'!U28,"ч:мм")&amp;CHAR(10)&amp;TEXT('Ш Лист 1'!T28,"дд.мм.гг"),"")</f>
-      </c>
-      <c r="C14" s="112">
-        <f>IF('Ш Лист 1'!T28,TEXT('Ш Лист 1'!W28,"ч:мм")&amp;CHAR(10)&amp;TEXT('Ш Лист 1'!V28,"дд.мм.гг"),"")</f>
-      </c>
-      <c r="D14" s="113"/>
-      <c r="E14" s="113"/>
-      <c r="F14" s="114">
-        <f>IFERROR('Ш Лист 1'!R28-'Ш Лист 1'!P28,0)</f>
-        <v>0</v>
-      </c>
-      <c r="G14" s="113"/>
-      <c r="H14" s="113"/>
-      <c r="I14" s="113"/>
-      <c r="J14" s="113"/>
-      <c r="K14" s="113"/>
-      <c r="L14" s="113"/>
-      <c r="M14" s="113"/>
-      <c r="N14" s="115" t="e">
-        <f>IF('Ш Лист 1'!R28,'Ш Лист 1'!R28,"")</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="P14" s="116">
+      <c r="A14" s="111" t="s">
+        <v>69</v>
+      </c>
+      <c r="B14" s="112" t="s">
+        <v>69</v>
+      </c>
+      <c r="C14" s="112" t="s">
+        <v>69</v>
+      </c>
+      <c r="D14" s="113" t="s">
+        <v>69</v>
+      </c>
+      <c r="E14" s="113" t="s">
+        <v>69</v>
+      </c>
+      <c r="F14" s="114" t="s">
+        <v>69</v>
+      </c>
+      <c r="G14" s="113" t="s">
+        <v>69</v>
+      </c>
+      <c r="H14" s="113" t="s">
+        <v>69</v>
+      </c>
+      <c r="I14" s="113" t="s">
+        <v>69</v>
+      </c>
+      <c r="J14" s="113" t="s">
+        <v>69</v>
+      </c>
+      <c r="K14" s="113" t="s">
+        <v>69</v>
+      </c>
+      <c r="L14" s="113" t="s">
+        <v>69</v>
+      </c>
+      <c r="M14" s="113" t="s">
+        <v>69</v>
+      </c>
+      <c r="N14" s="115" t="s">
+        <v>69</v>
+      </c>
+      <c r="O14" s="116" t="s">
+        <v>69</v>
+      </c>
+      <c r="P14" s="117">
         <v>9</v>
       </c>
     </row>
     <row r="15" ht="16.7" customHeight="1" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A15" s="111"/>
-      <c r="B15" s="112">
-        <f>IF('Ш Лист 1'!T30,TEXT('Ш Лист 1'!U30,"ч:мм")&amp;CHAR(10)&amp;TEXT('Ш Лист 1'!T30,"дд.мм.гг"),"")</f>
-      </c>
-      <c r="C15" s="112">
-        <f>IF('Ш Лист 1'!T30,TEXT('Ш Лист 1'!W30,"ч:мм")&amp;CHAR(10)&amp;TEXT('Ш Лист 1'!V30,"дд.мм.гг"),"")</f>
-      </c>
-      <c r="D15" s="113"/>
-      <c r="E15" s="113"/>
-      <c r="F15" s="114">
-        <f>IFERROR('Ш Лист 1'!R30-'Ш Лист 1'!P30,0)</f>
-        <v>0</v>
-      </c>
-      <c r="G15" s="113"/>
-      <c r="H15" s="113"/>
-      <c r="I15" s="113"/>
-      <c r="J15" s="113"/>
-      <c r="K15" s="113"/>
-      <c r="L15" s="113"/>
-      <c r="M15" s="113"/>
-      <c r="N15" s="115" t="e">
-        <f>IF('Ш Лист 1'!R30,'Ш Лист 1'!R30,"")</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="P15" s="116">
+      <c r="A15" s="111" t="s">
+        <v>69</v>
+      </c>
+      <c r="B15" s="112" t="s">
+        <v>69</v>
+      </c>
+      <c r="C15" s="112" t="s">
+        <v>69</v>
+      </c>
+      <c r="D15" s="113" t="s">
+        <v>69</v>
+      </c>
+      <c r="E15" s="113" t="s">
+        <v>69</v>
+      </c>
+      <c r="F15" s="114" t="s">
+        <v>69</v>
+      </c>
+      <c r="G15" s="113" t="s">
+        <v>69</v>
+      </c>
+      <c r="H15" s="113" t="s">
+        <v>69</v>
+      </c>
+      <c r="I15" s="113" t="s">
+        <v>69</v>
+      </c>
+      <c r="J15" s="113" t="s">
+        <v>69</v>
+      </c>
+      <c r="K15" s="113" t="s">
+        <v>69</v>
+      </c>
+      <c r="L15" s="113" t="s">
+        <v>69</v>
+      </c>
+      <c r="M15" s="113" t="s">
+        <v>69</v>
+      </c>
+      <c r="N15" s="115" t="s">
+        <v>69</v>
+      </c>
+      <c r="O15" s="116" t="s">
+        <v>69</v>
+      </c>
+      <c r="P15" s="117">
         <v>10</v>
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" s="55" t="s">
-        <v>120</v>
-      </c>
-      <c r="B16" s="117"/>
-      <c r="C16" s="117"/>
+        <v>127</v>
+      </c>
+      <c r="B16" s="118"/>
+      <c r="C16" s="118"/>
       <c r="D16" s="114">
         <f t="shared" ref="D16:E16" si="0">SUM(D6:D15)</f>
         <v>0</v>
@@ -4554,45 +4910,40 @@
         <f t="shared" ref="M16" si="5">SUM(M6:M15)</f>
         <v>0</v>
       </c>
-      <c r="N16" s="117"/>
+      <c r="N16" s="118"/>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" s="29" t="s">
-        <v>121</v>
+        <v>128</v>
       </c>
     </row>
     <row r="18" ht="12" customHeight="1" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A18" s="76" t="e">
-        <f>INDEX(#REF!,MATCH('Ш Лист 1'!L33,#REF!,0))</f>
-        <v>#REF!</v>
-      </c>
-      <c r="B18" s="118" t="e">
-        <f>INDEX(#REF!,MATCH('Ш Лист 1'!L33,#REF!,0))</f>
-        <v>#REF!</v>
-      </c>
-      <c r="C18" s="119" t="s">
-        <v>122</v>
-      </c>
-      <c r="D18" s="120">
-        <f>F16</f>
-        <v>15</v>
+      <c r="A18" s="76" t="s">
+        <v>129</v>
+      </c>
+      <c r="B18" s="119">
+        <v>11.5</v>
+      </c>
+      <c r="C18" s="120" t="s">
+        <v>130</v>
+      </c>
+      <c r="D18" s="121">
+        <v>1557</v>
       </c>
       <c r="E18" s="76" t="s">
-        <v>123</v>
-      </c>
-      <c r="F18" s="121">
-        <f>A15</f>
-        <v>0</v>
+        <v>131</v>
+      </c>
+      <c r="F18" s="122" t="s">
+        <v>132</v>
       </c>
       <c r="G18" s="76" t="s">
-        <v>124</v>
-      </c>
-      <c r="H18" s="122" t="e">
-        <f>ROUND(B18*D18/C19-B18*D18/C19*F18,0)</f>
-        <v>#REF!</v>
-      </c>
-      <c r="I18" s="123" t="s">
-        <v>125</v>
+        <v>133</v>
+      </c>
+      <c r="H18" s="123">
+        <v>152</v>
+      </c>
+      <c r="I18" s="124" t="s">
+        <v>134</v>
       </c>
       <c r="J18" s="1"/>
       <c r="K18" s="1"/>
@@ -4608,10 +4959,10 @@
       </c>
       <c r="D19" s="1"/>
       <c r="E19" s="76"/>
-      <c r="F19" s="121"/>
+      <c r="F19" s="122"/>
       <c r="G19" s="76"/>
-      <c r="H19" s="122"/>
-      <c r="I19" s="123"/>
+      <c r="H19" s="123"/>
+      <c r="I19" s="124"/>
       <c r="J19" s="1"/>
       <c r="K19" s="1"/>
       <c r="L19" s="1"/>
@@ -4622,13 +4973,13 @@
       <c r="A20" s="76">
         <f>IF(HideOil,"",INDEX(#REF!,MATCH('Ш Лист 1'!L33,#REF!,0)))</f>
       </c>
-      <c r="B20" s="118">
+      <c r="B20" s="119">
         <f>IF(HideOil,"",INDEX(#REF!,MATCH('Ш Лист 1'!L33,#REF!,0)))</f>
       </c>
-      <c r="C20" s="119">
+      <c r="C20" s="120">
         <f>IF(HideOil,"","x")</f>
       </c>
-      <c r="D20" s="120">
+      <c r="D20" s="121">
         <f>IF(HideOil,"",H18)</f>
       </c>
       <c r="E20" s="76">
@@ -4637,7 +4988,7 @@
       <c r="F20" s="76">
         <f>IF(HideOil,"",ROUND(B20*D20/C21,1))</f>
       </c>
-      <c r="G20" s="123">
+      <c r="G20" s="124">
         <f>IF(HideOil,"","л")</f>
       </c>
       <c r="H20" s="1"/>
@@ -4660,7 +5011,7 @@
       <c r="D21" s="1"/>
       <c r="E21" s="76"/>
       <c r="F21" s="76"/>
-      <c r="G21" s="123"/>
+      <c r="G21" s="124"/>
       <c r="H21" s="1"/>
       <c r="I21" s="1"/>
       <c r="J21" s="1"/>
@@ -4671,85 +5022,87 @@
     </row>
     <row r="22" ht="15.75" customHeight="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="19" t="s">
-        <v>126</v>
-      </c>
-      <c r="B22" s="124">
+        <v>135</v>
+      </c>
+      <c r="B22" s="125">
         <f>F16</f>
         <v>15</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>127</v>
+        <v>136</v>
       </c>
     </row>
     <row r="23" ht="15.75" customHeight="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="19" t="s">
-        <v>128</v>
-      </c>
-      <c r="B23" s="124" t="e">
+        <v>137</v>
+      </c>
+      <c r="B23" s="125" t="e">
         <f>H18</f>
         <v>#REF!</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>125</v>
+        <v>134</v>
       </c>
     </row>
     <row r="24" ht="15.75" customHeight="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24" s="19" t="s">
-        <v>129</v>
-      </c>
-      <c r="D24" s="125" t="str">
-        <f>'Ш Лист 1'!J5</f>
-        <v>солдат</v>
-      </c>
-      <c r="E24" s="126"/>
-      <c r="F24" s="126"/>
-      <c r="G24" s="126"/>
-      <c r="H24" s="126"/>
-      <c r="I24" s="126"/>
-      <c r="J24" s="126"/>
-      <c r="K24" s="126"/>
-      <c r="M24" s="125" t="str">
+        <v>138</v>
+      </c>
+      <c r="D24" s="126" t="s">
+        <v>11</v>
+      </c>
+      <c r="E24" s="127"/>
+      <c r="F24" s="127"/>
+      <c r="G24" s="127"/>
+      <c r="H24" s="127"/>
+      <c r="I24" s="127"/>
+      <c r="J24" s="127"/>
+      <c r="K24" s="127"/>
+      <c r="L24" t="s">
+        <v>12</v>
+      </c>
+      <c r="M24" s="126" t="str">
         <f>'Ш Лист 1'!L5</f>
         <v>Петренко В.В.</v>
       </c>
     </row>
     <row r="25" ht="12" customHeight="1" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B25" s="127" t="s">
-        <v>130</v>
-      </c>
-      <c r="C25" s="127"/>
-      <c r="D25" s="127"/>
-      <c r="E25" s="127"/>
-      <c r="F25" s="127"/>
-      <c r="G25" s="127"/>
-      <c r="H25" s="127"/>
-      <c r="I25" s="127"/>
-      <c r="J25" s="127"/>
-      <c r="K25" s="127"/>
-      <c r="L25" s="127"/>
-      <c r="M25" s="127"/>
-      <c r="N25" s="127"/>
+      <c r="B25" s="128" t="s">
+        <v>139</v>
+      </c>
+      <c r="C25" s="128"/>
+      <c r="D25" s="128"/>
+      <c r="E25" s="128"/>
+      <c r="F25" s="128"/>
+      <c r="G25" s="128"/>
+      <c r="H25" s="128"/>
+      <c r="I25" s="128"/>
+      <c r="J25" s="128"/>
+      <c r="K25" s="128"/>
+      <c r="L25" s="128"/>
+      <c r="M25" s="128"/>
+      <c r="N25" s="128"/>
     </row>
     <row r="26" ht="15.75" customHeight="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A26" s="30" t="s">
-        <v>131</v>
-      </c>
-      <c r="G26" s="118">
+        <v>140</v>
+      </c>
+      <c r="G26" s="119">
         <f>IFERROR(INDEX(#REF!,MATCH(N26,#REF!,0)),"")</f>
       </c>
-      <c r="H26" s="126"/>
-      <c r="I26" s="126"/>
-      <c r="J26" s="126"/>
-      <c r="K26" s="126"/>
-      <c r="L26" s="126"/>
-      <c r="M26" s="126"/>
-      <c r="N26" s="128" t="s">
-        <v>132</v>
+      <c r="H26" s="127"/>
+      <c r="I26" s="127"/>
+      <c r="J26" s="127"/>
+      <c r="K26" s="127"/>
+      <c r="L26" s="127"/>
+      <c r="M26" s="127"/>
+      <c r="N26" s="129" t="s">
+        <v>141</v>
       </c>
     </row>
     <row r="27" ht="16.35" customHeight="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>133</v>
+        <v>142</v>
       </c>
       <c r="B27" s="1">
         <v>2023</v>
@@ -4757,16 +5110,16 @@
       <c r="C27" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="G27" s="129" t="s">
-        <v>134</v>
-      </c>
-      <c r="H27" s="129"/>
-      <c r="I27" s="129"/>
-      <c r="J27" s="129"/>
-      <c r="K27" s="129"/>
-      <c r="L27" s="129"/>
-      <c r="M27" s="129"/>
-      <c r="N27" s="129"/>
+      <c r="G27" s="130" t="s">
+        <v>143</v>
+      </c>
+      <c r="H27" s="130"/>
+      <c r="I27" s="130"/>
+      <c r="J27" s="130"/>
+      <c r="K27" s="130"/>
+      <c r="L27" s="130"/>
+      <c r="M27" s="130"/>
+      <c r="N27" s="130"/>
     </row>
   </sheetData>
   <mergeCells count="23">

</xml_diff>

<commit_message>
Redux and carInfo edit
</commit_message>
<xml_diff>
--- a/src/backend/fileStorage/excel/roadXS.xlsx
+++ b/src/backend/fileStorage/excel/roadXS.xlsx
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="408" uniqueCount="208">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="492" uniqueCount="216">
   <si>
     <t>року</t>
   </si>
@@ -70,7 +70,7 @@
     <t>Дійсний до</t>
   </si>
   <si>
-    <t>15.10.2023</t>
+    <t>17.10.2024</t>
   </si>
   <si>
     <t>Збройних Силах України (пункт 4 розділу ХVІІІ)</t>
@@ -169,6 +169,12 @@
     <t>За нарядом</t>
   </si>
   <si>
+    <t>7:30 29.09.2023</t>
+  </si>
+  <si>
+    <t>18:10 29.09.2023</t>
+  </si>
+  <si>
     <t>EndSpeedometer4</t>
   </si>
   <si>
@@ -295,6 +301,9 @@
     <t>маса вантажу, т</t>
   </si>
   <si>
+    <t>15.10.2024</t>
+  </si>
+  <si>
     <t>Наряд № 25</t>
   </si>
   <si>
@@ -304,6 +313,9 @@
     <t>AA1234FF</t>
   </si>
   <si>
+    <t>Транспорт</t>
+  </si>
+  <si>
     <t>1. Витрата пально-мастильних матеріалів (у літрах)</t>
   </si>
   <si>
@@ -347,9 +359,6 @@
   </si>
   <si>
     <t>Масло</t>
-  </si>
-  <si>
-    <t>24</t>
   </si>
   <si>
     <t>Марка машини</t>
@@ -416,16 +425,31 @@
     <t>Корінець дорожнього листа</t>
   </si>
   <si>
+    <t>Київ - Вінниця - Київ</t>
+  </si>
+  <si>
+    <t>7:30, 29.00.23</t>
+  </si>
+  <si>
+    <t>18:10, 29.00.23</t>
+  </si>
+  <si>
+    <t>Пісок</t>
+  </si>
+  <si>
+    <t>Львів - Хмельницький - Львів</t>
+  </si>
+  <si>
     <t>Кременець - Тернопіль</t>
   </si>
   <si>
-    <t>Львів - Хмельницький - Львів</t>
-  </si>
-  <si>
     <t>Всього:</t>
   </si>
   <si>
     <t>Рух по дорозі з покращеним покриттям</t>
+  </si>
+  <si>
+    <t>ДТ</t>
   </si>
   <si>
     <t>x</t>
@@ -480,10 +504,16 @@
     </r>
   </si>
   <si>
-    <t>Фара К.Л.</t>
-  </si>
-  <si>
-    <t>"____"__________________</t>
+    <t>сержант</t>
+  </si>
+  <si>
+    <t>Петрович А.І.</t>
+  </si>
+  <si>
+    <t>"16" Листопада</t>
+  </si>
+  <si>
+    <t>2024</t>
   </si>
   <si>
     <t>(посада, військове звання,  підпис,  прізвище, ініціали)</t>
@@ -561,9 +591,6 @@
     <t>AI8523FE</t>
   </si>
   <si>
-    <t>ДТ</t>
-  </si>
-  <si>
     <t>12</t>
   </si>
   <si>
@@ -580,9 +607,6 @@
   </si>
   <si>
     <t>Чек А.Ф.</t>
-  </si>
-  <si>
-    <t>сержант</t>
   </si>
   <si>
     <t>А0000 (ПВЗ)</t>
@@ -960,6 +984,13 @@
     </border>
     <border>
       <left/>
+      <right/>
+      <top/>
+      <bottom style="thin"/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
       <right style="thin">
         <color indexed="64"/>
       </right>
@@ -992,13 +1023,6 @@
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="thin"/>
       <diagonal/>
     </border>
     <border>
@@ -1100,53 +1124,52 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="133">
+  <cellXfs count="132">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="90"/>
     </xf>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="6" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="9" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="9" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="90"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="9" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1154,8 +1177,8 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1167,8 +1190,8 @@
     <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="17" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -1181,7 +1204,7 @@
     <xf numFmtId="0" fontId="18" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
@@ -1191,13 +1214,13 @@
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="centerContinuous" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="centerContinuous" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="90"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1212,22 +1235,22 @@
     <xf numFmtId="0" fontId="21" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
@@ -1245,10 +1268,10 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="12" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1260,17 +1283,17 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="14" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -1284,17 +1307,17 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="90"/>
     </xf>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1303,10 +1326,10 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1330,7 +1353,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="centerContinuous"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="centerContinuous"/>
     </xf>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1384,14 +1407,20 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="28" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1870,119 +1899,119 @@
     <col min="29" max="29" width="34.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" ht="45" customHeight="1" spans="1:29" s="130" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="130" t="s">
-        <v>135</v>
-      </c>
-      <c r="B2" s="130" t="s">
-        <v>136</v>
-      </c>
-      <c r="C2" s="130" t="s">
-        <v>137</v>
-      </c>
-      <c r="D2" s="130" t="s">
-        <v>138</v>
-      </c>
-      <c r="E2" s="130" t="s">
-        <v>139</v>
-      </c>
-      <c r="F2" s="130" t="s">
-        <v>140</v>
-      </c>
-      <c r="G2" s="130" t="s">
-        <v>75</v>
-      </c>
-      <c r="H2" s="130" t="s">
-        <v>141</v>
-      </c>
-      <c r="I2" s="130" t="s">
+    <row r="2" ht="45" customHeight="1" spans="1:29" s="129" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="129" t="s">
+        <v>145</v>
+      </c>
+      <c r="B2" s="129" t="s">
+        <v>146</v>
+      </c>
+      <c r="C2" s="129" t="s">
+        <v>147</v>
+      </c>
+      <c r="D2" s="129" t="s">
+        <v>148</v>
+      </c>
+      <c r="E2" s="129" t="s">
+        <v>149</v>
+      </c>
+      <c r="F2" s="129" t="s">
+        <v>150</v>
+      </c>
+      <c r="G2" s="129" t="s">
+        <v>77</v>
+      </c>
+      <c r="H2" s="129" t="s">
+        <v>151</v>
+      </c>
+      <c r="I2" s="129" t="s">
         <v>10</v>
       </c>
-      <c r="J2" s="130" t="s">
-        <v>142</v>
-      </c>
-      <c r="K2" s="130" t="s">
-        <v>143</v>
-      </c>
-      <c r="L2" s="130" t="s">
-        <v>144</v>
-      </c>
-      <c r="M2" s="130" t="s">
-        <v>145</v>
-      </c>
-      <c r="O2" s="130" t="s">
-        <v>146</v>
-      </c>
-      <c r="P2" s="130" t="s">
-        <v>147</v>
-      </c>
-      <c r="Q2" s="130" t="s">
-        <v>148</v>
-      </c>
-      <c r="S2" s="130" t="s">
-        <v>149</v>
-      </c>
-      <c r="T2" s="130" t="s">
-        <v>150</v>
-      </c>
-      <c r="U2" s="130" t="s">
-        <v>151</v>
-      </c>
-      <c r="V2" s="130" t="s">
+      <c r="J2" s="129" t="s">
         <v>152</v>
       </c>
-      <c r="Y2" s="130" t="s">
-        <v>146</v>
-      </c>
-      <c r="Z2" s="130" t="s">
+      <c r="K2" s="129" t="s">
         <v>153</v>
       </c>
-      <c r="AA2" s="130" t="s">
+      <c r="L2" s="129" t="s">
         <v>154</v>
       </c>
-      <c r="AB2" s="130" t="s">
+      <c r="M2" s="129" t="s">
         <v>155</v>
       </c>
-      <c r="AC2" s="130" t="s">
+      <c r="O2" s="129" t="s">
         <v>156</v>
+      </c>
+      <c r="P2" s="129" t="s">
+        <v>157</v>
+      </c>
+      <c r="Q2" s="129" t="s">
+        <v>158</v>
+      </c>
+      <c r="S2" s="129" t="s">
+        <v>159</v>
+      </c>
+      <c r="T2" s="129" t="s">
+        <v>160</v>
+      </c>
+      <c r="U2" s="129" t="s">
+        <v>161</v>
+      </c>
+      <c r="V2" s="129" t="s">
+        <v>162</v>
+      </c>
+      <c r="Y2" s="129" t="s">
+        <v>156</v>
+      </c>
+      <c r="Z2" s="129" t="s">
+        <v>163</v>
+      </c>
+      <c r="AA2" s="129" t="s">
+        <v>164</v>
+      </c>
+      <c r="AB2" s="129" t="s">
+        <v>165</v>
+      </c>
+      <c r="AC2" s="129" t="s">
+        <v>166</v>
       </c>
     </row>
     <row r="3" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>157</v>
+        <v>167</v>
       </c>
       <c r="B3" t="s">
-        <v>158</v>
+        <v>168</v>
       </c>
       <c r="C3" t="s">
-        <v>159</v>
+        <v>129</v>
       </c>
       <c r="D3" t="s">
-        <v>160</v>
+        <v>169</v>
       </c>
       <c r="E3" t="s">
-        <v>161</v>
+        <v>170</v>
       </c>
       <c r="F3" t="s">
-        <v>162</v>
+        <v>171</v>
       </c>
       <c r="G3" t="s">
-        <v>163</v>
+        <v>172</v>
       </c>
       <c r="H3" t="s">
-        <v>164</v>
+        <v>173</v>
       </c>
       <c r="I3" t="s">
-        <v>165</v>
+        <v>174</v>
       </c>
       <c r="J3" t="s">
-        <v>166</v>
+        <v>140</v>
       </c>
       <c r="K3" t="s">
-        <v>167</v>
+        <v>175</v>
       </c>
       <c r="L3" t="s">
-        <v>168</v>
+        <v>176</v>
       </c>
       <c r="M3" t="s">
         <v>14</v>
@@ -1991,128 +2020,128 @@
         <v>10</v>
       </c>
       <c r="P3" t="s">
-        <v>169</v>
-      </c>
-      <c r="Q3" s="131">
+        <v>177</v>
+      </c>
+      <c r="Q3" s="130">
         <v>0.15</v>
       </c>
       <c r="S3" t="s">
-        <v>170</v>
+        <v>178</v>
       </c>
       <c r="T3" t="s">
-        <v>171</v>
+        <v>179</v>
       </c>
       <c r="U3" t="s">
-        <v>172</v>
+        <v>180</v>
       </c>
       <c r="V3" t="s">
-        <v>173</v>
+        <v>181</v>
       </c>
       <c r="Y3">
         <v>1</v>
       </c>
       <c r="Z3" t="s">
-        <v>174</v>
+        <v>182</v>
       </c>
       <c r="AA3" t="s">
-        <v>175</v>
+        <v>183</v>
       </c>
       <c r="AB3" t="s">
-        <v>176</v>
+        <v>184</v>
       </c>
       <c r="AC3" t="s">
-        <v>177</v>
+        <v>185</v>
       </c>
     </row>
     <row r="4" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>178</v>
+        <v>186</v>
       </c>
       <c r="B4" t="s">
-        <v>179</v>
+        <v>187</v>
       </c>
       <c r="C4" t="s">
-        <v>159</v>
+        <v>129</v>
       </c>
       <c r="D4">
         <v>9</v>
       </c>
       <c r="E4" t="s">
-        <v>180</v>
-      </c>
-      <c r="F4" s="132">
+        <v>188</v>
+      </c>
+      <c r="F4" s="131">
         <v>1.2</v>
       </c>
       <c r="G4" t="s">
-        <v>163</v>
+        <v>172</v>
       </c>
       <c r="H4" t="s">
-        <v>164</v>
+        <v>173</v>
       </c>
       <c r="I4" t="s">
-        <v>165</v>
+        <v>174</v>
       </c>
       <c r="J4" t="s">
-        <v>166</v>
+        <v>140</v>
       </c>
       <c r="K4" t="s">
-        <v>167</v>
+        <v>175</v>
       </c>
       <c r="L4" t="s">
-        <v>181</v>
+        <v>189</v>
       </c>
       <c r="M4" t="s">
         <v>14</v>
       </c>
       <c r="S4" t="s">
-        <v>182</v>
+        <v>190</v>
       </c>
       <c r="T4" t="s">
         <v>14</v>
       </c>
       <c r="U4" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="V4" t="s">
-        <v>181</v>
+        <v>189</v>
       </c>
     </row>
     <row r="5" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>183</v>
+        <v>191</v>
       </c>
       <c r="B5" t="s">
-        <v>184</v>
+        <v>192</v>
       </c>
       <c r="C5" t="s">
-        <v>185</v>
+        <v>193</v>
       </c>
       <c r="D5">
         <v>11</v>
       </c>
       <c r="E5" t="s">
-        <v>186</v>
+        <v>194</v>
       </c>
       <c r="F5">
         <v>1.1</v>
       </c>
       <c r="G5" t="s">
-        <v>163</v>
+        <v>172</v>
       </c>
       <c r="H5" t="s">
-        <v>164</v>
+        <v>173</v>
       </c>
       <c r="I5" t="s">
-        <v>187</v>
+        <v>195</v>
       </c>
       <c r="J5" t="s">
         <v>11</v>
       </c>
       <c r="K5" t="s">
-        <v>188</v>
+        <v>196</v>
       </c>
       <c r="L5" t="s">
-        <v>181</v>
+        <v>189</v>
       </c>
       <c r="M5" t="s">
         <v>14</v>
@@ -2121,161 +2150,161 @@
         <v>17</v>
       </c>
       <c r="T5" t="s">
-        <v>189</v>
+        <v>197</v>
       </c>
       <c r="U5" t="s">
-        <v>190</v>
+        <v>198</v>
       </c>
       <c r="V5" t="s">
-        <v>191</v>
+        <v>199</v>
       </c>
     </row>
     <row r="6" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>192</v>
+        <v>200</v>
       </c>
       <c r="B6" t="s">
-        <v>193</v>
+        <v>201</v>
       </c>
       <c r="C6" t="s">
-        <v>194</v>
+        <v>202</v>
       </c>
       <c r="D6" t="s">
-        <v>195</v>
+        <v>203</v>
       </c>
       <c r="E6" t="s">
+        <v>204</v>
+      </c>
+      <c r="F6" t="s">
+        <v>205</v>
+      </c>
+      <c r="G6" t="s">
+        <v>206</v>
+      </c>
+      <c r="H6" t="s">
+        <v>207</v>
+      </c>
+      <c r="I6" t="s">
+        <v>174</v>
+      </c>
+      <c r="J6" t="s">
+        <v>140</v>
+      </c>
+      <c r="K6" t="s">
         <v>196</v>
       </c>
-      <c r="F6" t="s">
-        <v>197</v>
-      </c>
-      <c r="G6" t="s">
-        <v>198</v>
-      </c>
-      <c r="H6" t="s">
-        <v>199</v>
-      </c>
-      <c r="I6" t="s">
-        <v>165</v>
-      </c>
-      <c r="J6" t="s">
-        <v>166</v>
-      </c>
-      <c r="K6" t="s">
-        <v>188</v>
-      </c>
       <c r="L6" t="s">
-        <v>168</v>
+        <v>176</v>
       </c>
       <c r="M6" t="s">
         <v>14</v>
       </c>
       <c r="S6" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="T6" t="s">
-        <v>166</v>
+        <v>140</v>
       </c>
       <c r="U6" t="s">
-        <v>200</v>
+        <v>208</v>
       </c>
       <c r="V6" t="s">
-        <v>201</v>
+        <v>209</v>
       </c>
     </row>
     <row r="7" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>202</v>
+        <v>210</v>
       </c>
       <c r="B7" t="s">
-        <v>203</v>
+        <v>211</v>
       </c>
       <c r="C7" t="s">
-        <v>159</v>
+        <v>129</v>
       </c>
       <c r="D7" t="s">
-        <v>160</v>
+        <v>169</v>
       </c>
       <c r="E7" t="s">
-        <v>204</v>
+        <v>212</v>
       </c>
       <c r="F7" t="s">
-        <v>205</v>
+        <v>213</v>
       </c>
       <c r="G7" t="s">
-        <v>163</v>
+        <v>172</v>
       </c>
       <c r="H7" t="s">
-        <v>164</v>
+        <v>173</v>
       </c>
       <c r="I7" t="s">
-        <v>206</v>
+        <v>214</v>
       </c>
       <c r="J7" t="s">
-        <v>171</v>
+        <v>179</v>
       </c>
       <c r="K7" t="s">
-        <v>188</v>
+        <v>196</v>
       </c>
       <c r="L7" t="s">
-        <v>173</v>
+        <v>181</v>
       </c>
       <c r="M7" t="s">
-        <v>171</v>
+        <v>179</v>
       </c>
       <c r="S7" t="s">
         <v>10</v>
       </c>
       <c r="T7" t="s">
-        <v>171</v>
+        <v>179</v>
       </c>
       <c r="U7" t="s">
-        <v>172</v>
+        <v>180</v>
       </c>
       <c r="V7" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="8" spans="2:22" x14ac:dyDescent="0.25">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="8" spans="19:22" x14ac:dyDescent="0.25">
       <c r="S8" t="s">
         <v>10</v>
       </c>
       <c r="T8" t="s">
-        <v>166</v>
+        <v>140</v>
       </c>
       <c r="U8" t="s">
-        <v>200</v>
+        <v>208</v>
       </c>
       <c r="V8" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="9" spans="2:22" x14ac:dyDescent="0.25">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="9" spans="19:22" x14ac:dyDescent="0.25">
       <c r="S9" t="s">
         <v>10</v>
       </c>
       <c r="T9" t="s">
-        <v>207</v>
+        <v>215</v>
       </c>
       <c r="U9" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="V9" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="10" spans="2:22" x14ac:dyDescent="0.25">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="10" spans="19:22" x14ac:dyDescent="0.25">
       <c r="S10" t="s">
-        <v>144</v>
+        <v>154</v>
       </c>
       <c r="T10" t="s">
         <v>14</v>
       </c>
       <c r="U10" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="V10" t="s">
-        <v>168</v>
+        <v>176</v>
       </c>
     </row>
   </sheetData>
@@ -2409,16 +2438,16 @@
       <c r="L4" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="M4" s="21"/>
-      <c r="N4" s="21"/>
-      <c r="O4" s="21"/>
-      <c r="P4" s="21"/>
-      <c r="Q4" s="21"/>
-      <c r="R4" s="22"/>
-      <c r="U4" s="23"/>
+      <c r="M4" s="1"/>
+      <c r="N4" s="1"/>
+      <c r="O4" s="1"/>
+      <c r="P4" s="1"/>
+      <c r="Q4" s="1"/>
+      <c r="R4" s="21"/>
+      <c r="U4" s="22"/>
     </row>
     <row r="5" ht="13.35" customHeight="1" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B5" s="24" t="s">
+      <c r="B5" s="23" t="s">
         <v>9</v>
       </c>
       <c r="C5" s="3"/>
@@ -2430,76 +2459,76 @@
       <c r="I5" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="J5" s="25" t="s">
+      <c r="J5" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="K5" s="21"/>
-      <c r="L5" s="26" t="s">
+      <c r="K5" s="1"/>
+      <c r="L5" s="25" t="s">
         <v>12</v>
       </c>
-      <c r="M5" s="21"/>
-      <c r="O5" s="27" t="s">
+      <c r="M5" s="1"/>
+      <c r="O5" s="26" t="s">
         <v>13</v>
       </c>
-      <c r="P5" s="25" t="s">
+      <c r="P5" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="Q5" s="21"/>
-      <c r="R5" s="28" t="str">
+      <c r="Q5" s="1"/>
+      <c r="R5" s="27" t="str">
         <f>СhiefVec</f>
         <v>Кумар М.Б.</v>
       </c>
-      <c r="U5" s="29"/>
+      <c r="U5" s="28"/>
     </row>
     <row r="6" ht="13.7" customHeight="1" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B6" s="24"/>
+      <c r="B6" s="23"/>
       <c r="C6" s="3"/>
       <c r="D6" s="4"/>
       <c r="E6" s="5"/>
       <c r="F6" s="18"/>
       <c r="G6" s="7"/>
       <c r="H6" s="8"/>
-      <c r="I6" s="30" t="s">
+      <c r="I6" s="29" t="s">
         <v>15</v>
       </c>
-      <c r="K6" s="31" t="s">
+      <c r="K6" s="30" t="s">
         <v>16</v>
       </c>
-      <c r="L6" s="31"/>
-      <c r="M6" s="31"/>
-      <c r="N6" s="31"/>
-      <c r="O6" s="31"/>
-      <c r="P6" s="31"/>
-      <c r="Q6" s="31"/>
-      <c r="R6" s="31"/>
-      <c r="U6" s="29"/>
+      <c r="L6" s="30"/>
+      <c r="M6" s="30"/>
+      <c r="N6" s="30"/>
+      <c r="O6" s="30"/>
+      <c r="P6" s="30"/>
+      <c r="Q6" s="30"/>
+      <c r="R6" s="30"/>
+      <c r="U6" s="28"/>
     </row>
     <row r="7" ht="15.75" customHeight="1" spans="2:34" x14ac:dyDescent="0.25">
-      <c r="B7" s="24"/>
+      <c r="B7" s="23"/>
       <c r="C7" s="3"/>
       <c r="D7" s="4"/>
       <c r="E7" s="5"/>
       <c r="F7" s="18"/>
       <c r="G7" s="7"/>
       <c r="H7" s="8"/>
-      <c r="I7" s="32" t="s">
+      <c r="I7" s="31" t="s">
         <v>17</v>
       </c>
-      <c r="J7" s="32"/>
-      <c r="K7" s="32"/>
-      <c r="L7" s="32"/>
-      <c r="M7" s="32"/>
-      <c r="N7" s="33"/>
-      <c r="O7" s="33"/>
-      <c r="P7" s="33"/>
-      <c r="Q7" s="33"/>
-      <c r="R7" s="34" t="s">
+      <c r="J7" s="31"/>
+      <c r="K7" s="31"/>
+      <c r="L7" s="31"/>
+      <c r="M7" s="31"/>
+      <c r="N7" s="32"/>
+      <c r="O7" s="32"/>
+      <c r="P7" s="32"/>
+      <c r="Q7" s="32"/>
+      <c r="R7" s="33" t="s">
         <v>18</v>
       </c>
-      <c r="T7" s="35"/>
-      <c r="U7" s="35"/>
-      <c r="V7" s="35"/>
-      <c r="W7" s="35"/>
+      <c r="T7" s="34"/>
+      <c r="U7" s="34"/>
+      <c r="V7" s="34"/>
+      <c r="W7" s="34"/>
       <c r="AE7" s="1" t="s">
         <v>19</v>
       </c>
@@ -2514,33 +2543,33 @@
       </c>
     </row>
     <row r="8" ht="10.35" customHeight="1" spans="2:34" x14ac:dyDescent="0.25">
-      <c r="B8" s="24"/>
+      <c r="B8" s="23"/>
       <c r="C8" s="3"/>
       <c r="D8" s="4"/>
       <c r="E8" s="5"/>
-      <c r="F8" s="36"/>
-      <c r="G8" s="37" t="s">
+      <c r="F8" s="35"/>
+      <c r="G8" s="36" t="s">
         <v>23</v>
       </c>
-      <c r="H8" s="38"/>
-      <c r="I8" s="39" t="s">
+      <c r="H8" s="37"/>
+      <c r="I8" s="38" t="s">
         <v>24</v>
       </c>
-      <c r="J8" s="40" t="s">
+      <c r="J8" s="39" t="s">
         <v>25</v>
       </c>
-      <c r="K8" s="41"/>
-      <c r="L8" s="41"/>
-      <c r="M8" s="41"/>
-      <c r="N8" s="41"/>
-      <c r="O8" s="41"/>
-      <c r="P8" s="41"/>
-      <c r="Q8" s="41"/>
-      <c r="R8" s="42"/>
-      <c r="T8" s="35"/>
-      <c r="U8" s="35"/>
-      <c r="V8" s="35"/>
-      <c r="W8" s="35"/>
+      <c r="K8" s="40"/>
+      <c r="L8" s="40"/>
+      <c r="M8" s="40"/>
+      <c r="N8" s="40"/>
+      <c r="O8" s="40"/>
+      <c r="P8" s="40"/>
+      <c r="Q8" s="40"/>
+      <c r="R8" s="41"/>
+      <c r="T8" s="34"/>
+      <c r="U8" s="34"/>
+      <c r="V8" s="34"/>
+      <c r="W8" s="34"/>
       <c r="AE8" s="1" t="s">
         <v>19</v>
       </c>
@@ -2555,38 +2584,38 @@
       </c>
     </row>
     <row r="9" ht="9" customHeight="1" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A9" s="43"/>
-      <c r="B9" s="24"/>
+      <c r="A9" s="42"/>
+      <c r="B9" s="23"/>
       <c r="D9" s="4"/>
       <c r="E9" s="5"/>
-      <c r="F9" s="44" t="str">
+      <c r="F9" s="43" t="str">
         <f>СhiefVec</f>
         <v>Кумар М.Б.</v>
       </c>
-      <c r="G9" s="37"/>
+      <c r="G9" s="36"/>
       <c r="H9" s="8"/>
-      <c r="I9" s="45" t="s">
+      <c r="I9" s="44" t="s">
         <v>27</v>
       </c>
-      <c r="J9" s="46"/>
-      <c r="K9" s="47"/>
-      <c r="L9" s="45" t="s">
+      <c r="J9" s="45"/>
+      <c r="K9" s="46"/>
+      <c r="L9" s="44" t="s">
         <v>28</v>
       </c>
-      <c r="M9" s="46"/>
-      <c r="N9" s="47"/>
-      <c r="O9" s="48" t="s">
+      <c r="M9" s="45"/>
+      <c r="N9" s="46"/>
+      <c r="O9" s="47" t="s">
         <v>29</v>
       </c>
-      <c r="P9" s="48"/>
-      <c r="Q9" s="48" t="s">
+      <c r="P9" s="47"/>
+      <c r="Q9" s="47" t="s">
         <v>30</v>
       </c>
-      <c r="R9" s="48"/>
-      <c r="T9" s="35"/>
-      <c r="U9" s="35"/>
-      <c r="V9" s="35"/>
-      <c r="W9" s="35"/>
+      <c r="R9" s="47"/>
+      <c r="T9" s="34"/>
+      <c r="U9" s="34"/>
+      <c r="V9" s="34"/>
+      <c r="W9" s="34"/>
       <c r="AE9" s="1" t="s">
         <v>19</v>
       </c>
@@ -2601,47 +2630,47 @@
       </c>
     </row>
     <row r="10" ht="10.7" customHeight="1" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A10" s="43"/>
-      <c r="B10" s="24"/>
-      <c r="C10" s="24" t="s">
+      <c r="A10" s="42"/>
+      <c r="B10" s="23"/>
+      <c r="C10" s="23" t="s">
         <v>32</v>
       </c>
       <c r="D10" s="4"/>
       <c r="E10" s="5"/>
-      <c r="F10" s="44"/>
-      <c r="G10" s="37"/>
+      <c r="F10" s="43"/>
+      <c r="G10" s="36"/>
       <c r="H10" s="8"/>
-      <c r="I10" s="49" t="s">
+      <c r="I10" s="48" t="s">
         <v>33</v>
       </c>
-      <c r="J10" s="50"/>
-      <c r="K10" s="51"/>
-      <c r="L10" s="52" t="s">
+      <c r="J10" s="49"/>
+      <c r="K10" s="50"/>
+      <c r="L10" s="51" t="s">
         <v>34</v>
       </c>
-      <c r="M10" s="53"/>
-      <c r="N10" s="54"/>
-      <c r="O10" s="55" t="s">
+      <c r="M10" s="52"/>
+      <c r="N10" s="53"/>
+      <c r="O10" s="54" t="s">
         <v>35</v>
       </c>
-      <c r="P10" s="56">
-        <f>IF(T10,TEXT(U10,"ч:мм")&amp;" "&amp;TEXT(T10,"дд.мм.гггг"),"")</f>
-      </c>
-      <c r="Q10" s="55" t="s">
+      <c r="P10" s="55" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q10" s="54" t="s">
         <v>35</v>
       </c>
-      <c r="R10" s="57">
-        <f>IF(V10,TEXT(W10,"ч:мм")&amp;" "&amp;TEXT(V10,"дд.мм.гггг"),"")</f>
-      </c>
-      <c r="T10" s="58"/>
-      <c r="U10" s="59"/>
-      <c r="V10" s="58"/>
-      <c r="W10" s="59"/>
+      <c r="R10" s="56" t="s">
+        <v>37</v>
+      </c>
+      <c r="T10" s="57"/>
+      <c r="U10" s="58"/>
+      <c r="V10" s="57"/>
+      <c r="W10" s="58"/>
       <c r="AE10" s="1" t="s">
         <v>19</v>
       </c>
       <c r="AF10" s="1" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="AG10" s="1" t="s">
         <v>21</v>
@@ -2651,38 +2680,38 @@
       </c>
     </row>
     <row r="11" ht="11.45" customHeight="1" spans="2:34" x14ac:dyDescent="0.25">
-      <c r="B11" s="24"/>
-      <c r="C11" s="24"/>
+      <c r="B11" s="23"/>
+      <c r="C11" s="23"/>
       <c r="D11" s="4"/>
       <c r="E11" s="5"/>
-      <c r="F11" s="44"/>
-      <c r="G11" s="37"/>
+      <c r="F11" s="43"/>
+      <c r="G11" s="36"/>
       <c r="H11" s="8"/>
-      <c r="I11" s="49"/>
-      <c r="J11" s="50"/>
-      <c r="K11" s="51"/>
-      <c r="L11" s="52" t="s">
-        <v>37</v>
-      </c>
-      <c r="M11" s="53"/>
-      <c r="N11" s="54"/>
-      <c r="O11" s="60" t="s">
-        <v>38</v>
-      </c>
-      <c r="P11" s="60"/>
-      <c r="Q11" s="60" t="s">
-        <v>38</v>
-      </c>
-      <c r="R11" s="60"/>
-      <c r="T11" s="61"/>
-      <c r="U11" s="61"/>
-      <c r="V11" s="61"/>
-      <c r="W11" s="61"/>
+      <c r="I11" s="48"/>
+      <c r="J11" s="49"/>
+      <c r="K11" s="50"/>
+      <c r="L11" s="51" t="s">
+        <v>39</v>
+      </c>
+      <c r="M11" s="52"/>
+      <c r="N11" s="53"/>
+      <c r="O11" s="59" t="s">
+        <v>40</v>
+      </c>
+      <c r="P11" s="59"/>
+      <c r="Q11" s="59" t="s">
+        <v>40</v>
+      </c>
+      <c r="R11" s="59"/>
+      <c r="T11" s="60"/>
+      <c r="U11" s="60"/>
+      <c r="V11" s="60"/>
+      <c r="W11" s="60"/>
       <c r="AE11" s="1" t="s">
         <v>19</v>
       </c>
       <c r="AF11" s="1" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="AG11" s="1" t="s">
         <v>21</v>
@@ -2692,7 +2721,7 @@
       </c>
     </row>
     <row r="12" ht="9.6" customHeight="1" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A12" s="62" t="str">
+      <c r="A12" s="61" t="str">
         <f>O3</f>
         <v>123456</v>
       </c>
@@ -2700,52 +2729,52 @@
         <f>M33</f>
         <v>AA1234FF</v>
       </c>
-      <c r="C12" s="24"/>
+      <c r="C12" s="23"/>
       <c r="D12" s="4"/>
       <c r="E12" s="5"/>
-      <c r="F12" s="44"/>
-      <c r="G12" s="37"/>
+      <c r="F12" s="43"/>
+      <c r="G12" s="36"/>
       <c r="H12" s="8"/>
-      <c r="I12" s="63" t="s">
-        <v>40</v>
-      </c>
-      <c r="J12" s="63" t="s">
+      <c r="I12" s="62" t="s">
+        <v>42</v>
+      </c>
+      <c r="J12" s="62" t="s">
         <v>18</v>
       </c>
-      <c r="K12" s="64" t="s">
-        <v>41</v>
-      </c>
-      <c r="L12" s="63" t="s">
-        <v>42</v>
-      </c>
-      <c r="M12" s="63" t="s">
+      <c r="K12" s="63" t="s">
         <v>43</v>
       </c>
-      <c r="N12" s="64" t="s">
-        <v>41</v>
-      </c>
-      <c r="O12" s="63" t="s">
+      <c r="L12" s="62" t="s">
         <v>44</v>
       </c>
-      <c r="P12" s="65">
+      <c r="M12" s="62" t="s">
+        <v>45</v>
+      </c>
+      <c r="N12" s="63" t="s">
+        <v>43</v>
+      </c>
+      <c r="O12" s="62" t="s">
+        <v>46</v>
+      </c>
+      <c r="P12" s="64">
         <v>12337</v>
       </c>
-      <c r="Q12" s="63" t="s">
-        <v>45</v>
-      </c>
-      <c r="R12" s="65">
+      <c r="Q12" s="62" t="s">
+        <v>47</v>
+      </c>
+      <c r="R12" s="64">
         <v>12338</v>
       </c>
-      <c r="S12" s="66"/>
-      <c r="T12" s="58"/>
-      <c r="U12" s="59"/>
-      <c r="V12" s="58"/>
-      <c r="W12" s="59"/>
+      <c r="S12" s="65"/>
+      <c r="T12" s="57"/>
+      <c r="U12" s="58"/>
+      <c r="V12" s="57"/>
+      <c r="W12" s="58"/>
       <c r="AE12" s="1" t="s">
         <v>19</v>
       </c>
       <c r="AF12" s="1" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="AG12" s="1" t="s">
         <v>21</v>
@@ -2755,41 +2784,41 @@
       </c>
     </row>
     <row r="13" ht="6" customHeight="1" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A13" s="62"/>
+      <c r="A13" s="61"/>
       <c r="B13" s="3"/>
-      <c r="C13" s="24"/>
+      <c r="C13" s="23"/>
       <c r="D13" s="4"/>
       <c r="E13" s="5"/>
-      <c r="F13" s="44"/>
-      <c r="G13" s="37"/>
+      <c r="F13" s="43"/>
+      <c r="G13" s="36"/>
       <c r="H13" s="8"/>
-      <c r="I13" s="67"/>
-      <c r="J13" s="68" t="s">
-        <v>47</v>
+      <c r="I13" s="66"/>
+      <c r="J13" s="67" t="s">
+        <v>49</v>
       </c>
       <c r="K13" s="17"/>
-      <c r="L13" s="67"/>
-      <c r="M13" s="68" t="s">
-        <v>47</v>
+      <c r="L13" s="66"/>
+      <c r="M13" s="67" t="s">
+        <v>49</v>
       </c>
       <c r="N13" s="17"/>
-      <c r="O13" s="69" t="s">
-        <v>48</v>
-      </c>
-      <c r="P13" s="70"/>
-      <c r="Q13" s="69" t="s">
-        <v>48</v>
-      </c>
-      <c r="R13" s="71"/>
-      <c r="T13" s="72"/>
-      <c r="U13" s="73"/>
-      <c r="V13" s="74"/>
-      <c r="W13" s="73"/>
+      <c r="O13" s="68" t="s">
+        <v>50</v>
+      </c>
+      <c r="P13" s="69"/>
+      <c r="Q13" s="68" t="s">
+        <v>50</v>
+      </c>
+      <c r="R13" s="70"/>
+      <c r="T13" s="71"/>
+      <c r="U13" s="72"/>
+      <c r="V13" s="73"/>
+      <c r="W13" s="72"/>
       <c r="AE13" s="1" t="s">
         <v>19</v>
       </c>
       <c r="AF13" s="1" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="AG13" s="1" t="s">
         <v>21</v>
@@ -2799,54 +2828,54 @@
       </c>
     </row>
     <row r="14" ht="9.6" customHeight="1" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A14" s="62"/>
+      <c r="A14" s="61"/>
       <c r="B14" s="3"/>
-      <c r="C14" s="24"/>
+      <c r="C14" s="23"/>
       <c r="D14" s="4"/>
       <c r="E14" s="5"/>
-      <c r="F14" s="44"/>
-      <c r="G14" s="37"/>
+      <c r="F14" s="43"/>
+      <c r="G14" s="36"/>
       <c r="H14" s="8"/>
-      <c r="I14" s="63" t="s">
-        <v>40</v>
-      </c>
-      <c r="J14" s="63" t="s">
+      <c r="I14" s="62" t="s">
+        <v>42</v>
+      </c>
+      <c r="J14" s="62" t="s">
         <v>18</v>
       </c>
-      <c r="K14" s="64" t="s">
-        <v>50</v>
-      </c>
-      <c r="L14" s="63" t="s">
-        <v>42</v>
-      </c>
-      <c r="M14" s="63" t="s">
-        <v>43</v>
-      </c>
-      <c r="N14" s="64" t="s">
-        <v>50</v>
-      </c>
-      <c r="O14" s="63" t="s">
-        <v>51</v>
-      </c>
-      <c r="P14" s="75">
+      <c r="K14" s="63" t="s">
+        <v>52</v>
+      </c>
+      <c r="L14" s="62" t="s">
+        <v>44</v>
+      </c>
+      <c r="M14" s="62" t="s">
+        <v>45</v>
+      </c>
+      <c r="N14" s="63" t="s">
+        <v>52</v>
+      </c>
+      <c r="O14" s="62" t="s">
+        <v>53</v>
+      </c>
+      <c r="P14" s="74">
         <v>12339</v>
       </c>
-      <c r="Q14" s="63" t="s">
-        <v>52</v>
-      </c>
-      <c r="R14" s="65">
+      <c r="Q14" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="R14" s="64">
         <v>12340</v>
       </c>
-      <c r="S14" s="76"/>
-      <c r="T14" s="58"/>
-      <c r="U14" s="59"/>
-      <c r="V14" s="58"/>
-      <c r="W14" s="59"/>
+      <c r="S14" s="75"/>
+      <c r="T14" s="57"/>
+      <c r="U14" s="58"/>
+      <c r="V14" s="57"/>
+      <c r="W14" s="58"/>
       <c r="AE14" s="1" t="s">
         <v>19</v>
       </c>
       <c r="AF14" s="1" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="AG14" s="1" t="s">
         <v>21</v>
@@ -2856,42 +2885,42 @@
       </c>
     </row>
     <row r="15" ht="6" customHeight="1" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A15" s="62"/>
+      <c r="A15" s="61"/>
       <c r="B15" s="3"/>
-      <c r="C15" s="24"/>
+      <c r="C15" s="23"/>
       <c r="D15" s="4"/>
       <c r="E15" s="5"/>
-      <c r="F15" s="44"/>
-      <c r="G15" s="37"/>
+      <c r="F15" s="43"/>
+      <c r="G15" s="36"/>
       <c r="H15" s="8"/>
-      <c r="I15" s="67"/>
-      <c r="J15" s="68" t="s">
-        <v>47</v>
+      <c r="I15" s="66"/>
+      <c r="J15" s="67" t="s">
+        <v>49</v>
       </c>
       <c r="K15" s="17"/>
-      <c r="L15" s="67"/>
-      <c r="M15" s="68" t="s">
-        <v>47</v>
+      <c r="L15" s="66"/>
+      <c r="M15" s="67" t="s">
+        <v>49</v>
       </c>
       <c r="N15" s="17"/>
-      <c r="O15" s="69" t="s">
-        <v>48</v>
-      </c>
-      <c r="P15" s="70"/>
-      <c r="Q15" s="69" t="s">
-        <v>48</v>
-      </c>
-      <c r="R15" s="71"/>
-      <c r="S15" s="76"/>
-      <c r="T15" s="72"/>
-      <c r="U15" s="73"/>
-      <c r="V15" s="74"/>
-      <c r="W15" s="73"/>
+      <c r="O15" s="68" t="s">
+        <v>50</v>
+      </c>
+      <c r="P15" s="69"/>
+      <c r="Q15" s="68" t="s">
+        <v>50</v>
+      </c>
+      <c r="R15" s="70"/>
+      <c r="S15" s="75"/>
+      <c r="T15" s="71"/>
+      <c r="U15" s="72"/>
+      <c r="V15" s="73"/>
+      <c r="W15" s="72"/>
       <c r="AE15" s="1" t="s">
         <v>19</v>
       </c>
       <c r="AF15" s="1" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="AG15" s="1" t="s">
         <v>21</v>
@@ -2901,54 +2930,54 @@
       </c>
     </row>
     <row r="16" ht="9.6" customHeight="1" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A16" s="62"/>
+      <c r="A16" s="61"/>
       <c r="B16" s="3"/>
-      <c r="C16" s="24"/>
+      <c r="C16" s="23"/>
       <c r="D16" s="4"/>
       <c r="E16" s="5"/>
-      <c r="F16" s="44"/>
-      <c r="G16" s="37"/>
+      <c r="F16" s="43"/>
+      <c r="G16" s="36"/>
       <c r="H16" s="8"/>
-      <c r="I16" s="63" t="s">
-        <v>40</v>
-      </c>
-      <c r="J16" s="63" t="s">
+      <c r="I16" s="62" t="s">
+        <v>42</v>
+      </c>
+      <c r="J16" s="62" t="s">
         <v>18</v>
       </c>
-      <c r="K16" s="64" t="s">
-        <v>55</v>
-      </c>
-      <c r="L16" s="63" t="s">
-        <v>42</v>
-      </c>
-      <c r="M16" s="63" t="s">
-        <v>43</v>
-      </c>
-      <c r="N16" s="64" t="s">
-        <v>55</v>
-      </c>
-      <c r="O16" s="63" t="s">
-        <v>56</v>
-      </c>
-      <c r="P16" s="75">
+      <c r="K16" s="63" t="s">
+        <v>57</v>
+      </c>
+      <c r="L16" s="62" t="s">
+        <v>44</v>
+      </c>
+      <c r="M16" s="62" t="s">
+        <v>45</v>
+      </c>
+      <c r="N16" s="63" t="s">
+        <v>57</v>
+      </c>
+      <c r="O16" s="62" t="s">
+        <v>58</v>
+      </c>
+      <c r="P16" s="74">
         <v>12340</v>
       </c>
-      <c r="Q16" s="63" t="s">
-        <v>57</v>
-      </c>
-      <c r="R16" s="65">
+      <c r="Q16" s="62" t="s">
+        <v>59</v>
+      </c>
+      <c r="R16" s="64">
         <v>12345</v>
       </c>
-      <c r="S16" s="76"/>
-      <c r="T16" s="58"/>
-      <c r="U16" s="59"/>
-      <c r="V16" s="58"/>
-      <c r="W16" s="59"/>
+      <c r="S16" s="75"/>
+      <c r="T16" s="57"/>
+      <c r="U16" s="58"/>
+      <c r="V16" s="57"/>
+      <c r="W16" s="58"/>
       <c r="AE16" s="1" t="s">
         <v>19</v>
       </c>
       <c r="AF16" s="1" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="AG16" s="1" t="s">
         <v>21</v>
@@ -2958,992 +2987,1101 @@
       </c>
     </row>
     <row r="17" ht="6" customHeight="1" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A17" s="62"/>
+      <c r="A17" s="61"/>
       <c r="B17" s="3"/>
-      <c r="C17" s="24"/>
+      <c r="C17" s="23"/>
       <c r="D17" s="4"/>
       <c r="E17" s="5"/>
-      <c r="F17" s="44"/>
-      <c r="G17" s="37"/>
+      <c r="F17" s="43"/>
+      <c r="G17" s="36"/>
       <c r="H17" s="8"/>
-      <c r="I17" s="67"/>
-      <c r="J17" s="68" t="s">
-        <v>47</v>
-      </c>
-      <c r="K17" s="77"/>
-      <c r="L17" s="67"/>
-      <c r="M17" s="68" t="s">
-        <v>47</v>
-      </c>
-      <c r="N17" s="77"/>
-      <c r="O17" s="69" t="s">
-        <v>48</v>
-      </c>
-      <c r="P17" s="70"/>
-      <c r="Q17" s="69" t="s">
-        <v>48</v>
-      </c>
-      <c r="R17" s="71"/>
-      <c r="S17" s="76"/>
-      <c r="T17" s="72"/>
-      <c r="U17" s="73"/>
-      <c r="V17" s="74"/>
-      <c r="W17" s="73"/>
+      <c r="I17" s="66"/>
+      <c r="J17" s="67" t="s">
+        <v>49</v>
+      </c>
+      <c r="K17" s="76"/>
+      <c r="L17" s="66"/>
+      <c r="M17" s="67" t="s">
+        <v>49</v>
+      </c>
+      <c r="N17" s="76"/>
+      <c r="O17" s="68" t="s">
+        <v>50</v>
+      </c>
+      <c r="P17" s="69"/>
+      <c r="Q17" s="68" t="s">
+        <v>50</v>
+      </c>
+      <c r="R17" s="70"/>
+      <c r="S17" s="75"/>
+      <c r="T17" s="71"/>
+      <c r="U17" s="72"/>
+      <c r="V17" s="73"/>
+      <c r="W17" s="72"/>
     </row>
     <row r="18" ht="9.6" customHeight="1" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A18" s="78" t="s">
-        <v>59</v>
+      <c r="A18" s="77" t="s">
+        <v>61</v>
       </c>
       <c r="B18" s="3"/>
-      <c r="C18" s="24"/>
+      <c r="C18" s="23"/>
       <c r="D18" s="4"/>
       <c r="E18" s="5"/>
-      <c r="F18" s="44"/>
-      <c r="G18" s="37"/>
+      <c r="F18" s="43"/>
+      <c r="G18" s="36"/>
       <c r="H18" s="8"/>
-      <c r="I18" s="63" t="s">
-        <v>40</v>
-      </c>
-      <c r="J18" s="63" t="s">
+      <c r="I18" s="62" t="s">
+        <v>42</v>
+      </c>
+      <c r="J18" s="62" t="s">
         <v>18</v>
       </c>
-      <c r="K18" s="64" t="s">
-        <v>60</v>
-      </c>
-      <c r="L18" s="63" t="s">
-        <v>42</v>
-      </c>
-      <c r="M18" s="63" t="s">
-        <v>43</v>
-      </c>
-      <c r="N18" s="64" t="s">
-        <v>60</v>
-      </c>
-      <c r="O18" s="63" t="s">
-        <v>61</v>
-      </c>
-      <c r="P18" s="75">
+      <c r="K18" s="63" t="s">
+        <v>62</v>
+      </c>
+      <c r="L18" s="62" t="s">
+        <v>44</v>
+      </c>
+      <c r="M18" s="62" t="s">
+        <v>45</v>
+      </c>
+      <c r="N18" s="63" t="s">
+        <v>62</v>
+      </c>
+      <c r="O18" s="62" t="s">
+        <v>63</v>
+      </c>
+      <c r="P18" s="74">
         <v>12345</v>
       </c>
-      <c r="Q18" s="63" t="s">
-        <v>62</v>
-      </c>
-      <c r="R18" s="65">
+      <c r="Q18" s="62" t="s">
+        <v>64</v>
+      </c>
+      <c r="R18" s="64">
         <v>12349</v>
       </c>
-      <c r="S18" s="76"/>
-      <c r="T18" s="58"/>
-      <c r="U18" s="59"/>
-      <c r="V18" s="58"/>
-      <c r="W18" s="59"/>
+      <c r="S18" s="75"/>
+      <c r="T18" s="57"/>
+      <c r="U18" s="58"/>
+      <c r="V18" s="57"/>
+      <c r="W18" s="58"/>
     </row>
     <row r="19" ht="6" customHeight="1" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A19" s="78"/>
+      <c r="A19" s="77"/>
       <c r="B19" s="3"/>
-      <c r="C19" s="24"/>
+      <c r="C19" s="23"/>
       <c r="D19" s="4"/>
       <c r="E19" s="5"/>
-      <c r="F19" s="44"/>
-      <c r="G19" s="37"/>
+      <c r="F19" s="43"/>
+      <c r="G19" s="36"/>
       <c r="H19" s="8"/>
-      <c r="I19" s="67"/>
-      <c r="J19" s="68" t="s">
-        <v>47</v>
-      </c>
-      <c r="K19" s="77"/>
-      <c r="L19" s="67"/>
-      <c r="M19" s="68" t="s">
-        <v>47</v>
-      </c>
-      <c r="N19" s="77"/>
-      <c r="O19" s="69" t="s">
-        <v>48</v>
-      </c>
-      <c r="P19" s="70"/>
-      <c r="Q19" s="69" t="s">
-        <v>48</v>
-      </c>
-      <c r="R19" s="71"/>
-      <c r="S19" s="76"/>
-      <c r="T19" s="72"/>
-      <c r="U19" s="73"/>
-      <c r="V19" s="74"/>
-      <c r="W19" s="73"/>
+      <c r="I19" s="66"/>
+      <c r="J19" s="67" t="s">
+        <v>49</v>
+      </c>
+      <c r="K19" s="76"/>
+      <c r="L19" s="66"/>
+      <c r="M19" s="67" t="s">
+        <v>49</v>
+      </c>
+      <c r="N19" s="76"/>
+      <c r="O19" s="68" t="s">
+        <v>50</v>
+      </c>
+      <c r="P19" s="69"/>
+      <c r="Q19" s="68" t="s">
+        <v>50</v>
+      </c>
+      <c r="R19" s="70"/>
+      <c r="S19" s="75"/>
+      <c r="T19" s="71"/>
+      <c r="U19" s="72"/>
+      <c r="V19" s="73"/>
+      <c r="W19" s="72"/>
     </row>
     <row r="20" ht="9.6" customHeight="1" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A20" s="78"/>
-      <c r="B20" s="24" t="s">
-        <v>63</v>
-      </c>
-      <c r="C20" s="24"/>
+      <c r="A20" s="77"/>
+      <c r="B20" s="23" t="s">
+        <v>65</v>
+      </c>
+      <c r="C20" s="23"/>
       <c r="D20" s="4"/>
       <c r="E20" s="5"/>
-      <c r="F20" s="44"/>
-      <c r="G20" s="37"/>
+      <c r="F20" s="43"/>
+      <c r="G20" s="36"/>
       <c r="H20" s="8"/>
-      <c r="I20" s="63" t="s">
-        <v>40</v>
-      </c>
-      <c r="J20" s="63" t="s">
+      <c r="I20" s="62" t="s">
+        <v>42</v>
+      </c>
+      <c r="J20" s="62" t="s">
         <v>18</v>
       </c>
-      <c r="K20" s="64" t="s">
-        <v>64</v>
-      </c>
-      <c r="L20" s="63" t="s">
-        <v>42</v>
-      </c>
-      <c r="M20" s="63" t="s">
-        <v>43</v>
-      </c>
-      <c r="N20" s="64" t="s">
-        <v>64</v>
-      </c>
-      <c r="O20" s="63" t="s">
-        <v>65</v>
-      </c>
-      <c r="P20" s="75">
+      <c r="K20" s="63" t="s">
+        <v>66</v>
+      </c>
+      <c r="L20" s="62" t="s">
+        <v>44</v>
+      </c>
+      <c r="M20" s="62" t="s">
+        <v>45</v>
+      </c>
+      <c r="N20" s="63" t="s">
+        <v>66</v>
+      </c>
+      <c r="O20" s="62" t="s">
+        <v>67</v>
+      </c>
+      <c r="P20" s="74">
         <v>12349</v>
       </c>
-      <c r="Q20" s="63" t="s">
-        <v>66</v>
-      </c>
-      <c r="R20" s="65">
+      <c r="Q20" s="62" t="s">
+        <v>68</v>
+      </c>
+      <c r="R20" s="64">
         <v>12353</v>
       </c>
-      <c r="S20" s="76"/>
-      <c r="T20" s="58"/>
-      <c r="U20" s="59"/>
-      <c r="V20" s="58"/>
-      <c r="W20" s="59"/>
+      <c r="S20" s="75"/>
+      <c r="T20" s="57"/>
+      <c r="U20" s="58"/>
+      <c r="V20" s="57"/>
+      <c r="W20" s="58"/>
     </row>
     <row r="21" ht="6" customHeight="1" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A21" s="78"/>
-      <c r="B21" s="24"/>
-      <c r="C21" s="36"/>
+      <c r="A21" s="77"/>
+      <c r="B21" s="23"/>
+      <c r="C21" s="35"/>
       <c r="D21" s="4"/>
       <c r="E21" s="5"/>
-      <c r="F21" s="44"/>
-      <c r="G21" s="37"/>
+      <c r="F21" s="43"/>
+      <c r="G21" s="36"/>
       <c r="H21" s="8"/>
-      <c r="I21" s="67"/>
-      <c r="J21" s="68" t="s">
-        <v>47</v>
-      </c>
-      <c r="K21" s="77"/>
-      <c r="L21" s="67"/>
-      <c r="M21" s="68" t="s">
-        <v>47</v>
-      </c>
-      <c r="N21" s="77"/>
-      <c r="O21" s="69" t="s">
-        <v>48</v>
-      </c>
-      <c r="P21" s="70"/>
-      <c r="Q21" s="69" t="s">
-        <v>48</v>
-      </c>
-      <c r="R21" s="71"/>
-      <c r="S21" s="76"/>
-      <c r="T21" s="72"/>
-      <c r="U21" s="73"/>
-      <c r="V21" s="74"/>
-      <c r="W21" s="73"/>
+      <c r="I21" s="66"/>
+      <c r="J21" s="67" t="s">
+        <v>49</v>
+      </c>
+      <c r="K21" s="76"/>
+      <c r="L21" s="66"/>
+      <c r="M21" s="67" t="s">
+        <v>49</v>
+      </c>
+      <c r="N21" s="76"/>
+      <c r="O21" s="68" t="s">
+        <v>50</v>
+      </c>
+      <c r="P21" s="69"/>
+      <c r="Q21" s="68" t="s">
+        <v>50</v>
+      </c>
+      <c r="R21" s="70"/>
+      <c r="S21" s="75"/>
+      <c r="T21" s="71"/>
+      <c r="U21" s="72"/>
+      <c r="V21" s="73"/>
+      <c r="W21" s="72"/>
     </row>
     <row r="22" ht="9.6" customHeight="1" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A22" s="78"/>
-      <c r="B22" s="24"/>
-      <c r="C22" s="36"/>
+      <c r="A22" s="77"/>
+      <c r="B22" s="23"/>
+      <c r="C22" s="35"/>
       <c r="D22" s="4"/>
       <c r="E22" s="5"/>
-      <c r="F22" s="44"/>
-      <c r="G22" s="37"/>
+      <c r="F22" s="43"/>
+      <c r="G22" s="36"/>
       <c r="H22" s="8"/>
-      <c r="I22" s="63" t="s">
-        <v>67</v>
-      </c>
-      <c r="J22" s="63" t="s">
-        <v>67</v>
-      </c>
-      <c r="K22" s="64" t="s">
-        <v>67</v>
-      </c>
-      <c r="L22" s="63" t="s">
-        <v>67</v>
-      </c>
-      <c r="M22" s="63" t="s">
-        <v>67</v>
-      </c>
-      <c r="N22" s="64" t="s">
-        <v>67</v>
-      </c>
-      <c r="O22" s="63" t="s">
-        <v>67</v>
-      </c>
-      <c r="P22" s="75" t="s">
-        <v>67</v>
-      </c>
-      <c r="Q22" s="63" t="s">
-        <v>67</v>
-      </c>
-      <c r="R22" s="65" t="s">
-        <v>67</v>
-      </c>
-      <c r="S22" s="76"/>
-      <c r="T22" s="58"/>
-      <c r="U22" s="59"/>
-      <c r="V22" s="58"/>
-      <c r="W22" s="59"/>
+      <c r="I22" s="62" t="s">
+        <v>69</v>
+      </c>
+      <c r="J22" s="62" t="s">
+        <v>69</v>
+      </c>
+      <c r="K22" s="63" t="s">
+        <v>69</v>
+      </c>
+      <c r="L22" s="62" t="s">
+        <v>69</v>
+      </c>
+      <c r="M22" s="62" t="s">
+        <v>69</v>
+      </c>
+      <c r="N22" s="63" t="s">
+        <v>69</v>
+      </c>
+      <c r="O22" s="62" t="s">
+        <v>69</v>
+      </c>
+      <c r="P22" s="74" t="s">
+        <v>69</v>
+      </c>
+      <c r="Q22" s="62" t="s">
+        <v>69</v>
+      </c>
+      <c r="R22" s="64" t="s">
+        <v>69</v>
+      </c>
+      <c r="S22" s="75"/>
+      <c r="T22" s="57"/>
+      <c r="U22" s="58"/>
+      <c r="V22" s="57"/>
+      <c r="W22" s="58"/>
     </row>
     <row r="23" ht="6" customHeight="1" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A23" s="78"/>
-      <c r="B23" s="24"/>
-      <c r="C23" s="36"/>
+      <c r="A23" s="77"/>
+      <c r="B23" s="23"/>
+      <c r="C23" s="35"/>
       <c r="D23" s="4"/>
       <c r="E23" s="5"/>
-      <c r="F23" s="44"/>
-      <c r="G23" s="37"/>
+      <c r="F23" s="43"/>
+      <c r="G23" s="36"/>
       <c r="H23" s="8"/>
-      <c r="I23" s="67"/>
-      <c r="J23" s="68" t="s">
-        <v>47</v>
-      </c>
-      <c r="K23" s="77"/>
-      <c r="L23" s="67"/>
-      <c r="M23" s="68" t="s">
-        <v>47</v>
-      </c>
-      <c r="N23" s="77"/>
-      <c r="O23" s="69" t="s">
-        <v>48</v>
-      </c>
-      <c r="P23" s="70"/>
-      <c r="Q23" s="69" t="s">
-        <v>48</v>
-      </c>
-      <c r="R23" s="71"/>
-      <c r="S23" s="76"/>
-      <c r="T23" s="72"/>
-      <c r="U23" s="73"/>
-      <c r="V23" s="74"/>
-      <c r="W23" s="73"/>
+      <c r="I23" s="66"/>
+      <c r="J23" s="67" t="s">
+        <v>49</v>
+      </c>
+      <c r="K23" s="76"/>
+      <c r="L23" s="66"/>
+      <c r="M23" s="67" t="s">
+        <v>49</v>
+      </c>
+      <c r="N23" s="76"/>
+      <c r="O23" s="68" t="s">
+        <v>50</v>
+      </c>
+      <c r="P23" s="69"/>
+      <c r="Q23" s="68" t="s">
+        <v>50</v>
+      </c>
+      <c r="R23" s="70"/>
+      <c r="S23" s="75"/>
+      <c r="T23" s="71"/>
+      <c r="U23" s="72"/>
+      <c r="V23" s="73"/>
+      <c r="W23" s="72"/>
     </row>
     <row r="24" ht="10.35" customHeight="1" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A24" s="78"/>
-      <c r="B24" s="24"/>
-      <c r="C24" s="36"/>
+      <c r="A24" s="77"/>
+      <c r="B24" s="23"/>
+      <c r="C24" s="35"/>
       <c r="D24" s="4"/>
       <c r="E24" s="5"/>
-      <c r="F24" s="44"/>
-      <c r="G24" s="37"/>
+      <c r="F24" s="43"/>
+      <c r="G24" s="36"/>
       <c r="H24" s="8"/>
-      <c r="I24" s="63" t="s">
-        <v>67</v>
-      </c>
-      <c r="J24" s="63" t="s">
-        <v>67</v>
-      </c>
-      <c r="K24" s="64" t="s">
-        <v>67</v>
-      </c>
-      <c r="L24" s="63" t="s">
-        <v>67</v>
-      </c>
-      <c r="M24" s="63" t="s">
-        <v>67</v>
-      </c>
-      <c r="N24" s="64" t="s">
-        <v>67</v>
-      </c>
-      <c r="O24" s="63" t="s">
-        <v>67</v>
-      </c>
-      <c r="P24" s="75" t="s">
-        <v>67</v>
-      </c>
-      <c r="Q24" s="63" t="s">
-        <v>67</v>
-      </c>
-      <c r="R24" s="65" t="s">
-        <v>67</v>
-      </c>
-      <c r="S24" s="76"/>
-      <c r="T24" s="58"/>
-      <c r="U24" s="59"/>
-      <c r="V24" s="58"/>
-      <c r="W24" s="59"/>
+      <c r="I24" s="62" t="s">
+        <v>69</v>
+      </c>
+      <c r="J24" s="62" t="s">
+        <v>69</v>
+      </c>
+      <c r="K24" s="63" t="s">
+        <v>69</v>
+      </c>
+      <c r="L24" s="62" t="s">
+        <v>69</v>
+      </c>
+      <c r="M24" s="62" t="s">
+        <v>69</v>
+      </c>
+      <c r="N24" s="63" t="s">
+        <v>69</v>
+      </c>
+      <c r="O24" s="62" t="s">
+        <v>69</v>
+      </c>
+      <c r="P24" s="74" t="s">
+        <v>69</v>
+      </c>
+      <c r="Q24" s="62" t="s">
+        <v>69</v>
+      </c>
+      <c r="R24" s="64" t="s">
+        <v>69</v>
+      </c>
+      <c r="S24" s="75"/>
+      <c r="T24" s="57"/>
+      <c r="U24" s="58"/>
+      <c r="V24" s="57"/>
+      <c r="W24" s="58"/>
     </row>
     <row r="25" ht="6" customHeight="1" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A25" s="78"/>
-      <c r="B25" s="24"/>
-      <c r="C25" s="36"/>
+      <c r="A25" s="77"/>
+      <c r="B25" s="23"/>
+      <c r="C25" s="35"/>
       <c r="D25" s="4"/>
       <c r="E25" s="5"/>
-      <c r="F25" s="44"/>
-      <c r="G25" s="37"/>
+      <c r="F25" s="43"/>
+      <c r="G25" s="36"/>
       <c r="H25" s="8"/>
-      <c r="I25" s="67"/>
-      <c r="J25" s="68" t="s">
-        <v>47</v>
-      </c>
-      <c r="K25" s="77"/>
-      <c r="L25" s="67"/>
-      <c r="M25" s="68" t="s">
-        <v>47</v>
-      </c>
-      <c r="N25" s="77"/>
-      <c r="O25" s="69" t="s">
-        <v>48</v>
-      </c>
-      <c r="P25" s="70"/>
-      <c r="Q25" s="69" t="s">
-        <v>48</v>
-      </c>
-      <c r="R25" s="71"/>
-      <c r="S25" s="76"/>
-      <c r="T25" s="72"/>
-      <c r="U25" s="73"/>
-      <c r="V25" s="74"/>
-      <c r="W25" s="73"/>
+      <c r="I25" s="66"/>
+      <c r="J25" s="67" t="s">
+        <v>49</v>
+      </c>
+      <c r="K25" s="76"/>
+      <c r="L25" s="66"/>
+      <c r="M25" s="67" t="s">
+        <v>49</v>
+      </c>
+      <c r="N25" s="76"/>
+      <c r="O25" s="68" t="s">
+        <v>50</v>
+      </c>
+      <c r="P25" s="69"/>
+      <c r="Q25" s="68" t="s">
+        <v>50</v>
+      </c>
+      <c r="R25" s="70"/>
+      <c r="S25" s="75"/>
+      <c r="T25" s="71"/>
+      <c r="U25" s="72"/>
+      <c r="V25" s="73"/>
+      <c r="W25" s="72"/>
     </row>
     <row r="26" ht="10.35" customHeight="1" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A26" s="78"/>
-      <c r="B26" s="24"/>
-      <c r="C26" s="79">
+      <c r="A26" s="77"/>
+      <c r="B26" s="23"/>
+      <c r="C26" s="78">
         <f>O33</f>
       </c>
       <c r="D26" s="4"/>
       <c r="E26" s="5"/>
-      <c r="F26" s="44"/>
-      <c r="G26" s="37"/>
+      <c r="F26" s="43"/>
+      <c r="G26" s="36"/>
       <c r="H26" s="8"/>
-      <c r="I26" s="63" t="s">
-        <v>67</v>
-      </c>
-      <c r="J26" s="63" t="s">
-        <v>67</v>
-      </c>
-      <c r="K26" s="64" t="s">
-        <v>67</v>
-      </c>
-      <c r="L26" s="63" t="s">
-        <v>67</v>
-      </c>
-      <c r="M26" s="63" t="s">
-        <v>67</v>
-      </c>
-      <c r="N26" s="64" t="s">
-        <v>67</v>
-      </c>
-      <c r="O26" s="63" t="s">
-        <v>67</v>
-      </c>
-      <c r="P26" s="75" t="s">
-        <v>67</v>
-      </c>
-      <c r="Q26" s="63" t="s">
-        <v>67</v>
-      </c>
-      <c r="R26" s="65" t="s">
-        <v>67</v>
-      </c>
-      <c r="S26" s="76"/>
-      <c r="T26" s="58"/>
-      <c r="U26" s="59"/>
-      <c r="V26" s="58"/>
-      <c r="W26" s="59"/>
+      <c r="I26" s="62" t="s">
+        <v>69</v>
+      </c>
+      <c r="J26" s="62" t="s">
+        <v>69</v>
+      </c>
+      <c r="K26" s="63" t="s">
+        <v>69</v>
+      </c>
+      <c r="L26" s="62" t="s">
+        <v>69</v>
+      </c>
+      <c r="M26" s="62" t="s">
+        <v>69</v>
+      </c>
+      <c r="N26" s="63" t="s">
+        <v>69</v>
+      </c>
+      <c r="O26" s="62" t="s">
+        <v>69</v>
+      </c>
+      <c r="P26" s="74" t="s">
+        <v>69</v>
+      </c>
+      <c r="Q26" s="62" t="s">
+        <v>69</v>
+      </c>
+      <c r="R26" s="64" t="s">
+        <v>69</v>
+      </c>
+      <c r="S26" s="75"/>
+      <c r="T26" s="57"/>
+      <c r="U26" s="58"/>
+      <c r="V26" s="57"/>
+      <c r="W26" s="58"/>
     </row>
     <row r="27" ht="6" customHeight="1" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A27" s="78"/>
-      <c r="B27" s="24"/>
-      <c r="C27" s="79"/>
+      <c r="A27" s="77"/>
+      <c r="B27" s="23"/>
+      <c r="C27" s="78"/>
       <c r="D27" s="4"/>
       <c r="E27" s="5"/>
-      <c r="F27" s="44"/>
-      <c r="G27" s="37"/>
+      <c r="F27" s="43"/>
+      <c r="G27" s="36"/>
       <c r="H27" s="8"/>
-      <c r="I27" s="67"/>
-      <c r="J27" s="68" t="s">
-        <v>47</v>
-      </c>
-      <c r="K27" s="77"/>
-      <c r="L27" s="67"/>
-      <c r="M27" s="68" t="s">
-        <v>47</v>
-      </c>
-      <c r="N27" s="77"/>
-      <c r="O27" s="69" t="s">
-        <v>48</v>
-      </c>
-      <c r="P27" s="70"/>
-      <c r="Q27" s="69" t="s">
-        <v>48</v>
-      </c>
-      <c r="R27" s="71"/>
-      <c r="S27" s="76"/>
-      <c r="T27" s="72"/>
-      <c r="U27" s="73"/>
-      <c r="V27" s="74"/>
-      <c r="W27" s="73"/>
+      <c r="I27" s="66"/>
+      <c r="J27" s="67" t="s">
+        <v>49</v>
+      </c>
+      <c r="K27" s="76"/>
+      <c r="L27" s="66"/>
+      <c r="M27" s="67" t="s">
+        <v>49</v>
+      </c>
+      <c r="N27" s="76"/>
+      <c r="O27" s="68" t="s">
+        <v>50</v>
+      </c>
+      <c r="P27" s="69"/>
+      <c r="Q27" s="68" t="s">
+        <v>50</v>
+      </c>
+      <c r="R27" s="70"/>
+      <c r="S27" s="75"/>
+      <c r="T27" s="71"/>
+      <c r="U27" s="72"/>
+      <c r="V27" s="73"/>
+      <c r="W27" s="72"/>
     </row>
     <row r="28" ht="9.6" customHeight="1" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A28" s="78"/>
-      <c r="B28" s="24"/>
-      <c r="C28" s="79"/>
+      <c r="A28" s="77"/>
+      <c r="B28" s="23"/>
+      <c r="C28" s="78"/>
       <c r="D28" s="4"/>
       <c r="E28" s="5"/>
-      <c r="F28" s="44"/>
-      <c r="G28" s="37"/>
+      <c r="F28" s="43"/>
+      <c r="G28" s="36"/>
       <c r="H28" s="8"/>
-      <c r="I28" s="63" t="s">
-        <v>67</v>
-      </c>
-      <c r="J28" s="63" t="s">
-        <v>67</v>
-      </c>
-      <c r="K28" s="64" t="s">
-        <v>67</v>
-      </c>
-      <c r="L28" s="63" t="s">
-        <v>67</v>
-      </c>
-      <c r="M28" s="63" t="s">
-        <v>67</v>
-      </c>
-      <c r="N28" s="64" t="s">
-        <v>67</v>
-      </c>
-      <c r="O28" s="63" t="s">
-        <v>67</v>
-      </c>
-      <c r="P28" s="75" t="s">
-        <v>67</v>
-      </c>
-      <c r="Q28" s="63" t="s">
-        <v>67</v>
-      </c>
-      <c r="R28" s="65" t="s">
-        <v>67</v>
-      </c>
-      <c r="S28" s="76"/>
-      <c r="T28" s="58"/>
-      <c r="U28" s="59"/>
-      <c r="V28" s="58"/>
-      <c r="W28" s="59"/>
+      <c r="I28" s="62" t="s">
+        <v>69</v>
+      </c>
+      <c r="J28" s="62" t="s">
+        <v>69</v>
+      </c>
+      <c r="K28" s="63" t="s">
+        <v>69</v>
+      </c>
+      <c r="L28" s="62" t="s">
+        <v>69</v>
+      </c>
+      <c r="M28" s="62" t="s">
+        <v>69</v>
+      </c>
+      <c r="N28" s="63" t="s">
+        <v>69</v>
+      </c>
+      <c r="O28" s="62" t="s">
+        <v>69</v>
+      </c>
+      <c r="P28" s="74" t="s">
+        <v>69</v>
+      </c>
+      <c r="Q28" s="62" t="s">
+        <v>69</v>
+      </c>
+      <c r="R28" s="64" t="s">
+        <v>69</v>
+      </c>
+      <c r="S28" s="75"/>
+      <c r="T28" s="57"/>
+      <c r="U28" s="58"/>
+      <c r="V28" s="57"/>
+      <c r="W28" s="58"/>
     </row>
     <row r="29" ht="6" customHeight="1" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A29" s="78"/>
-      <c r="B29" s="24"/>
-      <c r="C29" s="79"/>
+      <c r="A29" s="77"/>
+      <c r="B29" s="23"/>
+      <c r="C29" s="78"/>
       <c r="D29" s="4"/>
       <c r="E29" s="5"/>
-      <c r="F29" s="44"/>
-      <c r="G29" s="37"/>
+      <c r="F29" s="43"/>
+      <c r="G29" s="36"/>
       <c r="H29" s="8"/>
-      <c r="I29" s="67"/>
-      <c r="J29" s="68" t="s">
-        <v>47</v>
-      </c>
-      <c r="K29" s="77"/>
-      <c r="L29" s="67"/>
-      <c r="M29" s="68" t="s">
-        <v>47</v>
-      </c>
-      <c r="N29" s="77"/>
-      <c r="O29" s="69" t="s">
-        <v>48</v>
-      </c>
-      <c r="P29" s="70"/>
-      <c r="Q29" s="69" t="s">
-        <v>48</v>
-      </c>
-      <c r="R29" s="71"/>
-      <c r="S29" s="76"/>
-      <c r="T29" s="72"/>
-      <c r="U29" s="73"/>
-      <c r="V29" s="74"/>
-      <c r="W29" s="73"/>
+      <c r="I29" s="66"/>
+      <c r="J29" s="67" t="s">
+        <v>49</v>
+      </c>
+      <c r="K29" s="76"/>
+      <c r="L29" s="66"/>
+      <c r="M29" s="67" t="s">
+        <v>49</v>
+      </c>
+      <c r="N29" s="76"/>
+      <c r="O29" s="68" t="s">
+        <v>50</v>
+      </c>
+      <c r="P29" s="69"/>
+      <c r="Q29" s="68" t="s">
+        <v>50</v>
+      </c>
+      <c r="R29" s="70"/>
+      <c r="S29" s="75"/>
+      <c r="T29" s="71"/>
+      <c r="U29" s="72"/>
+      <c r="V29" s="73"/>
+      <c r="W29" s="72"/>
     </row>
     <row r="30" ht="9.6" customHeight="1" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A30" s="78"/>
-      <c r="B30" s="24"/>
-      <c r="C30" s="79"/>
+      <c r="A30" s="77"/>
+      <c r="B30" s="23"/>
+      <c r="C30" s="78"/>
       <c r="D30" s="4"/>
       <c r="E30" s="5"/>
-      <c r="F30" s="44"/>
-      <c r="G30" s="37"/>
+      <c r="F30" s="43"/>
+      <c r="G30" s="36"/>
       <c r="H30" s="8"/>
-      <c r="I30" s="63" t="s">
-        <v>67</v>
-      </c>
-      <c r="J30" s="63" t="s">
-        <v>67</v>
-      </c>
-      <c r="K30" s="64" t="s">
-        <v>67</v>
-      </c>
-      <c r="L30" s="63" t="s">
-        <v>67</v>
-      </c>
-      <c r="M30" s="63" t="s">
-        <v>67</v>
-      </c>
-      <c r="N30" s="64" t="s">
-        <v>67</v>
-      </c>
-      <c r="O30" s="63" t="s">
-        <v>67</v>
-      </c>
-      <c r="P30" s="75" t="s">
-        <v>67</v>
-      </c>
-      <c r="Q30" s="63" t="s">
-        <v>67</v>
-      </c>
-      <c r="R30" s="65" t="s">
-        <v>67</v>
-      </c>
-      <c r="S30" s="76"/>
-      <c r="T30" s="58"/>
-      <c r="U30" s="59"/>
-      <c r="V30" s="58"/>
-      <c r="W30" s="59"/>
+      <c r="I30" s="62" t="s">
+        <v>69</v>
+      </c>
+      <c r="J30" s="62" t="s">
+        <v>69</v>
+      </c>
+      <c r="K30" s="63" t="s">
+        <v>69</v>
+      </c>
+      <c r="L30" s="62" t="s">
+        <v>69</v>
+      </c>
+      <c r="M30" s="62" t="s">
+        <v>69</v>
+      </c>
+      <c r="N30" s="63" t="s">
+        <v>69</v>
+      </c>
+      <c r="O30" s="62" t="s">
+        <v>69</v>
+      </c>
+      <c r="P30" s="74" t="s">
+        <v>69</v>
+      </c>
+      <c r="Q30" s="62" t="s">
+        <v>69</v>
+      </c>
+      <c r="R30" s="64" t="s">
+        <v>69</v>
+      </c>
+      <c r="S30" s="75"/>
+      <c r="T30" s="57"/>
+      <c r="U30" s="58"/>
+      <c r="V30" s="57"/>
+      <c r="W30" s="58"/>
     </row>
     <row r="31" ht="6" customHeight="1" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A31" s="78"/>
-      <c r="B31" s="24"/>
-      <c r="C31" s="79"/>
+      <c r="A31" s="77"/>
+      <c r="B31" s="23"/>
+      <c r="C31" s="78"/>
       <c r="D31" s="4"/>
       <c r="E31" s="5"/>
-      <c r="F31" s="80"/>
-      <c r="G31" s="37"/>
+      <c r="F31" s="79"/>
+      <c r="G31" s="36"/>
       <c r="H31" s="8"/>
-      <c r="I31" s="67"/>
-      <c r="J31" s="68" t="s">
-        <v>47</v>
+      <c r="I31" s="66"/>
+      <c r="J31" s="67" t="s">
+        <v>49</v>
       </c>
       <c r="K31" s="17"/>
-      <c r="L31" s="67"/>
-      <c r="M31" s="68" t="s">
-        <v>47</v>
+      <c r="L31" s="66"/>
+      <c r="M31" s="67" t="s">
+        <v>49</v>
       </c>
       <c r="N31" s="17"/>
-      <c r="O31" s="69" t="s">
-        <v>48</v>
-      </c>
-      <c r="P31" s="70"/>
-      <c r="Q31" s="69" t="s">
-        <v>48</v>
-      </c>
-      <c r="R31" s="71"/>
-      <c r="T31" s="72"/>
-      <c r="U31" s="73"/>
-      <c r="V31" s="74"/>
-      <c r="W31" s="73"/>
+      <c r="O31" s="68" t="s">
+        <v>50</v>
+      </c>
+      <c r="P31" s="69"/>
+      <c r="Q31" s="68" t="s">
+        <v>50</v>
+      </c>
+      <c r="R31" s="70"/>
+      <c r="T31" s="71"/>
+      <c r="U31" s="72"/>
+      <c r="V31" s="73"/>
+      <c r="W31" s="72"/>
     </row>
     <row r="32" ht="25.7" customHeight="1" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A32" s="78"/>
-      <c r="B32" s="24"/>
-      <c r="C32" s="79"/>
+      <c r="A32" s="77"/>
+      <c r="B32" s="23"/>
+      <c r="C32" s="78"/>
       <c r="D32" s="4"/>
       <c r="E32" s="5"/>
-      <c r="F32" s="81"/>
-      <c r="G32" s="37"/>
+      <c r="F32" s="80"/>
+      <c r="G32" s="36"/>
       <c r="H32" s="8"/>
-      <c r="I32" s="82" t="s">
-        <v>68</v>
-      </c>
-      <c r="J32" s="82" t="s">
-        <v>69</v>
-      </c>
-      <c r="K32" s="82" t="s">
+      <c r="I32" s="81" t="s">
         <v>70</v>
       </c>
-      <c r="L32" s="82" t="s">
+      <c r="J32" s="81" t="s">
         <v>71</v>
       </c>
-      <c r="M32" s="83" t="s">
+      <c r="K32" s="81" t="s">
         <v>72</v>
       </c>
-      <c r="N32" s="83" t="s">
+      <c r="L32" s="81" t="s">
         <v>73</v>
       </c>
-      <c r="O32" s="83" t="s">
+      <c r="M32" s="82" t="s">
         <v>74</v>
       </c>
-      <c r="P32" s="83" t="s">
+      <c r="N32" s="82" t="s">
         <v>75</v>
       </c>
-      <c r="Q32" s="83" t="s">
+      <c r="O32" s="82" t="s">
         <v>76</v>
       </c>
-      <c r="R32" s="83" t="s">
+      <c r="P32" s="82" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="33" ht="25.7" customHeight="1" spans="1:19" s="50" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="78"/>
-      <c r="B33" s="84" t="str">
+      <c r="Q32" s="82" t="s">
+        <v>78</v>
+      </c>
+      <c r="R32" s="82" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="33" ht="25.7" customHeight="1" spans="1:19" s="49" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="77"/>
+      <c r="B33" s="83" t="str">
         <f>L33</f>
         <v>ЗІЛ-131</v>
       </c>
-      <c r="C33" s="79"/>
+      <c r="C33" s="78"/>
       <c r="D33" s="4"/>
       <c r="E33" s="5"/>
-      <c r="F33" s="81"/>
-      <c r="G33" s="37"/>
-      <c r="H33" s="85"/>
-      <c r="I33" s="86" t="str">
+      <c r="F33" s="80"/>
+      <c r="G33" s="36"/>
+      <c r="H33" s="84"/>
+      <c r="I33" s="85" t="str">
         <f>Number</f>
         <v>123456</v>
       </c>
-      <c r="J33" s="87" t="s">
-        <v>3</v>
-      </c>
-      <c r="K33" s="88" t="s">
-        <v>78</v>
-      </c>
-      <c r="L33" s="89" t="s">
-        <v>79</v>
-      </c>
-      <c r="M33" s="86" t="s">
+      <c r="J33" s="86" t="s">
         <v>80</v>
       </c>
-      <c r="N33" s="89"/>
-      <c r="O33" s="86">
+      <c r="K33" s="87" t="s">
+        <v>81</v>
+      </c>
+      <c r="L33" s="88" t="s">
+        <v>82</v>
+      </c>
+      <c r="M33" s="85" t="s">
+        <v>83</v>
+      </c>
+      <c r="N33" s="88"/>
+      <c r="O33" s="85">
         <f>IFERROR(INDEX(#REF!,MATCH('Ш Лист 1'!N33,#REF!,0)),"")</f>
       </c>
-      <c r="P33" s="86" t="e">
-        <f>INDEX(#REF!,MATCH('Ш Лист 1'!L33,#REF!,0))</f>
-        <v>#REF!</v>
-      </c>
-      <c r="Q33" s="86"/>
-      <c r="R33" s="86"/>
-      <c r="S33" s="90"/>
+      <c r="P33" s="85" t="s">
+        <v>84</v>
+      </c>
+      <c r="Q33" s="85"/>
+      <c r="R33" s="85"/>
+      <c r="S33" s="89"/>
     </row>
     <row r="34" ht="12" customHeight="1" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A34" s="78"/>
-      <c r="B34" s="84"/>
-      <c r="C34" s="79"/>
+      <c r="A34" s="77"/>
+      <c r="B34" s="83"/>
+      <c r="C34" s="78"/>
       <c r="D34" s="4"/>
       <c r="E34" s="5"/>
-      <c r="F34" s="81"/>
-      <c r="G34" s="37"/>
+      <c r="F34" s="80"/>
+      <c r="G34" s="36"/>
       <c r="H34" s="8"/>
-      <c r="I34" s="91" t="s">
-        <v>81</v>
-      </c>
-      <c r="J34" s="92"/>
-      <c r="K34" s="92"/>
-      <c r="L34" s="92"/>
-      <c r="M34" s="92"/>
-      <c r="N34" s="92"/>
-      <c r="O34" s="92"/>
-      <c r="P34" s="92"/>
-      <c r="Q34" s="92"/>
-      <c r="R34" s="93"/>
-      <c r="S34" s="90"/>
+      <c r="I34" s="90" t="s">
+        <v>85</v>
+      </c>
+      <c r="J34" s="91"/>
+      <c r="K34" s="91"/>
+      <c r="L34" s="91"/>
+      <c r="M34" s="91"/>
+      <c r="N34" s="91"/>
+      <c r="O34" s="91"/>
+      <c r="P34" s="91"/>
+      <c r="Q34" s="91"/>
+      <c r="R34" s="92"/>
+      <c r="S34" s="89"/>
     </row>
     <row r="35" ht="34.7" customHeight="1" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A35" s="78"/>
-      <c r="B35" s="84"/>
-      <c r="C35" s="24" t="s">
-        <v>82</v>
+      <c r="A35" s="77"/>
+      <c r="B35" s="83"/>
+      <c r="C35" s="23" t="s">
+        <v>86</v>
       </c>
       <c r="D35" s="4"/>
       <c r="E35" s="5"/>
-      <c r="F35" s="24" t="s">
-        <v>83</v>
-      </c>
-      <c r="G35" s="37"/>
+      <c r="F35" s="23" t="s">
+        <v>87</v>
+      </c>
+      <c r="G35" s="36"/>
       <c r="H35" s="8"/>
-      <c r="I35" s="82" t="s">
-        <v>84</v>
-      </c>
-      <c r="J35" s="82" t="s">
-        <v>85</v>
-      </c>
-      <c r="K35" s="82" t="s">
-        <v>86</v>
-      </c>
-      <c r="L35" s="94" t="s">
-        <v>87</v>
-      </c>
-      <c r="M35" s="95"/>
-      <c r="N35" s="83" t="s">
+      <c r="I35" s="81" t="s">
         <v>88</v>
       </c>
-      <c r="O35" s="83" t="s">
+      <c r="J35" s="81" t="s">
         <v>89</v>
       </c>
-      <c r="P35" s="83" t="s">
+      <c r="K35" s="81" t="s">
         <v>90</v>
       </c>
-      <c r="Q35" s="83" t="s">
+      <c r="L35" s="93" t="s">
         <v>91</v>
       </c>
-      <c r="R35" s="83" t="s">
+      <c r="M35" s="94"/>
+      <c r="N35" s="82" t="s">
         <v>92</v>
       </c>
+      <c r="O35" s="82" t="s">
+        <v>93</v>
+      </c>
+      <c r="P35" s="82" t="s">
+        <v>94</v>
+      </c>
+      <c r="Q35" s="82" t="s">
+        <v>95</v>
+      </c>
+      <c r="R35" s="82" t="s">
+        <v>96</v>
+      </c>
     </row>
     <row r="36" ht="10.7" customHeight="1" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A36" s="43"/>
-      <c r="B36" s="84"/>
-      <c r="C36" s="24"/>
-      <c r="D36" s="24" t="s">
-        <v>93</v>
-      </c>
-      <c r="E36" s="24" t="s">
-        <v>94</v>
-      </c>
-      <c r="F36" s="24"/>
-      <c r="G36" s="96"/>
+      <c r="A36" s="42"/>
+      <c r="B36" s="83"/>
+      <c r="C36" s="23"/>
+      <c r="D36" s="23" t="s">
+        <v>97</v>
+      </c>
+      <c r="E36" s="23" t="s">
+        <v>98</v>
+      </c>
+      <c r="F36" s="23"/>
+      <c r="G36" s="95"/>
       <c r="H36" s="8"/>
-      <c r="I36" s="97" t="s">
-        <v>95</v>
-      </c>
-      <c r="J36" s="98" t="s">
-        <v>96</v>
-      </c>
-      <c r="K36" s="98">
+      <c r="I36" s="96" t="s">
+        <v>99</v>
+      </c>
+      <c r="J36" s="97">
+        <v>24</v>
+      </c>
+      <c r="K36" s="97">
         <v>10</v>
       </c>
-      <c r="L36" s="99" t="s">
-        <v>41</v>
-      </c>
-      <c r="M36" s="98">
+      <c r="L36" s="98" t="s">
+        <v>43</v>
+      </c>
+      <c r="M36" s="97">
         <v>5</v>
       </c>
-      <c r="N36" s="100">
+      <c r="N36" s="99">
         <v>5</v>
       </c>
-      <c r="O36" s="100">
+      <c r="O36" s="99">
         <v>5</v>
       </c>
-      <c r="P36" s="100">
+      <c r="P36" s="99">
         <v>5</v>
       </c>
-      <c r="Q36" s="100">
+      <c r="Q36" s="99">
         <v>0</v>
       </c>
-      <c r="R36" s="100"/>
-      <c r="S36" s="29"/>
+      <c r="R36" s="99"/>
+      <c r="S36" s="28"/>
     </row>
     <row r="37" ht="10.7" customHeight="1" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A37" s="43"/>
-      <c r="B37" s="84"/>
-      <c r="C37" s="24"/>
-      <c r="D37" s="24"/>
-      <c r="E37" s="24"/>
-      <c r="F37" s="24"/>
-      <c r="G37" s="96"/>
+      <c r="A37" s="42"/>
+      <c r="B37" s="83"/>
+      <c r="C37" s="23"/>
+      <c r="D37" s="23"/>
+      <c r="E37" s="23"/>
+      <c r="F37" s="23"/>
+      <c r="G37" s="95"/>
       <c r="H37" s="8"/>
-      <c r="I37" s="97"/>
-      <c r="J37" s="98"/>
-      <c r="K37" s="98"/>
-      <c r="L37" s="99"/>
-      <c r="M37" s="98"/>
-      <c r="N37" s="100"/>
-      <c r="O37" s="100"/>
-      <c r="P37" s="100"/>
-      <c r="Q37" s="100"/>
-      <c r="R37" s="100"/>
-      <c r="S37" s="29"/>
+      <c r="I37" s="96" t="s">
+        <v>69</v>
+      </c>
+      <c r="J37" s="97" t="s">
+        <v>69</v>
+      </c>
+      <c r="K37" s="97" t="s">
+        <v>69</v>
+      </c>
+      <c r="L37" s="98" t="s">
+        <v>69</v>
+      </c>
+      <c r="M37" s="97" t="s">
+        <v>69</v>
+      </c>
+      <c r="N37" s="99" t="s">
+        <v>69</v>
+      </c>
+      <c r="O37" s="99" t="s">
+        <v>69</v>
+      </c>
+      <c r="P37" s="99" t="s">
+        <v>69</v>
+      </c>
+      <c r="Q37" s="99" t="s">
+        <v>69</v>
+      </c>
+      <c r="R37" s="99"/>
+      <c r="S37" s="28"/>
     </row>
     <row r="38" ht="10.7" customHeight="1" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A38" s="43"/>
-      <c r="B38" s="84"/>
-      <c r="C38" s="24"/>
-      <c r="D38" s="24"/>
-      <c r="E38" s="24"/>
-      <c r="F38" s="24"/>
-      <c r="G38" s="96"/>
+      <c r="A38" s="42"/>
+      <c r="B38" s="83"/>
+      <c r="C38" s="23"/>
+      <c r="D38" s="23"/>
+      <c r="E38" s="23"/>
+      <c r="F38" s="23"/>
+      <c r="G38" s="95"/>
       <c r="H38" s="8"/>
-      <c r="I38" s="97">
-        <f>IF(M38,'Ш Лист 2'!$A$18,"")</f>
-      </c>
-      <c r="J38" s="98"/>
-      <c r="K38" s="98"/>
-      <c r="L38" s="99"/>
-      <c r="M38" s="98"/>
-      <c r="N38" s="100"/>
-      <c r="O38" s="100"/>
-      <c r="P38" s="100"/>
-      <c r="Q38" s="100">
-        <f t="shared" ref="Q38:Q42" si="0">IF(O38&lt;P38,P38-O38,"")</f>
-      </c>
-      <c r="R38" s="100">
-        <f t="shared" ref="R38:R42" si="1">IF(O38&gt;P38,O38-P38,"")</f>
-      </c>
-      <c r="S38" s="29"/>
+      <c r="I38" s="96" t="s">
+        <v>69</v>
+      </c>
+      <c r="J38" s="97" t="s">
+        <v>69</v>
+      </c>
+      <c r="K38" s="97" t="s">
+        <v>69</v>
+      </c>
+      <c r="L38" s="98" t="s">
+        <v>69</v>
+      </c>
+      <c r="M38" s="97" t="s">
+        <v>69</v>
+      </c>
+      <c r="N38" s="99" t="s">
+        <v>69</v>
+      </c>
+      <c r="O38" s="99" t="s">
+        <v>69</v>
+      </c>
+      <c r="P38" s="99" t="s">
+        <v>69</v>
+      </c>
+      <c r="Q38" s="99" t="s">
+        <v>69</v>
+      </c>
+      <c r="R38" s="99">
+        <f t="shared" ref="R38:R42" si="0">IF(O38&gt;P38,O38-P38,"")</f>
+      </c>
+      <c r="S38" s="28"/>
     </row>
     <row r="39" ht="10.7" customHeight="1" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A39" s="43"/>
-      <c r="B39" s="24" t="s">
-        <v>97</v>
-      </c>
-      <c r="C39" s="24"/>
-      <c r="D39" s="24"/>
-      <c r="E39" s="24"/>
-      <c r="F39" s="24"/>
-      <c r="G39" s="96"/>
+      <c r="A39" s="42"/>
+      <c r="B39" s="23" t="s">
+        <v>100</v>
+      </c>
+      <c r="C39" s="23"/>
+      <c r="D39" s="23"/>
+      <c r="E39" s="23"/>
+      <c r="F39" s="23"/>
+      <c r="G39" s="95"/>
       <c r="H39" s="8"/>
-      <c r="I39" s="97">
-        <f>IF(M39,'Ш Лист 2'!$A$18,"")</f>
-      </c>
-      <c r="J39" s="98"/>
-      <c r="K39" s="98"/>
-      <c r="L39" s="99"/>
-      <c r="M39" s="98"/>
-      <c r="N39" s="100"/>
-      <c r="O39" s="100"/>
-      <c r="P39" s="100"/>
-      <c r="Q39" s="100">
+      <c r="I39" s="96" t="s">
+        <v>69</v>
+      </c>
+      <c r="J39" s="97" t="s">
+        <v>69</v>
+      </c>
+      <c r="K39" s="97" t="s">
+        <v>69</v>
+      </c>
+      <c r="L39" s="98" t="s">
+        <v>69</v>
+      </c>
+      <c r="M39" s="97" t="s">
+        <v>69</v>
+      </c>
+      <c r="N39" s="99" t="s">
+        <v>69</v>
+      </c>
+      <c r="O39" s="99" t="s">
+        <v>69</v>
+      </c>
+      <c r="P39" s="99" t="s">
+        <v>69</v>
+      </c>
+      <c r="Q39" s="99" t="s">
+        <v>69</v>
+      </c>
+      <c r="R39" s="99">
         <f t="shared" si="0"/>
       </c>
-      <c r="R39" s="100">
+    </row>
+    <row r="40" ht="10.7" customHeight="1" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A40" s="42"/>
+      <c r="B40" s="23"/>
+      <c r="C40" s="23"/>
+      <c r="D40" s="23"/>
+      <c r="E40" s="23"/>
+      <c r="F40" s="23"/>
+      <c r="G40" s="95"/>
+      <c r="H40" s="8"/>
+      <c r="I40" s="96" t="s">
+        <v>69</v>
+      </c>
+      <c r="J40" s="97" t="s">
+        <v>69</v>
+      </c>
+      <c r="K40" s="97" t="s">
+        <v>69</v>
+      </c>
+      <c r="L40" s="98" t="s">
+        <v>69</v>
+      </c>
+      <c r="M40" s="97" t="s">
+        <v>69</v>
+      </c>
+      <c r="N40" s="99" t="s">
+        <v>69</v>
+      </c>
+      <c r="O40" s="99" t="s">
+        <v>69</v>
+      </c>
+      <c r="P40" s="99" t="s">
+        <v>69</v>
+      </c>
+      <c r="Q40" s="99" t="s">
+        <v>69</v>
+      </c>
+      <c r="R40" s="99">
+        <f t="shared" si="0"/>
+      </c>
+      <c r="S40" s="28"/>
+    </row>
+    <row r="41" ht="10.7" customHeight="1" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A41" s="42"/>
+      <c r="B41" s="23"/>
+      <c r="C41" s="23"/>
+      <c r="D41" s="23"/>
+      <c r="E41" s="23"/>
+      <c r="F41" s="23"/>
+      <c r="G41" s="95"/>
+      <c r="H41" s="8"/>
+      <c r="I41" s="96" t="s">
+        <v>69</v>
+      </c>
+      <c r="J41" s="100" t="s">
+        <v>69</v>
+      </c>
+      <c r="K41" s="100" t="s">
+        <v>69</v>
+      </c>
+      <c r="L41" s="101" t="s">
+        <v>69</v>
+      </c>
+      <c r="M41" s="100" t="s">
+        <v>69</v>
+      </c>
+      <c r="N41" s="99" t="s">
+        <v>69</v>
+      </c>
+      <c r="O41" s="99" t="s">
+        <v>69</v>
+      </c>
+      <c r="P41" s="99" t="s">
+        <v>69</v>
+      </c>
+      <c r="Q41" s="99" t="s">
+        <v>69</v>
+      </c>
+      <c r="R41" s="99">
+        <f t="shared" si="0"/>
+      </c>
+      <c r="S41" s="28"/>
+    </row>
+    <row r="42" ht="10.7" customHeight="1" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A42" s="42"/>
+      <c r="B42" s="23"/>
+      <c r="C42" s="23"/>
+      <c r="D42" s="23"/>
+      <c r="E42" s="23"/>
+      <c r="F42" s="23"/>
+      <c r="G42" s="95"/>
+      <c r="H42" s="8"/>
+      <c r="I42" s="96" t="s">
+        <v>69</v>
+      </c>
+      <c r="J42" s="100" t="s">
+        <v>69</v>
+      </c>
+      <c r="K42" s="100" t="s">
+        <v>69</v>
+      </c>
+      <c r="L42" s="101" t="s">
+        <v>69</v>
+      </c>
+      <c r="M42" s="100" t="s">
+        <v>69</v>
+      </c>
+      <c r="N42" s="99" t="s">
+        <v>69</v>
+      </c>
+      <c r="O42" s="99" t="s">
+        <v>69</v>
+      </c>
+      <c r="P42" s="99" t="s">
+        <v>69</v>
+      </c>
+      <c r="Q42" s="99" t="s">
+        <v>69</v>
+      </c>
+      <c r="R42" s="99">
+        <f t="shared" si="0"/>
+      </c>
+      <c r="S42" s="28"/>
+    </row>
+    <row r="43" ht="10.7" customHeight="1" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A43" s="42"/>
+      <c r="B43" s="23"/>
+      <c r="C43" s="23"/>
+      <c r="D43" s="23"/>
+      <c r="E43" s="23"/>
+      <c r="F43" s="23"/>
+      <c r="G43" s="95"/>
+      <c r="H43" s="8"/>
+      <c r="I43" s="96" t="s">
+        <v>69</v>
+      </c>
+      <c r="J43" s="100" t="s">
+        <v>69</v>
+      </c>
+      <c r="K43" s="100" t="s">
+        <v>69</v>
+      </c>
+      <c r="L43" s="101" t="s">
+        <v>69</v>
+      </c>
+      <c r="M43" s="100" t="s">
+        <v>69</v>
+      </c>
+      <c r="N43" s="99" t="s">
+        <v>69</v>
+      </c>
+      <c r="O43" s="99" t="s">
+        <v>69</v>
+      </c>
+      <c r="P43" s="99" t="s">
+        <v>69</v>
+      </c>
+      <c r="Q43" s="99" t="s">
+        <v>69</v>
+      </c>
+      <c r="R43" s="99">
+        <f t="shared" ref="R43:R44" si="1">IF(O43&gt;P43,O43-P43,"")</f>
+      </c>
+      <c r="S43" s="28"/>
+    </row>
+    <row r="44" ht="10.7" customHeight="1" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B44" s="23"/>
+      <c r="C44" s="23"/>
+      <c r="D44" s="23"/>
+      <c r="E44" s="23"/>
+      <c r="F44" s="23"/>
+      <c r="G44" s="95"/>
+      <c r="H44" s="8"/>
+      <c r="I44" s="96" t="s">
+        <v>69</v>
+      </c>
+      <c r="J44" s="100" t="s">
+        <v>69</v>
+      </c>
+      <c r="K44" s="100" t="s">
+        <v>69</v>
+      </c>
+      <c r="L44" s="101" t="s">
+        <v>69</v>
+      </c>
+      <c r="M44" s="100" t="s">
+        <v>69</v>
+      </c>
+      <c r="N44" s="99" t="s">
+        <v>69</v>
+      </c>
+      <c r="O44" s="99" t="s">
+        <v>69</v>
+      </c>
+      <c r="P44" s="99" t="s">
+        <v>69</v>
+      </c>
+      <c r="Q44" s="99" t="s">
+        <v>69</v>
+      </c>
+      <c r="R44" s="99">
         <f t="shared" si="1"/>
       </c>
-    </row>
-    <row r="40" ht="10.7" customHeight="1" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A40" s="43"/>
-      <c r="B40" s="24"/>
-      <c r="C40" s="24"/>
-      <c r="D40" s="24"/>
-      <c r="E40" s="24"/>
-      <c r="F40" s="24"/>
-      <c r="G40" s="96"/>
-      <c r="H40" s="8"/>
-      <c r="I40" s="97">
-        <f>IF(M40,'Ш Лист 2'!$A$18,"")</f>
-      </c>
-      <c r="J40" s="98"/>
-      <c r="K40" s="98"/>
-      <c r="L40" s="99"/>
-      <c r="M40" s="98"/>
-      <c r="N40" s="100"/>
-      <c r="O40" s="100"/>
-      <c r="P40" s="100"/>
-      <c r="Q40" s="100">
-        <f t="shared" si="0"/>
-      </c>
-      <c r="R40" s="100">
-        <f t="shared" si="1"/>
-      </c>
-      <c r="S40" s="29"/>
-    </row>
-    <row r="41" ht="10.7" customHeight="1" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A41" s="43"/>
-      <c r="B41" s="24"/>
-      <c r="C41" s="24"/>
-      <c r="D41" s="24"/>
-      <c r="E41" s="24"/>
-      <c r="F41" s="24"/>
-      <c r="G41" s="96"/>
-      <c r="H41" s="8"/>
-      <c r="I41" s="97">
-        <f>IF(M41,'Ш Лист 2'!$A$20,"")</f>
-      </c>
-      <c r="J41" s="101"/>
-      <c r="K41" s="101"/>
-      <c r="L41" s="102"/>
-      <c r="M41" s="101"/>
-      <c r="N41" s="100">
-        <f>IFERROR(SUMIFS($M$36:$M$44,$I$36:$I$44,I41)+SUMIFS($K$36:$K$44,$I$36:$I$44,I41)-O41,"")</f>
-      </c>
-      <c r="O41" s="100">
-        <f>'Ш Лист 2'!F20</f>
-      </c>
-      <c r="P41" s="100">
-        <f t="shared" ref="P41" si="2">O41</f>
-      </c>
-      <c r="Q41" s="100">
-        <f t="shared" si="0"/>
-      </c>
-      <c r="R41" s="100">
-        <f t="shared" si="1"/>
-      </c>
-      <c r="S41" s="29"/>
-    </row>
-    <row r="42" ht="10.7" customHeight="1" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A42" s="43"/>
-      <c r="B42" s="24"/>
-      <c r="C42" s="24"/>
-      <c r="D42" s="24"/>
-      <c r="E42" s="24"/>
-      <c r="F42" s="24"/>
-      <c r="G42" s="96"/>
-      <c r="H42" s="8"/>
-      <c r="I42" s="97">
-        <f>IF(M42,'Ш Лист 2'!$A$20,"")</f>
-      </c>
-      <c r="J42" s="101"/>
-      <c r="K42" s="101"/>
-      <c r="L42" s="102"/>
-      <c r="M42" s="101"/>
-      <c r="N42" s="100"/>
-      <c r="O42" s="100"/>
-      <c r="P42" s="100"/>
-      <c r="Q42" s="100">
-        <f t="shared" si="0"/>
-      </c>
-      <c r="R42" s="100">
-        <f t="shared" si="1"/>
-      </c>
-      <c r="S42" s="29"/>
-    </row>
-    <row r="43" ht="10.7" customHeight="1" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A43" s="43"/>
-      <c r="B43" s="24"/>
-      <c r="C43" s="24"/>
-      <c r="D43" s="24"/>
-      <c r="E43" s="24"/>
-      <c r="F43" s="24"/>
-      <c r="G43" s="96"/>
-      <c r="H43" s="8"/>
-      <c r="I43" s="97">
-        <f>IF(M43,'Ш Лист 2'!$A$20,"")</f>
-      </c>
-      <c r="J43" s="101"/>
-      <c r="K43" s="101"/>
-      <c r="L43" s="102"/>
-      <c r="M43" s="101"/>
-      <c r="N43" s="100"/>
-      <c r="O43" s="100"/>
-      <c r="P43" s="100"/>
-      <c r="Q43" s="100">
-        <f t="shared" ref="Q43:Q44" si="3">IF(O43&lt;P43,P43-O43,"")</f>
-      </c>
-      <c r="R43" s="100">
-        <f t="shared" ref="R43:R44" si="4">IF(O43&gt;P43,O43-P43,"")</f>
-      </c>
-      <c r="S43" s="29"/>
-    </row>
-    <row r="44" ht="10.7" customHeight="1" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B44" s="24"/>
-      <c r="C44" s="24"/>
-      <c r="D44" s="24"/>
-      <c r="E44" s="24"/>
-      <c r="F44" s="24"/>
-      <c r="G44" s="96"/>
-      <c r="H44" s="8"/>
-      <c r="I44" s="97">
-        <f>IF(M44,'Ш Лист 2'!$A$20,"")</f>
-      </c>
-      <c r="J44" s="101"/>
-      <c r="K44" s="101"/>
-      <c r="L44" s="102"/>
-      <c r="M44" s="101"/>
-      <c r="N44" s="100"/>
-      <c r="O44" s="100"/>
-      <c r="P44" s="100"/>
-      <c r="Q44" s="100">
-        <f t="shared" si="3"/>
-      </c>
-      <c r="R44" s="100">
-        <f t="shared" si="4"/>
-      </c>
-      <c r="S44" s="29"/>
+      <c r="S44" s="28"/>
     </row>
   </sheetData>
   <autoFilter ref="I1:R44"/>
@@ -4112,547 +4250,559 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A1" s="103" t="s">
-        <v>98</v>
-      </c>
-      <c r="B1" s="103"/>
-      <c r="C1" s="103"/>
-      <c r="D1" s="103"/>
-      <c r="E1" s="103"/>
-      <c r="F1" s="103"/>
-      <c r="G1" s="103"/>
-      <c r="H1" s="103"/>
-      <c r="I1" s="103"/>
-      <c r="J1" s="103"/>
-      <c r="K1" s="103"/>
-      <c r="L1" s="103"/>
-      <c r="M1" s="103"/>
-      <c r="N1" s="103"/>
+      <c r="A1" s="102" t="s">
+        <v>101</v>
+      </c>
+      <c r="B1" s="102"/>
+      <c r="C1" s="102"/>
+      <c r="D1" s="102"/>
+      <c r="E1" s="102"/>
+      <c r="F1" s="102"/>
+      <c r="G1" s="102"/>
+      <c r="H1" s="102"/>
+      <c r="I1" s="102"/>
+      <c r="J1" s="102"/>
+      <c r="K1" s="102"/>
+      <c r="L1" s="102"/>
+      <c r="M1" s="102"/>
+      <c r="N1" s="102"/>
     </row>
     <row r="2" ht="15.75" customHeight="1" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A2" s="104" t="s">
-        <v>99</v>
-      </c>
-      <c r="B2" s="105" t="s">
-        <v>100</v>
-      </c>
-      <c r="C2" s="105"/>
-      <c r="D2" s="106" t="s">
-        <v>101</v>
-      </c>
-      <c r="E2" s="106"/>
-      <c r="F2" s="106"/>
-      <c r="G2" s="106"/>
-      <c r="H2" s="106"/>
-      <c r="I2" s="105" t="s">
+      <c r="A2" s="103" t="s">
         <v>102</v>
       </c>
-      <c r="J2" s="105"/>
-      <c r="K2" s="105"/>
-      <c r="L2" s="105" t="s">
+      <c r="B2" s="104" t="s">
         <v>103</v>
       </c>
-      <c r="M2" s="105"/>
-      <c r="N2" s="105" t="s">
+      <c r="C2" s="104"/>
+      <c r="D2" s="105" t="s">
         <v>104</v>
       </c>
+      <c r="E2" s="105"/>
+      <c r="F2" s="105"/>
+      <c r="G2" s="105"/>
+      <c r="H2" s="105"/>
+      <c r="I2" s="104" t="s">
+        <v>105</v>
+      </c>
+      <c r="J2" s="104"/>
+      <c r="K2" s="104"/>
+      <c r="L2" s="104" t="s">
+        <v>106</v>
+      </c>
+      <c r="M2" s="104"/>
+      <c r="N2" s="104" t="s">
+        <v>107</v>
+      </c>
     </row>
     <row r="3" ht="30.6" customHeight="1" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A3" s="104"/>
-      <c r="B3" s="105"/>
-      <c r="C3" s="105"/>
-      <c r="D3" s="107" t="s">
-        <v>105</v>
-      </c>
-      <c r="E3" s="107" t="s">
-        <v>106</v>
-      </c>
-      <c r="F3" s="107" t="s">
-        <v>107</v>
-      </c>
-      <c r="G3" s="106" t="s">
+      <c r="A3" s="103"/>
+      <c r="B3" s="104"/>
+      <c r="C3" s="104"/>
+      <c r="D3" s="106" t="s">
         <v>108</v>
       </c>
-      <c r="H3" s="106"/>
-      <c r="I3" s="105"/>
-      <c r="J3" s="105"/>
-      <c r="K3" s="105"/>
-      <c r="L3" s="105"/>
-      <c r="M3" s="105"/>
-      <c r="N3" s="105"/>
+      <c r="E3" s="106" t="s">
+        <v>109</v>
+      </c>
+      <c r="F3" s="106" t="s">
+        <v>110</v>
+      </c>
+      <c r="G3" s="105" t="s">
+        <v>111</v>
+      </c>
+      <c r="H3" s="105"/>
+      <c r="I3" s="104"/>
+      <c r="J3" s="104"/>
+      <c r="K3" s="104"/>
+      <c r="L3" s="104"/>
+      <c r="M3" s="104"/>
+      <c r="N3" s="104"/>
     </row>
     <row r="4" ht="91.35" customHeight="1" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A4" s="104"/>
-      <c r="B4" s="107" t="s">
-        <v>109</v>
-      </c>
-      <c r="C4" s="107" t="s">
+      <c r="A4" s="103"/>
+      <c r="B4" s="106" t="s">
+        <v>112</v>
+      </c>
+      <c r="C4" s="106" t="s">
+        <v>113</v>
+      </c>
+      <c r="D4" s="106"/>
+      <c r="E4" s="106"/>
+      <c r="F4" s="106"/>
+      <c r="G4" s="107" t="s">
+        <v>114</v>
+      </c>
+      <c r="H4" s="107" t="s">
+        <v>115</v>
+      </c>
+      <c r="I4" s="106" t="s">
+        <v>116</v>
+      </c>
+      <c r="J4" s="106" t="s">
+        <v>117</v>
+      </c>
+      <c r="K4" s="106" t="s">
         <v>110</v>
       </c>
-      <c r="D4" s="107"/>
-      <c r="E4" s="107"/>
-      <c r="F4" s="107"/>
-      <c r="G4" s="108" t="s">
-        <v>111</v>
-      </c>
-      <c r="H4" s="108" t="s">
-        <v>112</v>
-      </c>
-      <c r="I4" s="107" t="s">
-        <v>113</v>
-      </c>
-      <c r="J4" s="107" t="s">
-        <v>114</v>
-      </c>
-      <c r="K4" s="107" t="s">
-        <v>107</v>
-      </c>
-      <c r="L4" s="108" t="s">
-        <v>115</v>
-      </c>
-      <c r="M4" s="107" t="s">
-        <v>116</v>
-      </c>
-      <c r="N4" s="105"/>
-      <c r="O4" s="109" t="s">
-        <v>117</v>
+      <c r="L4" s="107" t="s">
+        <v>118</v>
+      </c>
+      <c r="M4" s="106" t="s">
+        <v>119</v>
+      </c>
+      <c r="N4" s="104"/>
+      <c r="O4" s="108" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="5" ht="15.75" customHeight="1" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A5" s="110">
+      <c r="A5" s="109">
         <v>1</v>
       </c>
-      <c r="B5" s="110">
+      <c r="B5" s="109">
         <v>2</v>
       </c>
-      <c r="C5" s="110">
+      <c r="C5" s="109">
         <v>3</v>
       </c>
-      <c r="D5" s="110">
+      <c r="D5" s="109">
         <v>4</v>
       </c>
-      <c r="E5" s="110">
+      <c r="E5" s="109">
         <v>5</v>
       </c>
-      <c r="F5" s="110">
+      <c r="F5" s="109">
         <v>6</v>
       </c>
-      <c r="G5" s="110">
+      <c r="G5" s="109">
         <v>7</v>
       </c>
-      <c r="H5" s="110">
+      <c r="H5" s="109">
         <v>8</v>
       </c>
-      <c r="I5" s="110">
+      <c r="I5" s="109">
         <v>9</v>
       </c>
-      <c r="J5" s="110">
+      <c r="J5" s="109">
         <v>10</v>
       </c>
-      <c r="K5" s="110">
+      <c r="K5" s="109">
         <v>11</v>
       </c>
-      <c r="L5" s="110">
+      <c r="L5" s="109">
         <v>12</v>
       </c>
-      <c r="M5" s="110">
+      <c r="M5" s="109">
         <v>13</v>
       </c>
-      <c r="N5" s="110">
+      <c r="N5" s="109">
         <v>14</v>
       </c>
     </row>
     <row r="6" ht="16.7" customHeight="1" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A6" s="111" t="s">
-        <v>118</v>
-      </c>
-      <c r="B6" s="112">
-        <f>IF('Ш Лист 1'!T12,TEXT('Ш Лист 1'!U12,"ч:мм")&amp;CHAR(10)&amp;TEXT('Ш Лист 1'!T12,"дд.мм.гг"),"")</f>
-      </c>
-      <c r="C6" s="112">
-        <f>IF('Ш Лист 1'!T12,TEXT('Ш Лист 1'!W12,"ч:мм")&amp;CHAR(10)&amp;TEXT('Ш Лист 1'!V12,"дд.мм.гг"),"")</f>
-      </c>
-      <c r="D6" s="113"/>
-      <c r="E6" s="113"/>
-      <c r="F6" s="114">
-        <f>IFERROR('Ш Лист 1'!R12-'Ш Лист 1'!P12,0)</f>
+      <c r="A6" s="110" t="s">
+        <v>121</v>
+      </c>
+      <c r="B6" s="111" t="s">
+        <v>122</v>
+      </c>
+      <c r="C6" s="111" t="s">
+        <v>123</v>
+      </c>
+      <c r="D6" s="112">
+        <v>10</v>
+      </c>
+      <c r="E6" s="112">
+        <v>10</v>
+      </c>
+      <c r="F6" s="113">
+        <v>20</v>
+      </c>
+      <c r="G6" s="112" t="s">
+        <v>69</v>
+      </c>
+      <c r="H6" s="112" t="s">
+        <v>69</v>
+      </c>
+      <c r="I6" s="112">
+        <v>10</v>
+      </c>
+      <c r="J6" s="112">
+        <v>50</v>
+      </c>
+      <c r="K6" s="112">
+        <v>60</v>
+      </c>
+      <c r="L6" s="112" t="s">
+        <v>124</v>
+      </c>
+      <c r="M6" s="112">
+        <v>15</v>
+      </c>
+      <c r="N6" s="114">
+        <v>12354</v>
+      </c>
+      <c r="P6" s="115">
         <v>1</v>
       </c>
-      <c r="G6" s="113"/>
-      <c r="H6" s="113"/>
-      <c r="I6" s="113"/>
-      <c r="J6" s="113"/>
-      <c r="K6" s="113"/>
-      <c r="L6" s="113"/>
-      <c r="M6" s="113"/>
-      <c r="N6" s="115">
-        <f>IF('Ш Лист 1'!R12,'Ш Лист 1'!R12,"")</f>
-        <v>12338</v>
-      </c>
-      <c r="P6" s="116">
-        <v>1</v>
-      </c>
     </row>
     <row r="7" ht="16.7" customHeight="1" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A7" s="111" t="s">
-        <v>119</v>
-      </c>
-      <c r="B7" s="112">
+      <c r="A7" s="110" t="s">
+        <v>125</v>
+      </c>
+      <c r="B7" s="111">
         <f>IF('Ш Лист 1'!T14,TEXT('Ш Лист 1'!U14,"ч:мм")&amp;CHAR(10)&amp;TEXT('Ш Лист 1'!T14,"дд.мм.гг"),"")</f>
       </c>
-      <c r="C7" s="112">
+      <c r="C7" s="111">
         <f>IF('Ш Лист 1'!T14,TEXT('Ш Лист 1'!W14,"ч:мм")&amp;CHAR(10)&amp;TEXT('Ш Лист 1'!V14,"дд.мм.гг"),"")</f>
       </c>
-      <c r="D7" s="113"/>
-      <c r="E7" s="113"/>
-      <c r="F7" s="114">
+      <c r="D7" s="112"/>
+      <c r="E7" s="112"/>
+      <c r="F7" s="113">
         <f>IFERROR('Ш Лист 1'!R14-'Ш Лист 1'!P14,0)</f>
         <v>1</v>
       </c>
-      <c r="G7" s="113"/>
-      <c r="H7" s="113"/>
-      <c r="I7" s="113"/>
-      <c r="J7" s="113"/>
-      <c r="K7" s="113"/>
-      <c r="L7" s="113"/>
-      <c r="M7" s="113"/>
-      <c r="N7" s="115">
+      <c r="G7" s="112"/>
+      <c r="H7" s="112"/>
+      <c r="I7" s="112"/>
+      <c r="J7" s="112"/>
+      <c r="K7" s="112"/>
+      <c r="L7" s="112"/>
+      <c r="M7" s="112"/>
+      <c r="N7" s="114">
         <f>IF('Ш Лист 1'!R14,'Ш Лист 1'!R14,"")</f>
         <v>12340</v>
       </c>
-      <c r="P7" s="116">
+      <c r="P7" s="115">
         <v>2</v>
       </c>
     </row>
     <row r="8" ht="16.7" customHeight="1" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A8" s="111" t="s">
-        <v>119</v>
-      </c>
-      <c r="B8" s="112">
+      <c r="A8" s="110" t="s">
+        <v>125</v>
+      </c>
+      <c r="B8" s="111">
         <f>IF('Ш Лист 1'!T16,TEXT('Ш Лист 1'!U16,"ч:мм")&amp;CHAR(10)&amp;TEXT('Ш Лист 1'!T16,"дд.мм.гг"),"")</f>
       </c>
-      <c r="C8" s="112">
+      <c r="C8" s="111">
         <f>IF('Ш Лист 1'!T16,TEXT('Ш Лист 1'!W16,"ч:мм")&amp;CHAR(10)&amp;TEXT('Ш Лист 1'!V16,"дд.мм.гг"),"")</f>
       </c>
-      <c r="D8" s="113"/>
-      <c r="E8" s="113"/>
-      <c r="F8" s="114">
+      <c r="D8" s="112"/>
+      <c r="E8" s="112"/>
+      <c r="F8" s="113">
         <f>IFERROR('Ш Лист 1'!R16-'Ш Лист 1'!P16,0)</f>
         <v>5</v>
       </c>
-      <c r="G8" s="113"/>
-      <c r="H8" s="113"/>
-      <c r="I8" s="113"/>
-      <c r="J8" s="113"/>
-      <c r="K8" s="113"/>
-      <c r="L8" s="113"/>
-      <c r="M8" s="113"/>
-      <c r="N8" s="115">
+      <c r="G8" s="112"/>
+      <c r="H8" s="112"/>
+      <c r="I8" s="112"/>
+      <c r="J8" s="112"/>
+      <c r="K8" s="112"/>
+      <c r="L8" s="112"/>
+      <c r="M8" s="112"/>
+      <c r="N8" s="114">
         <f>IF('Ш Лист 1'!R16,'Ш Лист 1'!R16,"")</f>
         <v>12345</v>
       </c>
-      <c r="P8" s="116">
+      <c r="P8" s="115">
         <v>3</v>
       </c>
     </row>
     <row r="9" ht="16.7" customHeight="1" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A9" s="111" t="s">
-        <v>119</v>
-      </c>
-      <c r="B9" s="112">
+      <c r="A9" s="110" t="s">
+        <v>125</v>
+      </c>
+      <c r="B9" s="111">
         <f>IF('Ш Лист 1'!T18,TEXT('Ш Лист 1'!U18,"ч:мм")&amp;CHAR(10)&amp;TEXT('Ш Лист 1'!T18,"дд.мм.гг"),"")</f>
       </c>
-      <c r="C9" s="112">
+      <c r="C9" s="111">
         <f>IF('Ш Лист 1'!T18,TEXT('Ш Лист 1'!W18,"ч:мм")&amp;CHAR(10)&amp;TEXT('Ш Лист 1'!V18,"дд.мм.гг"),"")</f>
       </c>
-      <c r="D9" s="113"/>
-      <c r="E9" s="113"/>
-      <c r="F9" s="114">
+      <c r="D9" s="112"/>
+      <c r="E9" s="112"/>
+      <c r="F9" s="113">
         <f>IFERROR('Ш Лист 1'!R18-'Ш Лист 1'!P18,0)</f>
         <v>4</v>
       </c>
-      <c r="G9" s="113"/>
-      <c r="H9" s="113"/>
-      <c r="I9" s="113"/>
-      <c r="J9" s="113"/>
-      <c r="K9" s="113"/>
-      <c r="L9" s="113"/>
-      <c r="M9" s="113"/>
-      <c r="N9" s="115">
+      <c r="G9" s="112"/>
+      <c r="H9" s="112"/>
+      <c r="I9" s="112"/>
+      <c r="J9" s="112"/>
+      <c r="K9" s="112"/>
+      <c r="L9" s="112"/>
+      <c r="M9" s="112"/>
+      <c r="N9" s="114">
         <f>IF('Ш Лист 1'!R18,'Ш Лист 1'!R18,"")</f>
         <v>12349</v>
       </c>
-      <c r="P9" s="116">
+      <c r="P9" s="115">
         <v>4</v>
       </c>
     </row>
     <row r="10" ht="16.7" customHeight="1" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A10" s="111" t="s">
-        <v>118</v>
-      </c>
-      <c r="B10" s="112">
+      <c r="A10" s="110" t="s">
+        <v>126</v>
+      </c>
+      <c r="B10" s="111">
         <f>IF('Ш Лист 1'!T20,TEXT('Ш Лист 1'!U20,"ч:мм")&amp;CHAR(10)&amp;TEXT('Ш Лист 1'!T20,"дд.мм.гг"),"")</f>
       </c>
-      <c r="C10" s="112">
+      <c r="C10" s="111">
         <f>IF('Ш Лист 1'!T20,TEXT('Ш Лист 1'!W20,"ч:мм")&amp;CHAR(10)&amp;TEXT('Ш Лист 1'!V20,"дд.мм.гг"),"")</f>
       </c>
-      <c r="D10" s="113"/>
-      <c r="E10" s="113"/>
-      <c r="F10" s="114">
+      <c r="D10" s="112"/>
+      <c r="E10" s="112"/>
+      <c r="F10" s="113">
         <f>IFERROR('Ш Лист 1'!R20-'Ш Лист 1'!P20,0)</f>
         <v>4</v>
       </c>
-      <c r="G10" s="113"/>
-      <c r="H10" s="113"/>
-      <c r="I10" s="113"/>
-      <c r="J10" s="113"/>
-      <c r="K10" s="113"/>
-      <c r="L10" s="113"/>
-      <c r="M10" s="113"/>
-      <c r="N10" s="115">
+      <c r="G10" s="112"/>
+      <c r="H10" s="112"/>
+      <c r="I10" s="112"/>
+      <c r="J10" s="112"/>
+      <c r="K10" s="112"/>
+      <c r="L10" s="112"/>
+      <c r="M10" s="112"/>
+      <c r="N10" s="114">
         <f>IF('Ш Лист 1'!R20,'Ш Лист 1'!R20,"")</f>
         <v>12353</v>
       </c>
-      <c r="P10" s="116">
+      <c r="P10" s="115">
         <v>5</v>
       </c>
     </row>
     <row r="11" ht="16.7" customHeight="1" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A11" s="111" t="s">
-        <v>118</v>
-      </c>
-      <c r="B11" s="112">
+      <c r="A11" s="110" t="s">
+        <v>126</v>
+      </c>
+      <c r="B11" s="111">
         <f>IF('Ш Лист 1'!T22,TEXT('Ш Лист 1'!U22,"ч:мм")&amp;CHAR(10)&amp;TEXT('Ш Лист 1'!T22,"дд.мм.гг"),"")</f>
       </c>
-      <c r="C11" s="112">
+      <c r="C11" s="111">
         <f>IF('Ш Лист 1'!T22,TEXT('Ш Лист 1'!W22,"ч:мм")&amp;CHAR(10)&amp;TEXT('Ш Лист 1'!V22,"дд.мм.гг"),"")</f>
       </c>
-      <c r="D11" s="113"/>
-      <c r="E11" s="113"/>
-      <c r="F11" s="114">
+      <c r="D11" s="112"/>
+      <c r="E11" s="112"/>
+      <c r="F11" s="113">
         <f>IFERROR('Ш Лист 1'!R22-'Ш Лист 1'!P22,0)</f>
         <v>0</v>
       </c>
-      <c r="G11" s="113"/>
-      <c r="H11" s="113"/>
-      <c r="I11" s="113"/>
-      <c r="J11" s="113"/>
-      <c r="K11" s="113"/>
-      <c r="L11" s="113"/>
-      <c r="M11" s="113"/>
-      <c r="N11" s="115" t="e">
+      <c r="G11" s="112"/>
+      <c r="H11" s="112"/>
+      <c r="I11" s="112"/>
+      <c r="J11" s="112"/>
+      <c r="K11" s="112"/>
+      <c r="L11" s="112"/>
+      <c r="M11" s="112"/>
+      <c r="N11" s="114" t="e">
         <f>IF('Ш Лист 1'!R22,'Ш Лист 1'!R22,"")</f>
         <v>#VALUE!</v>
       </c>
-      <c r="P11" s="116">
+      <c r="P11" s="115">
         <v>6</v>
       </c>
     </row>
     <row r="12" ht="16.7" customHeight="1" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A12" s="111" t="s">
-        <v>118</v>
-      </c>
-      <c r="B12" s="112">
+      <c r="A12" s="110" t="s">
+        <v>126</v>
+      </c>
+      <c r="B12" s="111">
         <f>IF('Ш Лист 1'!T24,TEXT('Ш Лист 1'!U24,"ч:мм")&amp;CHAR(10)&amp;TEXT('Ш Лист 1'!T24,"дд.мм.гг"),"")</f>
       </c>
-      <c r="C12" s="112">
+      <c r="C12" s="111">
         <f>IF('Ш Лист 1'!T24,TEXT('Ш Лист 1'!W24,"ч:мм")&amp;CHAR(10)&amp;TEXT('Ш Лист 1'!V24,"дд.мм.гг"),"")</f>
       </c>
-      <c r="D12" s="113"/>
-      <c r="E12" s="113"/>
-      <c r="F12" s="114">
+      <c r="D12" s="112"/>
+      <c r="E12" s="112"/>
+      <c r="F12" s="113">
         <f>IFERROR('Ш Лист 1'!R24-'Ш Лист 1'!P24,0)</f>
         <v>0</v>
       </c>
-      <c r="G12" s="113"/>
-      <c r="H12" s="113"/>
-      <c r="I12" s="113"/>
-      <c r="J12" s="113"/>
-      <c r="K12" s="113"/>
-      <c r="L12" s="113"/>
-      <c r="M12" s="113"/>
-      <c r="N12" s="115" t="e">
+      <c r="G12" s="112"/>
+      <c r="H12" s="112"/>
+      <c r="I12" s="112"/>
+      <c r="J12" s="112"/>
+      <c r="K12" s="112"/>
+      <c r="L12" s="112"/>
+      <c r="M12" s="112"/>
+      <c r="N12" s="114" t="e">
         <f>IF('Ш Лист 1'!R24,'Ш Лист 1'!R24,"")</f>
         <v>#VALUE!</v>
       </c>
-      <c r="P12" s="116">
+      <c r="P12" s="115">
         <v>7</v>
       </c>
     </row>
     <row r="13" ht="16.7" customHeight="1" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A13" s="111" t="s">
-        <v>118</v>
-      </c>
-      <c r="B13" s="112">
+      <c r="A13" s="110" t="s">
+        <v>126</v>
+      </c>
+      <c r="B13" s="111">
         <f>IF('Ш Лист 1'!T26,TEXT('Ш Лист 1'!U26,"ч:мм")&amp;CHAR(10)&amp;TEXT('Ш Лист 1'!T26,"дд.мм.гг"),"")</f>
       </c>
-      <c r="C13" s="112">
+      <c r="C13" s="111">
         <f>IF('Ш Лист 1'!T26,TEXT('Ш Лист 1'!W26,"ч:мм")&amp;CHAR(10)&amp;TEXT('Ш Лист 1'!V26,"дд.мм.гг"),"")</f>
       </c>
-      <c r="D13" s="113"/>
-      <c r="E13" s="113"/>
-      <c r="F13" s="114">
+      <c r="D13" s="112"/>
+      <c r="E13" s="112"/>
+      <c r="F13" s="113">
         <f>IFERROR('Ш Лист 1'!R26-'Ш Лист 1'!P26,0)</f>
         <v>0</v>
       </c>
-      <c r="G13" s="113"/>
-      <c r="H13" s="113"/>
-      <c r="I13" s="113"/>
-      <c r="J13" s="113"/>
-      <c r="K13" s="113"/>
-      <c r="L13" s="113"/>
-      <c r="M13" s="113"/>
-      <c r="N13" s="115" t="e">
+      <c r="G13" s="112"/>
+      <c r="H13" s="112"/>
+      <c r="I13" s="112"/>
+      <c r="J13" s="112"/>
+      <c r="K13" s="112"/>
+      <c r="L13" s="112"/>
+      <c r="M13" s="112"/>
+      <c r="N13" s="114" t="e">
         <f>IF('Ш Лист 1'!R26,'Ш Лист 1'!R26,"")</f>
         <v>#VALUE!</v>
       </c>
-      <c r="P13" s="116">
+      <c r="P13" s="115">
         <v>8</v>
       </c>
     </row>
     <row r="14" ht="16.7" customHeight="1" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A14" s="111"/>
-      <c r="B14" s="112">
+      <c r="A14" s="110"/>
+      <c r="B14" s="111">
         <f>IF('Ш Лист 1'!T28,TEXT('Ш Лист 1'!U28,"ч:мм")&amp;CHAR(10)&amp;TEXT('Ш Лист 1'!T28,"дд.мм.гг"),"")</f>
       </c>
-      <c r="C14" s="112">
+      <c r="C14" s="111">
         <f>IF('Ш Лист 1'!T28,TEXT('Ш Лист 1'!W28,"ч:мм")&amp;CHAR(10)&amp;TEXT('Ш Лист 1'!V28,"дд.мм.гг"),"")</f>
       </c>
-      <c r="D14" s="113"/>
-      <c r="E14" s="113"/>
-      <c r="F14" s="114">
+      <c r="D14" s="112"/>
+      <c r="E14" s="112"/>
+      <c r="F14" s="113">
         <f>IFERROR('Ш Лист 1'!R28-'Ш Лист 1'!P28,0)</f>
         <v>0</v>
       </c>
-      <c r="G14" s="113"/>
-      <c r="H14" s="113"/>
-      <c r="I14" s="113"/>
-      <c r="J14" s="113"/>
-      <c r="K14" s="113"/>
-      <c r="L14" s="113"/>
-      <c r="M14" s="113"/>
-      <c r="N14" s="115" t="e">
+      <c r="G14" s="112"/>
+      <c r="H14" s="112"/>
+      <c r="I14" s="112"/>
+      <c r="J14" s="112"/>
+      <c r="K14" s="112"/>
+      <c r="L14" s="112"/>
+      <c r="M14" s="112"/>
+      <c r="N14" s="114" t="e">
         <f>IF('Ш Лист 1'!R28,'Ш Лист 1'!R28,"")</f>
         <v>#VALUE!</v>
       </c>
-      <c r="P14" s="116">
+      <c r="P14" s="115">
         <v>9</v>
       </c>
     </row>
     <row r="15" ht="16.7" customHeight="1" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A15" s="111"/>
-      <c r="B15" s="112">
+      <c r="A15" s="110"/>
+      <c r="B15" s="111">
         <f>IF('Ш Лист 1'!T30,TEXT('Ш Лист 1'!U30,"ч:мм")&amp;CHAR(10)&amp;TEXT('Ш Лист 1'!T30,"дд.мм.гг"),"")</f>
       </c>
-      <c r="C15" s="112">
+      <c r="C15" s="111">
         <f>IF('Ш Лист 1'!T30,TEXT('Ш Лист 1'!W30,"ч:мм")&amp;CHAR(10)&amp;TEXT('Ш Лист 1'!V30,"дд.мм.гг"),"")</f>
       </c>
-      <c r="D15" s="113"/>
-      <c r="E15" s="113"/>
-      <c r="F15" s="114">
+      <c r="D15" s="112"/>
+      <c r="E15" s="112"/>
+      <c r="F15" s="113">
         <f>IFERROR('Ш Лист 1'!R30-'Ш Лист 1'!P30,0)</f>
         <v>0</v>
       </c>
-      <c r="G15" s="113"/>
-      <c r="H15" s="113"/>
-      <c r="I15" s="113"/>
-      <c r="J15" s="113"/>
-      <c r="K15" s="113"/>
-      <c r="L15" s="113"/>
-      <c r="M15" s="113"/>
-      <c r="N15" s="115" t="e">
+      <c r="G15" s="112"/>
+      <c r="H15" s="112"/>
+      <c r="I15" s="112"/>
+      <c r="J15" s="112"/>
+      <c r="K15" s="112"/>
+      <c r="L15" s="112"/>
+      <c r="M15" s="112"/>
+      <c r="N15" s="114" t="e">
         <f>IF('Ш Лист 1'!R30,'Ш Лист 1'!R30,"")</f>
         <v>#VALUE!</v>
       </c>
-      <c r="P15" s="116">
+      <c r="P15" s="115">
         <v>10</v>
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A16" s="55" t="s">
-        <v>120</v>
-      </c>
-      <c r="B16" s="117"/>
-      <c r="C16" s="117"/>
-      <c r="D16" s="114">
+      <c r="A16" s="54" t="s">
+        <v>127</v>
+      </c>
+      <c r="B16" s="116"/>
+      <c r="C16" s="116"/>
+      <c r="D16" s="113">
         <f t="shared" ref="D16:E16" si="0">SUM(D6:D15)</f>
         <v>0</v>
       </c>
-      <c r="E16" s="114">
+      <c r="E16" s="113">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="F16" s="114">
+      <c r="F16" s="113">
         <f>SUM(F6:F15)</f>
         <v>15</v>
       </c>
-      <c r="G16" s="114">
+      <c r="G16" s="113">
         <f t="shared" ref="G16" si="1">SUM(G6:G15)</f>
         <v>0</v>
       </c>
-      <c r="H16" s="114">
+      <c r="H16" s="113">
         <f t="shared" ref="H16:I16" si="2">SUM(H6:H15)</f>
         <v>0</v>
       </c>
-      <c r="I16" s="114">
+      <c r="I16" s="113">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="J16" s="114">
+      <c r="J16" s="113">
         <f t="shared" ref="J16" si="3">SUM(J6:J15)</f>
         <v>0</v>
       </c>
-      <c r="K16" s="114">
+      <c r="K16" s="113">
         <f t="shared" ref="K16:L16" si="4">SUM(K6:K15)</f>
         <v>0</v>
       </c>
-      <c r="L16" s="114">
+      <c r="L16" s="113">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="M16" s="114">
+      <c r="M16" s="113">
         <f t="shared" ref="M16" si="5">SUM(M6:M15)</f>
         <v>0</v>
       </c>
-      <c r="N16" s="117"/>
+      <c r="N16" s="116"/>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A17" s="29" t="s">
-        <v>121</v>
+      <c r="A17" s="28" t="s">
+        <v>128</v>
       </c>
     </row>
     <row r="18" ht="12" customHeight="1" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A18" s="76" t="e">
-        <f>INDEX(#REF!,MATCH('Ш Лист 1'!L33,#REF!,0))</f>
-        <v>#REF!</v>
-      </c>
-      <c r="B18" s="118" t="e">
-        <f>INDEX(#REF!,MATCH('Ш Лист 1'!L33,#REF!,0))</f>
-        <v>#REF!</v>
-      </c>
-      <c r="C18" s="119" t="s">
-        <v>122</v>
-      </c>
-      <c r="D18" s="120">
-        <f>F16</f>
-        <v>15</v>
-      </c>
-      <c r="E18" s="76" t="s">
-        <v>123</v>
-      </c>
-      <c r="F18" s="121">
+      <c r="A18" s="75" t="s">
+        <v>129</v>
+      </c>
+      <c r="B18" s="117">
+        <v>11.5</v>
+      </c>
+      <c r="C18" s="118" t="s">
+        <v>130</v>
+      </c>
+      <c r="D18" s="119">
+        <v>1557</v>
+      </c>
+      <c r="E18" s="75" t="s">
+        <v>131</v>
+      </c>
+      <c r="F18" s="120">
         <f>A15</f>
         <v>0</v>
       </c>
-      <c r="G18" s="76" t="s">
-        <v>124</v>
-      </c>
-      <c r="H18" s="122" t="e">
-        <f>ROUND(B18*D18/C19-B18*D18/C19*F18,0)</f>
-        <v>#REF!</v>
-      </c>
-      <c r="I18" s="123" t="s">
-        <v>125</v>
+      <c r="G18" s="75" t="s">
+        <v>132</v>
+      </c>
+      <c r="H18" s="121">
+        <v>152</v>
+      </c>
+      <c r="I18" s="122" t="s">
+        <v>133</v>
       </c>
       <c r="J18" s="1"/>
       <c r="K18" s="1"/>
@@ -4661,17 +4811,17 @@
       <c r="N18" s="1"/>
     </row>
     <row r="19" ht="12" customHeight="1" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A19" s="76"/>
+      <c r="A19" s="75"/>
       <c r="B19" s="1"/>
       <c r="C19" s="1">
         <v>100</v>
       </c>
       <c r="D19" s="1"/>
-      <c r="E19" s="76"/>
-      <c r="F19" s="121"/>
-      <c r="G19" s="76"/>
-      <c r="H19" s="122"/>
-      <c r="I19" s="123"/>
+      <c r="E19" s="75"/>
+      <c r="F19" s="120"/>
+      <c r="G19" s="75"/>
+      <c r="H19" s="121"/>
+      <c r="I19" s="122"/>
       <c r="J19" s="1"/>
       <c r="K19" s="1"/>
       <c r="L19" s="1"/>
@@ -4679,25 +4829,25 @@
       <c r="N19" s="1"/>
     </row>
     <row r="20" ht="12" customHeight="1" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A20" s="76">
+      <c r="A20" s="75">
         <f>IF(HideOil,"",INDEX(#REF!,MATCH('Ш Лист 1'!L33,#REF!,0)))</f>
       </c>
-      <c r="B20" s="118">
+      <c r="B20" s="117">
         <f>IF(HideOil,"",INDEX(#REF!,MATCH('Ш Лист 1'!L33,#REF!,0)))</f>
       </c>
-      <c r="C20" s="119">
+      <c r="C20" s="118">
         <f>IF(HideOil,"","x")</f>
       </c>
-      <c r="D20" s="120">
+      <c r="D20" s="119">
         <f>IF(HideOil,"",H18)</f>
       </c>
-      <c r="E20" s="76">
+      <c r="E20" s="75">
         <f>IF(HideOil,"","=")</f>
       </c>
-      <c r="F20" s="76">
+      <c r="F20" s="75">
         <f>IF(HideOil,"",ROUND(B20*D20/C21,1))</f>
       </c>
-      <c r="G20" s="123">
+      <c r="G20" s="122">
         <f>IF(HideOil,"","л")</f>
       </c>
       <c r="H20" s="1"/>
@@ -4712,15 +4862,15 @@
       </c>
     </row>
     <row r="21" ht="12" customHeight="1" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A21" s="76"/>
+      <c r="A21" s="75"/>
       <c r="B21" s="1"/>
       <c r="C21" s="1">
         <f>IF(HideOil,"",100)</f>
       </c>
       <c r="D21" s="1"/>
-      <c r="E21" s="76"/>
-      <c r="F21" s="76"/>
-      <c r="G21" s="123"/>
+      <c r="E21" s="75"/>
+      <c r="F21" s="75"/>
+      <c r="G21" s="122"/>
       <c r="H21" s="1"/>
       <c r="I21" s="1"/>
       <c r="J21" s="1"/>
@@ -4731,102 +4881,104 @@
     </row>
     <row r="22" ht="15.75" customHeight="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="19" t="s">
-        <v>126</v>
-      </c>
-      <c r="B22" s="124">
+        <v>134</v>
+      </c>
+      <c r="B22" s="123">
         <f>F16</f>
         <v>15</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>127</v>
+        <v>135</v>
       </c>
     </row>
     <row r="23" ht="15.75" customHeight="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="19" t="s">
-        <v>128</v>
-      </c>
-      <c r="B23" s="124" t="e">
+        <v>136</v>
+      </c>
+      <c r="B23" s="123" t="e">
         <f>H18</f>
         <v>#REF!</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>125</v>
+        <v>133</v>
       </c>
     </row>
     <row r="24" ht="15.75" customHeight="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24" s="19" t="s">
-        <v>129</v>
-      </c>
-      <c r="D24" s="125" t="str">
-        <f>'Ш Лист 1'!J5</f>
-        <v>солдат</v>
-      </c>
-      <c r="E24" s="126"/>
-      <c r="F24" s="126"/>
-      <c r="G24" s="126"/>
-      <c r="H24" s="126"/>
-      <c r="I24" s="126"/>
-      <c r="J24" s="126"/>
-      <c r="K24" s="126"/>
-      <c r="M24" s="125" t="str">
+        <v>137</v>
+      </c>
+      <c r="D24" s="124" t="s">
+        <v>11</v>
+      </c>
+      <c r="E24" s="125"/>
+      <c r="F24" s="125"/>
+      <c r="G24" s="125"/>
+      <c r="H24" s="125"/>
+      <c r="I24" s="125"/>
+      <c r="J24" s="125"/>
+      <c r="K24" s="125"/>
+      <c r="L24" t="s">
+        <v>12</v>
+      </c>
+      <c r="M24" s="124" t="str">
         <f>'Ш Лист 1'!L5</f>
         <v>Петренко В.В.</v>
       </c>
     </row>
     <row r="25" ht="12" customHeight="1" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B25" s="127" t="s">
-        <v>130</v>
-      </c>
-      <c r="C25" s="127"/>
-      <c r="D25" s="127"/>
-      <c r="E25" s="127"/>
-      <c r="F25" s="127"/>
-      <c r="G25" s="127"/>
-      <c r="H25" s="127"/>
-      <c r="I25" s="127"/>
-      <c r="J25" s="127"/>
-      <c r="K25" s="127"/>
-      <c r="L25" s="127"/>
-      <c r="M25" s="127"/>
-      <c r="N25" s="127"/>
+      <c r="B25" s="126" t="s">
+        <v>138</v>
+      </c>
+      <c r="C25" s="126"/>
+      <c r="D25" s="126"/>
+      <c r="E25" s="126"/>
+      <c r="F25" s="126"/>
+      <c r="G25" s="126"/>
+      <c r="H25" s="126"/>
+      <c r="I25" s="126"/>
+      <c r="J25" s="126"/>
+      <c r="K25" s="126"/>
+      <c r="L25" s="126"/>
+      <c r="M25" s="126"/>
+      <c r="N25" s="126"/>
     </row>
     <row r="26" ht="15.75" customHeight="1" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A26" s="30" t="s">
-        <v>131</v>
-      </c>
-      <c r="G26" s="118">
-        <f>IFERROR(INDEX(#REF!,MATCH(N26,#REF!,0)),"")</f>
-      </c>
-      <c r="H26" s="126"/>
-      <c r="I26" s="126"/>
-      <c r="J26" s="126"/>
-      <c r="K26" s="126"/>
-      <c r="L26" s="126"/>
-      <c r="M26" s="126"/>
-      <c r="N26" s="128" t="s">
-        <v>132</v>
+      <c r="A26" s="29" t="s">
+        <v>139</v>
+      </c>
+      <c r="G26" s="117" t="s">
+        <v>140</v>
+      </c>
+      <c r="H26" s="125"/>
+      <c r="I26" s="125"/>
+      <c r="J26" s="125"/>
+      <c r="K26" s="125"/>
+      <c r="L26" s="125"/>
+      <c r="M26" s="125"/>
+      <c r="N26" s="127" t="s">
+        <v>141</v>
       </c>
     </row>
     <row r="27" ht="16.35" customHeight="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="B27" s="1">
-        <v>2023</v>
+        <v>142</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>143</v>
       </c>
       <c r="C27" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="G27" s="129" t="s">
-        <v>134</v>
-      </c>
-      <c r="H27" s="129"/>
-      <c r="I27" s="129"/>
-      <c r="J27" s="129"/>
-      <c r="K27" s="129"/>
-      <c r="L27" s="129"/>
-      <c r="M27" s="129"/>
-      <c r="N27" s="129"/>
+      <c r="G27" s="128" t="s">
+        <v>144</v>
+      </c>
+      <c r="H27" s="128"/>
+      <c r="I27" s="128"/>
+      <c r="J27" s="128"/>
+      <c r="K27" s="128"/>
+      <c r="L27" s="128"/>
+      <c r="M27" s="128"/>
+      <c r="N27" s="128"/>
     </row>
   </sheetData>
   <mergeCells count="23">

</xml_diff>

<commit_message>
409 by update too
</commit_message>
<xml_diff>
--- a/src/backend/fileStorage/excel/roadXS.xlsx
+++ b/src/backend/fileStorage/excel/roadXS.xlsx
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="526" uniqueCount="224">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="465" uniqueCount="210">
   <si>
     <t>року</t>
   </si>
@@ -585,31 +585,34 @@
     <t>маршрут</t>
   </si>
   <si>
-    <t>тойота корито</t>
+    <t>Reno</t>
   </si>
   <si>
     <t>AI8523FE</t>
   </si>
   <si>
-    <t>12</t>
-  </si>
-  <si>
-    <t>10w401</t>
-  </si>
-  <si>
-    <t>1.5</t>
-  </si>
-  <si>
-    <t>Тр</t>
-  </si>
-  <si>
-    <t>Транспортна</t>
+    <t>Дріжі</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>Тісто</t>
+  </si>
+  <si>
+    <t>харч.</t>
+  </si>
+  <si>
+    <t>Харчова</t>
   </si>
   <si>
     <t>Чек А.Ф.</t>
   </si>
   <si>
-    <t>А0000 (ПВЗ)</t>
+    <t>старший сержант</t>
+  </si>
+  <si>
+    <t>Їдалка</t>
   </si>
   <si>
     <t>Кирило Володимир Петрович</t>
@@ -621,9 +624,6 @@
     <t>Старший (технік) підрозділу</t>
   </si>
   <si>
-    <t>старший сержант</t>
-  </si>
-  <si>
     <t>ст. с-т</t>
   </si>
   <si>
@@ -642,103 +642,61 @@
     <t>Київ - Теропіль</t>
   </si>
   <si>
-    <t>вольцваген</t>
-  </si>
-  <si>
-    <t>CE0548IS</t>
-  </si>
-  <si>
-    <t>10w40</t>
+    <t>Порш</t>
+  </si>
+  <si>
+    <t>AS1234AV</t>
+  </si>
+  <si>
+    <t>voda</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>maslo</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>Tr</t>
+  </si>
+  <si>
+    <t>Transportna</t>
+  </si>
+  <si>
+    <t>AZOV</t>
+  </si>
+  <si>
+    <t>старший відділення</t>
   </si>
   <si>
     <t>Вільний К.Ю.</t>
   </si>
   <si>
-    <t>старший відділення</t>
-  </si>
-  <si>
-    <t>мерседес транз</t>
-  </si>
-  <si>
-    <t>AS0025A5</t>
-  </si>
-  <si>
-    <t>Бензин</t>
-  </si>
-  <si>
-    <t>5w40</t>
+    <t>майор</t>
+  </si>
+  <si>
+    <t>м-р</t>
+  </si>
+  <si>
+    <t>Вар Ц.Ц.</t>
+  </si>
+  <si>
+    <t>с-т</t>
+  </si>
+  <si>
+    <t>Диван Ф.Ф.</t>
+  </si>
+  <si>
+    <t>Оранж В.Ф.</t>
+  </si>
+  <si>
+    <t>соладт</t>
   </si>
   <si>
     <t>Попов Й.Й.</t>
-  </si>
-  <si>
-    <t>AZOV</t>
-  </si>
-  <si>
-    <t>майор</t>
-  </si>
-  <si>
-    <t>м-р</t>
-  </si>
-  <si>
-    <t>Вар Ц.Ц.</t>
-  </si>
-  <si>
-    <t>Порш</t>
-  </si>
-  <si>
-    <t>AS1234AV</t>
-  </si>
-  <si>
-    <t>voda</t>
-  </si>
-  <si>
-    <t>4</t>
-  </si>
-  <si>
-    <t>maslo</t>
-  </si>
-  <si>
-    <t>1</t>
-  </si>
-  <si>
-    <t>Tr</t>
-  </si>
-  <si>
-    <t>Transportna</t>
-  </si>
-  <si>
-    <t>с-т</t>
-  </si>
-  <si>
-    <t>Диван Ф.Ф.</t>
-  </si>
-  <si>
-    <t>тойота корола кабріолет</t>
-  </si>
-  <si>
-    <t>AS1234AD</t>
-  </si>
-  <si>
-    <t>Олива</t>
-  </si>
-  <si>
-    <t>3</t>
-  </si>
-  <si>
-    <t>Оранж В.Ф.</t>
-  </si>
-  <si>
-    <t>Порш панамера</t>
-  </si>
-  <si>
-    <t>AS1234A3</t>
-  </si>
-  <si>
-    <t>AS1234A2</t>
-  </si>
-  <si>
-    <t>соладт</t>
   </si>
   <si>
     <t>Водій-технік-механік</t>
@@ -2008,16 +1966,16 @@
         <v>168</v>
       </c>
       <c r="C3" t="s">
-        <v>129</v>
+        <v>169</v>
       </c>
       <c r="D3" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="E3" t="s">
+        <v>171</v>
+      </c>
+      <c r="F3" t="s">
         <v>170</v>
-      </c>
-      <c r="F3" t="s">
-        <v>171</v>
       </c>
       <c r="G3" t="s">
         <v>172</v>
@@ -2029,13 +1987,13 @@
         <v>174</v>
       </c>
       <c r="J3" t="s">
-        <v>140</v>
+        <v>175</v>
       </c>
       <c r="K3" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="L3" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="M3" t="s">
         <v>14</v>
@@ -2044,16 +2002,16 @@
         <v>10</v>
       </c>
       <c r="P3" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="Q3" s="130">
         <v>0.15</v>
       </c>
       <c r="S3" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="T3" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="U3" t="s">
         <v>180</v>
@@ -2085,22 +2043,22 @@
         <v>187</v>
       </c>
       <c r="C4" t="s">
-        <v>129</v>
-      </c>
-      <c r="D4">
-        <v>9</v>
+        <v>188</v>
+      </c>
+      <c r="D4" t="s">
+        <v>189</v>
       </c>
       <c r="E4" t="s">
-        <v>188</v>
-      </c>
-      <c r="F4" s="131">
-        <v>1.2</v>
+        <v>190</v>
+      </c>
+      <c r="F4" s="131" t="s">
+        <v>191</v>
       </c>
       <c r="G4" t="s">
-        <v>172</v>
+        <v>192</v>
       </c>
       <c r="H4" t="s">
-        <v>173</v>
+        <v>193</v>
       </c>
       <c r="I4" t="s">
         <v>174</v>
@@ -2109,16 +2067,16 @@
         <v>140</v>
       </c>
       <c r="K4" t="s">
-        <v>175</v>
+        <v>194</v>
       </c>
       <c r="L4" t="s">
-        <v>189</v>
+        <v>177</v>
       </c>
       <c r="M4" t="s">
         <v>14</v>
       </c>
       <c r="S4" t="s">
-        <v>190</v>
+        <v>195</v>
       </c>
       <c r="T4" t="s">
         <v>14</v>
@@ -2127,49 +2085,10 @@
         <v>42</v>
       </c>
       <c r="V4" t="s">
-        <v>189</v>
+        <v>196</v>
       </c>
     </row>
     <row r="5" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>191</v>
-      </c>
-      <c r="B5" t="s">
-        <v>192</v>
-      </c>
-      <c r="C5" t="s">
-        <v>193</v>
-      </c>
-      <c r="D5">
-        <v>11</v>
-      </c>
-      <c r="E5" t="s">
-        <v>194</v>
-      </c>
-      <c r="F5">
-        <v>1.1</v>
-      </c>
-      <c r="G5" t="s">
-        <v>172</v>
-      </c>
-      <c r="H5" t="s">
-        <v>173</v>
-      </c>
-      <c r="I5" t="s">
-        <v>195</v>
-      </c>
-      <c r="J5" t="s">
-        <v>11</v>
-      </c>
-      <c r="K5" t="s">
-        <v>196</v>
-      </c>
-      <c r="L5" t="s">
-        <v>189</v>
-      </c>
-      <c r="M5" t="s">
-        <v>14</v>
-      </c>
       <c r="S5" t="s">
         <v>17</v>
       </c>
@@ -2183,46 +2102,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>200</v>
-      </c>
-      <c r="B6" t="s">
-        <v>201</v>
-      </c>
-      <c r="C6" t="s">
-        <v>202</v>
-      </c>
-      <c r="D6" t="s">
-        <v>203</v>
-      </c>
-      <c r="E6" t="s">
-        <v>204</v>
-      </c>
-      <c r="F6" t="s">
-        <v>205</v>
-      </c>
-      <c r="G6" t="s">
-        <v>206</v>
-      </c>
-      <c r="H6" t="s">
-        <v>207</v>
-      </c>
-      <c r="I6" t="s">
-        <v>174</v>
-      </c>
-      <c r="J6" t="s">
-        <v>140</v>
-      </c>
-      <c r="K6" t="s">
-        <v>196</v>
-      </c>
-      <c r="L6" t="s">
-        <v>176</v>
-      </c>
-      <c r="M6" t="s">
-        <v>14</v>
-      </c>
+    <row r="6" spans="2:22" x14ac:dyDescent="0.25">
       <c r="S6" t="s">
         <v>39</v>
       </c>
@@ -2230,105 +2110,27 @@
         <v>140</v>
       </c>
       <c r="U6" t="s">
-        <v>208</v>
+        <v>200</v>
       </c>
       <c r="V6" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>210</v>
-      </c>
-      <c r="B7" t="s">
-        <v>211</v>
-      </c>
-      <c r="C7" t="s">
-        <v>129</v>
-      </c>
-      <c r="D7" t="s">
-        <v>169</v>
-      </c>
-      <c r="E7" t="s">
-        <v>212</v>
-      </c>
-      <c r="F7" t="s">
-        <v>213</v>
-      </c>
-      <c r="G7" t="s">
-        <v>172</v>
-      </c>
-      <c r="H7" t="s">
-        <v>173</v>
-      </c>
-      <c r="I7" t="s">
-        <v>214</v>
-      </c>
-      <c r="J7" t="s">
-        <v>179</v>
-      </c>
-      <c r="K7" t="s">
-        <v>196</v>
-      </c>
-      <c r="L7" t="s">
-        <v>181</v>
-      </c>
-      <c r="M7" t="s">
-        <v>179</v>
-      </c>
+        <v>201</v>
+      </c>
+    </row>
+    <row r="7" spans="2:22" x14ac:dyDescent="0.25">
       <c r="S7" t="s">
         <v>10</v>
       </c>
       <c r="T7" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="U7" t="s">
         <v>180</v>
       </c>
       <c r="V7" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>215</v>
-      </c>
-      <c r="B8" t="s">
-        <v>216</v>
-      </c>
-      <c r="C8" t="s">
         <v>202</v>
       </c>
-      <c r="D8" t="s">
-        <v>203</v>
-      </c>
-      <c r="E8" t="s">
-        <v>204</v>
-      </c>
-      <c r="F8" t="s">
-        <v>205</v>
-      </c>
-      <c r="G8" t="s">
-        <v>206</v>
-      </c>
-      <c r="H8" t="s">
-        <v>207</v>
-      </c>
-      <c r="I8" t="s">
-        <v>189</v>
-      </c>
-      <c r="J8" t="s">
-        <v>14</v>
-      </c>
-      <c r="K8" t="s">
-        <v>196</v>
-      </c>
-      <c r="L8" t="s">
-        <v>176</v>
-      </c>
-      <c r="M8" t="s">
-        <v>14</v>
-      </c>
+    </row>
+    <row r="8" spans="2:22" x14ac:dyDescent="0.25">
       <c r="S8" t="s">
         <v>10</v>
       </c>
@@ -2336,66 +2138,27 @@
         <v>140</v>
       </c>
       <c r="U8" t="s">
-        <v>208</v>
+        <v>200</v>
       </c>
       <c r="V8" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>210</v>
-      </c>
-      <c r="B9" t="s">
-        <v>217</v>
-      </c>
-      <c r="C9" t="s">
-        <v>202</v>
-      </c>
-      <c r="D9" t="s">
-        <v>203</v>
-      </c>
-      <c r="E9" t="s">
-        <v>204</v>
-      </c>
-      <c r="F9" t="s">
-        <v>213</v>
-      </c>
-      <c r="G9" t="s">
-        <v>206</v>
-      </c>
-      <c r="H9" t="s">
-        <v>207</v>
-      </c>
-      <c r="I9" t="s">
-        <v>189</v>
-      </c>
-      <c r="J9" t="s">
-        <v>14</v>
-      </c>
-      <c r="K9" t="s">
-        <v>196</v>
-      </c>
-      <c r="L9" t="s">
-        <v>189</v>
-      </c>
-      <c r="M9" t="s">
-        <v>14</v>
-      </c>
+    <row r="9" spans="2:22" x14ac:dyDescent="0.25">
       <c r="S9" t="s">
         <v>10</v>
       </c>
       <c r="T9" t="s">
-        <v>218</v>
+        <v>203</v>
       </c>
       <c r="U9" t="s">
         <v>44</v>
       </c>
       <c r="V9" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="10" spans="19:22" x14ac:dyDescent="0.25">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="10" spans="2:22" x14ac:dyDescent="0.25">
       <c r="S10" t="s">
         <v>154</v>
       </c>
@@ -2406,12 +2169,12 @@
         <v>42</v>
       </c>
       <c r="V10" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="11" spans="19:22" x14ac:dyDescent="0.25">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="11" spans="2:22" x14ac:dyDescent="0.25">
       <c r="S11" t="s">
-        <v>219</v>
+        <v>205</v>
       </c>
       <c r="T11" t="s">
         <v>14</v>
@@ -2420,21 +2183,21 @@
         <v>42</v>
       </c>
       <c r="V11" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="12" spans="19:22" x14ac:dyDescent="0.25">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="12" spans="2:22" x14ac:dyDescent="0.25">
       <c r="S12" t="s">
-        <v>220</v>
+        <v>206</v>
       </c>
       <c r="T12" t="s">
-        <v>221</v>
+        <v>207</v>
       </c>
       <c r="U12" t="s">
-        <v>222</v>
+        <v>208</v>
       </c>
       <c r="V12" t="s">
-        <v>223</v>
+        <v>209</v>
       </c>
     </row>
   </sheetData>

</xml_diff>